<commit_message>
Funkční syntaktický analyzátor, nebere pouze víc jak dva nové řádky za sebou, opravím asap
Nová předpřipravená gramatika na opravu řádků, aktualizovaná LL tabulka (zatím bez řádků), nový testovací soubor
</commit_message>
<xml_diff>
--- a/doc/LL tabulka.xlsx
+++ b/doc/LL tabulka.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\OneDrive\VUT_FIT_BIT\IFJ\Projekt\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="365" documentId="6_{A882F6EA-21BA-4747-84DC-CE7C22B943DB}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{B2D9CECB-7AD1-4B70-B5F7-6B7D41A1FB6E}"/>
+  <xr:revisionPtr revIDLastSave="160" documentId="6_{9A5E4322-B6A2-4F6C-9661-AD2FA57F2F31}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{892EF6EB-727E-4D2B-8D85-FEE95D778E8A}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12165" xr2:uid="{C362D381-7D2B-4872-B2C9-60D26B6B778F}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12165" activeTab="1" xr2:uid="{C362D381-7D2B-4872-B2C9-60D26B6B778F}"/>
   </bookViews>
   <sheets>
     <sheet name="LL tabulka prediktivní analýzy" sheetId="2" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="311" uniqueCount="131">
   <si>
     <t>&lt;prog&gt;</t>
   </si>
@@ -261,9 +261,6 @@
     <t>&lt;def_func&gt; &lt;new_line&gt; &lt;prog&gt;</t>
   </si>
   <si>
-    <t>&lt;body&gt;  &lt;prog&gt;</t>
-  </si>
-  <si>
     <t>id &lt;body_id&gt; &lt;new_line&gt; &lt;body&gt;</t>
   </si>
   <si>
@@ -315,15 +312,9 @@
     <t>Expression</t>
   </si>
   <si>
-    <t>not &lt;expr&gt;</t>
-  </si>
-  <si>
     <t>&lt;expr&gt; &lt;expr_o&gt;</t>
   </si>
   <si>
-    <t>( &lt;expr&gt; )</t>
-  </si>
-  <si>
     <t>id &lt;expr_o&gt;</t>
   </si>
   <si>
@@ -367,6 +358,72 @@
   </si>
   <si>
     <t>$</t>
+  </si>
+  <si>
+    <t>&lt;expr_id&gt;</t>
+  </si>
+  <si>
+    <t>{id, nil, integer, float, string, (, not}</t>
+  </si>
+  <si>
+    <t>{+}</t>
+  </si>
+  <si>
+    <t>{-}</t>
+  </si>
+  <si>
+    <t>{/}</t>
+  </si>
+  <si>
+    <t>{*}</t>
+  </si>
+  <si>
+    <t>{==}</t>
+  </si>
+  <si>
+    <t>{!=}</t>
+  </si>
+  <si>
+    <t>{&lt;}</t>
+  </si>
+  <si>
+    <t>{&gt;}</t>
+  </si>
+  <si>
+    <t>{&lt;=}</t>
+  </si>
+  <si>
+    <t>{&gt;=}</t>
+  </si>
+  <si>
+    <t>{EOL $}</t>
+  </si>
+  <si>
+    <t>( &lt;expr_id&gt; )</t>
+  </si>
+  <si>
+    <t>not &lt;expr_id&gt;</t>
+  </si>
+  <si>
+    <t>&lt;def_var&gt;</t>
+  </si>
+  <si>
+    <t>&lt;def_var&gt;   -&gt;</t>
+  </si>
+  <si>
+    <t>&lt;def_var_id&gt;   -&gt;</t>
+  </si>
+  <si>
+    <t>id &lt;def_var_id&gt;</t>
+  </si>
+  <si>
+    <t>&lt;def_var_id&gt;</t>
+  </si>
+  <si>
+    <t>{(, id, nil, integer, float, string, +, -, /, *, ==, !=, &lt;, &gt;, &lt;=, &gt;=}</t>
+  </si>
+  <si>
+    <t>&lt;body&gt; &lt;prog&gt;</t>
   </si>
 </sst>
 </file>
@@ -420,7 +477,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="15">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -558,17 +615,6 @@
         <color indexed="64"/>
       </left>
       <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
       <top/>
       <bottom style="thin">
         <color indexed="64"/>
@@ -592,7 +638,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="59">
+  <cellXfs count="57">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -604,9 +650,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
@@ -687,23 +730,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -723,15 +757,11 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -739,7 +769,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
@@ -747,6 +777,16 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1062,10 +1102,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AC8D7845-686F-4A38-8521-27846C315129}">
-  <dimension ref="A1:AE14"/>
+  <dimension ref="A1:AE17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G23" sqref="G23"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1077,696 +1117,889 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A1" s="19"/>
-      <c r="B1" s="23" t="s">
+      <c r="A1" s="18"/>
+      <c r="B1" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="C1" s="23" t="s">
+      <c r="C1" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="D1" s="23" t="s">
+      <c r="D1" s="22" t="s">
         <v>9</v>
       </c>
-      <c r="E1" s="23" t="s">
+      <c r="E1" s="22" t="s">
         <v>10</v>
       </c>
-      <c r="F1" s="23" t="s">
+      <c r="F1" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="G1" s="23" t="s">
+      <c r="G1" s="22" t="s">
         <v>14</v>
       </c>
-      <c r="H1" s="23" t="s">
+      <c r="H1" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="I1" s="23" t="s">
+      <c r="I1" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="J1" s="23" t="s">
+      <c r="J1" s="22" t="s">
         <v>15</v>
       </c>
-      <c r="K1" s="23" t="s">
+      <c r="K1" s="22" t="s">
         <v>16</v>
       </c>
-      <c r="L1" s="23" t="s">
+      <c r="L1" s="22" t="s">
         <v>17</v>
       </c>
-      <c r="M1" s="23" t="s">
+      <c r="M1" s="22" t="s">
         <v>18</v>
       </c>
-      <c r="N1" s="45" t="s">
+      <c r="N1" s="41" t="s">
         <v>19</v>
       </c>
-      <c r="O1" s="23" t="s">
+      <c r="O1" s="22" t="s">
         <v>20</v>
       </c>
-      <c r="P1" s="23" t="s">
+      <c r="P1" s="22" t="s">
         <v>21</v>
       </c>
-      <c r="Q1" s="23" t="s">
+      <c r="Q1" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="R1" s="23" t="s">
+      <c r="R1" s="22" t="s">
         <v>23</v>
       </c>
-      <c r="S1" s="29" t="s">
+      <c r="S1" s="28" t="s">
         <v>24</v>
       </c>
-      <c r="T1" s="23" t="s">
+      <c r="T1" s="22" t="s">
         <v>25</v>
       </c>
-      <c r="U1" s="23" t="s">
+      <c r="U1" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="V1" s="23" t="s">
+      <c r="V1" s="22" t="s">
         <v>29</v>
       </c>
-      <c r="W1" s="23" t="s">
+      <c r="W1" s="22" t="s">
         <v>30</v>
       </c>
-      <c r="X1" s="23" t="s">
+      <c r="X1" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="Y1" s="23" t="s">
+      <c r="Y1" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="Z1" s="23" t="s">
+      <c r="Z1" s="22" t="s">
         <v>32</v>
       </c>
-      <c r="AA1" s="30" t="s">
+      <c r="AA1" s="29" t="s">
         <v>31</v>
       </c>
-      <c r="AB1" s="30" t="s">
+      <c r="AB1" s="29" t="s">
         <v>33</v>
       </c>
-      <c r="AC1" s="30" t="s">
+      <c r="AC1" s="29" t="s">
         <v>34</v>
       </c>
-      <c r="AD1" s="30" t="s">
+      <c r="AD1" s="29" t="s">
         <v>35</v>
       </c>
-      <c r="AE1" s="43" t="s">
-        <v>111</v>
+      <c r="AE1" s="39" t="s">
+        <v>108</v>
       </c>
     </row>
     <row r="2" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A2" s="20" t="s">
+      <c r="A2" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="46">
+      <c r="B2" s="42">
         <v>2</v>
       </c>
-      <c r="C2" s="47">
+      <c r="C2" s="43">
         <v>2</v>
       </c>
-      <c r="D2" s="47">
+      <c r="D2" s="43">
         <v>2</v>
       </c>
-      <c r="E2" s="47">
+      <c r="E2" s="43">
         <v>2</v>
       </c>
-      <c r="F2" s="47">
+      <c r="F2" s="43">
         <v>2</v>
       </c>
-      <c r="G2" s="47">
+      <c r="G2" s="43">
         <v>2</v>
       </c>
-      <c r="H2" s="47">
+      <c r="H2" s="43">
         <v>3</v>
       </c>
-      <c r="I2" s="47"/>
-      <c r="J2" s="47"/>
-      <c r="K2" s="47"/>
-      <c r="L2" s="47"/>
-      <c r="M2" s="47"/>
-      <c r="N2" s="47"/>
-      <c r="O2" s="47"/>
-      <c r="P2" s="47"/>
-      <c r="Q2" s="47"/>
-      <c r="R2" s="47"/>
-      <c r="S2" s="47"/>
-      <c r="T2" s="47">
+      <c r="I2" s="43"/>
+      <c r="J2" s="43"/>
+      <c r="K2" s="43"/>
+      <c r="L2" s="43"/>
+      <c r="M2" s="43"/>
+      <c r="N2" s="43"/>
+      <c r="O2" s="43"/>
+      <c r="P2" s="43"/>
+      <c r="Q2" s="43"/>
+      <c r="R2" s="43"/>
+      <c r="S2" s="43"/>
+      <c r="T2" s="43">
         <v>2</v>
       </c>
-      <c r="U2" s="47"/>
-      <c r="V2" s="47"/>
-      <c r="W2" s="47"/>
-      <c r="X2" s="47">
+      <c r="U2" s="43"/>
+      <c r="V2" s="43"/>
+      <c r="W2" s="43"/>
+      <c r="X2" s="43">
         <v>1</v>
       </c>
-      <c r="Y2" s="47"/>
-      <c r="Z2" s="47">
+      <c r="Y2" s="43"/>
+      <c r="Z2" s="43">
         <v>2</v>
       </c>
-      <c r="AA2" s="47"/>
-      <c r="AB2" s="47"/>
-      <c r="AC2" s="47">
+      <c r="AA2" s="43"/>
+      <c r="AB2" s="43"/>
+      <c r="AC2" s="43">
         <v>2</v>
       </c>
-      <c r="AD2" s="48"/>
-      <c r="AE2" s="49"/>
+      <c r="AD2" s="44"/>
+      <c r="AE2" s="45"/>
     </row>
     <row r="3" spans="1:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="20" t="s">
+      <c r="A3" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="46">
+      <c r="B3" s="42">
         <v>4</v>
       </c>
-      <c r="C3" s="47">
+      <c r="C3" s="43">
         <v>5</v>
       </c>
-      <c r="D3" s="47">
+      <c r="D3" s="43">
         <v>5</v>
       </c>
-      <c r="E3" s="47">
+      <c r="E3" s="43">
         <v>5</v>
       </c>
-      <c r="F3" s="47">
+      <c r="F3" s="43">
         <v>5</v>
       </c>
-      <c r="G3" s="47">
+      <c r="G3" s="43">
         <v>5</v>
       </c>
-      <c r="H3" s="47"/>
-      <c r="I3" s="47"/>
-      <c r="J3" s="47"/>
-      <c r="K3" s="47"/>
-      <c r="L3" s="47"/>
-      <c r="M3" s="47"/>
-      <c r="N3" s="47"/>
-      <c r="O3" s="47"/>
-      <c r="P3" s="47"/>
-      <c r="Q3" s="47"/>
-      <c r="R3" s="47"/>
-      <c r="S3" s="47"/>
-      <c r="T3" s="47">
+      <c r="H3" s="43"/>
+      <c r="I3" s="43"/>
+      <c r="J3" s="43"/>
+      <c r="K3" s="43"/>
+      <c r="L3" s="43"/>
+      <c r="M3" s="43"/>
+      <c r="N3" s="43"/>
+      <c r="O3" s="43"/>
+      <c r="P3" s="43"/>
+      <c r="Q3" s="43"/>
+      <c r="R3" s="43"/>
+      <c r="S3" s="43"/>
+      <c r="T3" s="43">
         <v>5</v>
       </c>
-      <c r="U3" s="47"/>
-      <c r="V3" s="47"/>
-      <c r="W3" s="47"/>
-      <c r="X3" s="47"/>
-      <c r="Y3" s="47">
+      <c r="U3" s="43"/>
+      <c r="V3" s="43"/>
+      <c r="W3" s="43"/>
+      <c r="X3" s="43"/>
+      <c r="Y3" s="43">
         <v>6</v>
       </c>
-      <c r="Z3" s="47">
+      <c r="Z3" s="43">
         <v>7</v>
       </c>
-      <c r="AA3" s="47"/>
-      <c r="AB3" s="47">
+      <c r="AA3" s="43"/>
+      <c r="AB3" s="43">
         <v>6</v>
       </c>
-      <c r="AC3" s="47">
+      <c r="AC3" s="43">
         <v>8</v>
       </c>
-      <c r="AD3" s="48"/>
-      <c r="AE3" s="49">
+      <c r="AD3" s="44"/>
+      <c r="AE3" s="45">
         <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A4" s="20" t="s">
+      <c r="A4" s="19" t="s">
+        <v>84</v>
+      </c>
+      <c r="B4" s="42">
+        <v>11</v>
+      </c>
+      <c r="C4" s="43">
+        <v>11</v>
+      </c>
+      <c r="D4" s="43">
+        <v>11</v>
+      </c>
+      <c r="E4" s="43">
+        <v>11</v>
+      </c>
+      <c r="F4" s="43">
+        <v>11</v>
+      </c>
+      <c r="G4" s="43"/>
+      <c r="H4" s="43"/>
+      <c r="I4" s="43">
+        <v>12</v>
+      </c>
+      <c r="J4" s="43">
+        <v>9</v>
+      </c>
+      <c r="K4" s="43">
+        <v>9</v>
+      </c>
+      <c r="L4" s="43">
+        <v>9</v>
+      </c>
+      <c r="M4" s="43">
+        <v>9</v>
+      </c>
+      <c r="N4" s="43">
+        <v>9</v>
+      </c>
+      <c r="O4" s="43">
+        <v>9</v>
+      </c>
+      <c r="P4" s="43">
+        <v>9</v>
+      </c>
+      <c r="Q4" s="43">
+        <v>9</v>
+      </c>
+      <c r="R4" s="43">
+        <v>9</v>
+      </c>
+      <c r="S4" s="43">
+        <v>9</v>
+      </c>
+      <c r="T4" s="43">
+        <v>11</v>
+      </c>
+      <c r="U4" s="43"/>
+      <c r="V4" s="43">
+        <v>10</v>
+      </c>
+      <c r="W4" s="43"/>
+      <c r="X4" s="43"/>
+      <c r="Y4" s="43"/>
+      <c r="Z4" s="43"/>
+      <c r="AA4" s="43"/>
+      <c r="AB4" s="43"/>
+      <c r="AC4" s="43"/>
+      <c r="AD4" s="44"/>
+      <c r="AE4" s="45"/>
+    </row>
+    <row r="5" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A5" s="19" t="s">
         <v>85</v>
       </c>
-      <c r="B4" s="46">
-        <v>11</v>
-      </c>
-      <c r="C4" s="47">
-        <v>11</v>
-      </c>
-      <c r="D4" s="47">
-        <v>11</v>
-      </c>
-      <c r="E4" s="47">
-        <v>11</v>
-      </c>
-      <c r="F4" s="47">
-        <v>11</v>
-      </c>
-      <c r="G4" s="47"/>
-      <c r="H4" s="47"/>
-      <c r="I4" s="47">
-        <v>12</v>
-      </c>
-      <c r="J4" s="47">
-        <v>9</v>
-      </c>
-      <c r="K4" s="47">
-        <v>9</v>
-      </c>
-      <c r="L4" s="47">
-        <v>9</v>
-      </c>
-      <c r="M4" s="47">
-        <v>9</v>
-      </c>
-      <c r="N4" s="47">
-        <v>9</v>
-      </c>
-      <c r="O4" s="47">
-        <v>9</v>
-      </c>
-      <c r="P4" s="47">
-        <v>9</v>
-      </c>
-      <c r="Q4" s="47">
-        <v>9</v>
-      </c>
-      <c r="R4" s="47">
-        <v>9</v>
-      </c>
-      <c r="S4" s="47">
-        <v>9</v>
-      </c>
-      <c r="T4" s="47">
-        <v>11</v>
-      </c>
-      <c r="U4" s="47"/>
-      <c r="V4" s="47">
-        <v>10</v>
-      </c>
-      <c r="W4" s="47"/>
-      <c r="X4" s="47"/>
-      <c r="Y4" s="47"/>
-      <c r="Z4" s="47"/>
-      <c r="AA4" s="47"/>
-      <c r="AB4" s="47"/>
-      <c r="AC4" s="47"/>
-      <c r="AD4" s="48"/>
-      <c r="AE4" s="49"/>
-    </row>
-    <row r="5" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A5" s="20" t="s">
-        <v>86</v>
-      </c>
-      <c r="B5" s="46"/>
-      <c r="C5" s="47">
+      <c r="B5" s="42"/>
+      <c r="C5" s="43">
         <v>13</v>
       </c>
-      <c r="D5" s="47">
+      <c r="D5" s="43">
         <v>14</v>
       </c>
-      <c r="E5" s="47">
+      <c r="E5" s="43">
         <v>16</v>
       </c>
-      <c r="F5" s="47">
+      <c r="F5" s="43">
         <v>15</v>
       </c>
-      <c r="G5" s="47"/>
-      <c r="H5" s="47"/>
-      <c r="I5" s="47"/>
-      <c r="J5" s="47"/>
-      <c r="K5" s="47"/>
-      <c r="L5" s="47"/>
-      <c r="M5" s="47"/>
-      <c r="N5" s="47"/>
-      <c r="O5" s="47"/>
-      <c r="P5" s="47"/>
-      <c r="Q5" s="47"/>
-      <c r="R5" s="47"/>
-      <c r="S5" s="47"/>
-      <c r="T5" s="47"/>
-      <c r="U5" s="47"/>
-      <c r="V5" s="47"/>
-      <c r="W5" s="47"/>
-      <c r="X5" s="47"/>
-      <c r="Y5" s="47"/>
-      <c r="Z5" s="47"/>
-      <c r="AA5" s="47"/>
-      <c r="AB5" s="47"/>
-      <c r="AC5" s="47"/>
-      <c r="AD5" s="48"/>
-      <c r="AE5" s="49"/>
+      <c r="G5" s="43"/>
+      <c r="H5" s="43"/>
+      <c r="I5" s="43"/>
+      <c r="J5" s="43"/>
+      <c r="K5" s="43"/>
+      <c r="L5" s="43"/>
+      <c r="M5" s="43"/>
+      <c r="N5" s="43"/>
+      <c r="O5" s="43"/>
+      <c r="P5" s="43"/>
+      <c r="Q5" s="43"/>
+      <c r="R5" s="43"/>
+      <c r="S5" s="43"/>
+      <c r="T5" s="43"/>
+      <c r="U5" s="43"/>
+      <c r="V5" s="43"/>
+      <c r="W5" s="43"/>
+      <c r="X5" s="43"/>
+      <c r="Y5" s="43"/>
+      <c r="Z5" s="43"/>
+      <c r="AA5" s="43"/>
+      <c r="AB5" s="43"/>
+      <c r="AC5" s="43"/>
+      <c r="AD5" s="44"/>
+      <c r="AE5" s="45"/>
     </row>
     <row r="6" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A6" s="20" t="s">
+      <c r="A6" s="19" t="s">
         <v>69</v>
       </c>
-      <c r="B6" s="46"/>
-      <c r="C6" s="47"/>
-      <c r="D6" s="47"/>
-      <c r="E6" s="47"/>
-      <c r="F6" s="47"/>
-      <c r="G6" s="47"/>
-      <c r="H6" s="47"/>
-      <c r="I6" s="47">
+      <c r="B6" s="42"/>
+      <c r="C6" s="43"/>
+      <c r="D6" s="43"/>
+      <c r="E6" s="43"/>
+      <c r="F6" s="43"/>
+      <c r="G6" s="43"/>
+      <c r="H6" s="43"/>
+      <c r="I6" s="43">
         <v>17</v>
       </c>
-      <c r="J6" s="47"/>
-      <c r="K6" s="47"/>
-      <c r="L6" s="47"/>
-      <c r="M6" s="47"/>
-      <c r="N6" s="47"/>
-      <c r="O6" s="47"/>
-      <c r="P6" s="47"/>
-      <c r="Q6" s="47"/>
-      <c r="R6" s="47"/>
-      <c r="S6" s="47"/>
-      <c r="T6" s="47"/>
-      <c r="U6" s="47"/>
-      <c r="V6" s="47"/>
-      <c r="W6" s="47"/>
-      <c r="X6" s="47"/>
-      <c r="Y6" s="47"/>
-      <c r="Z6" s="47"/>
-      <c r="AA6" s="47"/>
-      <c r="AB6" s="47"/>
-      <c r="AC6" s="47"/>
-      <c r="AD6" s="48"/>
-      <c r="AE6" s="49"/>
+      <c r="J6" s="43"/>
+      <c r="K6" s="43"/>
+      <c r="L6" s="43"/>
+      <c r="M6" s="43"/>
+      <c r="N6" s="43"/>
+      <c r="O6" s="43"/>
+      <c r="P6" s="43"/>
+      <c r="Q6" s="43"/>
+      <c r="R6" s="43"/>
+      <c r="S6" s="43"/>
+      <c r="T6" s="43"/>
+      <c r="U6" s="43"/>
+      <c r="V6" s="43"/>
+      <c r="W6" s="43"/>
+      <c r="X6" s="43"/>
+      <c r="Y6" s="43"/>
+      <c r="Z6" s="43"/>
+      <c r="AA6" s="43"/>
+      <c r="AB6" s="43"/>
+      <c r="AC6" s="43"/>
+      <c r="AD6" s="44"/>
+      <c r="AE6" s="45"/>
     </row>
     <row r="7" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A7" s="21" t="s">
+      <c r="A7" s="20" t="s">
         <v>73</v>
       </c>
-      <c r="B7" s="47">
+      <c r="B7" s="43">
         <v>18</v>
       </c>
-      <c r="C7" s="47">
+      <c r="C7" s="43">
         <v>18</v>
       </c>
-      <c r="D7" s="47">
+      <c r="D7" s="43">
         <v>18</v>
       </c>
-      <c r="E7" s="47">
+      <c r="E7" s="43">
         <v>18</v>
       </c>
-      <c r="F7" s="47">
+      <c r="F7" s="43">
         <v>18</v>
       </c>
-      <c r="G7" s="47">
+      <c r="G7" s="43">
         <v>18</v>
       </c>
-      <c r="H7" s="47">
+      <c r="H7" s="43">
         <v>18</v>
       </c>
-      <c r="I7" s="47">
+      <c r="I7" s="43">
         <v>19</v>
       </c>
-      <c r="J7" s="47"/>
-      <c r="K7" s="47"/>
-      <c r="L7" s="47"/>
-      <c r="M7" s="47"/>
-      <c r="N7" s="47"/>
-      <c r="O7" s="47"/>
-      <c r="P7" s="47"/>
-      <c r="Q7" s="47"/>
-      <c r="R7" s="47"/>
-      <c r="S7" s="47"/>
-      <c r="T7" s="47">
+      <c r="J7" s="43"/>
+      <c r="K7" s="43"/>
+      <c r="L7" s="43"/>
+      <c r="M7" s="43"/>
+      <c r="N7" s="43"/>
+      <c r="O7" s="43"/>
+      <c r="P7" s="43"/>
+      <c r="Q7" s="43"/>
+      <c r="R7" s="43"/>
+      <c r="S7" s="43"/>
+      <c r="T7" s="43">
         <v>18</v>
       </c>
-      <c r="U7" s="47"/>
-      <c r="V7" s="47"/>
-      <c r="W7" s="47"/>
-      <c r="X7" s="47">
+      <c r="U7" s="43"/>
+      <c r="V7" s="43"/>
+      <c r="W7" s="43"/>
+      <c r="X7" s="43">
         <v>18</v>
       </c>
-      <c r="Y7" s="47"/>
-      <c r="Z7" s="47">
+      <c r="Y7" s="43"/>
+      <c r="Z7" s="43">
         <v>18</v>
       </c>
-      <c r="AA7" s="47">
+      <c r="AA7" s="43">
         <v>18</v>
       </c>
-      <c r="AB7" s="47"/>
-      <c r="AC7" s="47"/>
-      <c r="AD7" s="48"/>
-      <c r="AE7" s="49">
+      <c r="AB7" s="43"/>
+      <c r="AC7" s="43"/>
+      <c r="AD7" s="44"/>
+      <c r="AE7" s="45">
         <v>18</v>
       </c>
     </row>
     <row r="8" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A8" s="21" t="s">
+      <c r="A8" s="20" t="s">
         <v>65</v>
       </c>
-      <c r="B8" s="46"/>
-      <c r="C8" s="47"/>
-      <c r="D8" s="47"/>
-      <c r="E8" s="47"/>
-      <c r="F8" s="47"/>
-      <c r="G8" s="47"/>
-      <c r="H8" s="47"/>
-      <c r="I8" s="47"/>
-      <c r="J8" s="47"/>
-      <c r="K8" s="47"/>
-      <c r="L8" s="47"/>
-      <c r="M8" s="47"/>
-      <c r="N8" s="47"/>
-      <c r="O8" s="47"/>
-      <c r="P8" s="47"/>
-      <c r="Q8" s="47"/>
-      <c r="R8" s="47"/>
-      <c r="S8" s="47"/>
-      <c r="T8" s="47"/>
-      <c r="U8" s="47"/>
-      <c r="V8" s="47"/>
-      <c r="W8" s="47"/>
-      <c r="X8" s="47">
+      <c r="B8" s="42"/>
+      <c r="C8" s="43"/>
+      <c r="D8" s="43"/>
+      <c r="E8" s="43"/>
+      <c r="F8" s="43"/>
+      <c r="G8" s="43"/>
+      <c r="H8" s="43"/>
+      <c r="I8" s="43"/>
+      <c r="J8" s="43"/>
+      <c r="K8" s="43"/>
+      <c r="L8" s="43"/>
+      <c r="M8" s="43"/>
+      <c r="N8" s="43"/>
+      <c r="O8" s="43"/>
+      <c r="P8" s="43"/>
+      <c r="Q8" s="43"/>
+      <c r="R8" s="43"/>
+      <c r="S8" s="43"/>
+      <c r="T8" s="43"/>
+      <c r="U8" s="43"/>
+      <c r="V8" s="43"/>
+      <c r="W8" s="43"/>
+      <c r="X8" s="43">
         <v>20</v>
       </c>
-      <c r="Y8" s="47"/>
-      <c r="Z8" s="47"/>
-      <c r="AA8" s="47"/>
-      <c r="AB8" s="47"/>
-      <c r="AC8" s="47"/>
-      <c r="AD8" s="48"/>
-      <c r="AE8" s="49"/>
+      <c r="Y8" s="43"/>
+      <c r="Z8" s="43"/>
+      <c r="AA8" s="43"/>
+      <c r="AB8" s="43"/>
+      <c r="AC8" s="43"/>
+      <c r="AD8" s="44"/>
+      <c r="AE8" s="45"/>
     </row>
     <row r="9" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A9" s="20" t="s">
+      <c r="A9" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="B9" s="46">
+      <c r="B9" s="42">
         <v>22</v>
       </c>
-      <c r="C9" s="47">
+      <c r="C9" s="43">
         <v>22</v>
       </c>
-      <c r="D9" s="47">
+      <c r="D9" s="43">
         <v>22</v>
       </c>
-      <c r="E9" s="47">
+      <c r="E9" s="43">
         <v>22</v>
       </c>
-      <c r="F9" s="47">
+      <c r="F9" s="43">
         <v>22</v>
       </c>
-      <c r="G9" s="47"/>
-      <c r="H9" s="47"/>
-      <c r="I9" s="47"/>
-      <c r="J9" s="47"/>
-      <c r="K9" s="47"/>
-      <c r="L9" s="47"/>
-      <c r="M9" s="47"/>
-      <c r="N9" s="47"/>
-      <c r="O9" s="47"/>
-      <c r="P9" s="47"/>
-      <c r="Q9" s="47"/>
-      <c r="R9" s="47"/>
-      <c r="S9" s="47"/>
-      <c r="T9" s="47">
+      <c r="G9" s="43"/>
+      <c r="H9" s="43"/>
+      <c r="I9" s="43"/>
+      <c r="J9" s="43"/>
+      <c r="K9" s="43"/>
+      <c r="L9" s="43"/>
+      <c r="M9" s="43"/>
+      <c r="N9" s="43"/>
+      <c r="O9" s="43"/>
+      <c r="P9" s="43"/>
+      <c r="Q9" s="43"/>
+      <c r="R9" s="43"/>
+      <c r="S9" s="43"/>
+      <c r="T9" s="43">
         <v>21</v>
       </c>
-      <c r="U9" s="47"/>
-      <c r="V9" s="47"/>
-      <c r="W9" s="47"/>
-      <c r="X9" s="47"/>
-      <c r="Y9" s="47"/>
-      <c r="Z9" s="47"/>
-      <c r="AA9" s="47"/>
-      <c r="AB9" s="47"/>
-      <c r="AC9" s="47"/>
-      <c r="AD9" s="48"/>
-      <c r="AE9" s="49"/>
+      <c r="U9" s="43"/>
+      <c r="V9" s="43"/>
+      <c r="W9" s="43"/>
+      <c r="X9" s="43"/>
+      <c r="Y9" s="43"/>
+      <c r="Z9" s="43"/>
+      <c r="AA9" s="43"/>
+      <c r="AB9" s="43"/>
+      <c r="AC9" s="43"/>
+      <c r="AD9" s="44"/>
+      <c r="AE9" s="45"/>
     </row>
     <row r="10" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A10" s="20" t="s">
+      <c r="A10" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="B10" s="46">
+      <c r="B10" s="42">
         <v>25</v>
       </c>
-      <c r="C10" s="47">
+      <c r="C10" s="43">
         <v>24</v>
       </c>
-      <c r="D10" s="47">
+      <c r="D10" s="43">
         <v>24</v>
       </c>
-      <c r="E10" s="47">
+      <c r="E10" s="43">
         <v>24</v>
       </c>
-      <c r="F10" s="47">
+      <c r="F10" s="43">
         <v>24</v>
       </c>
-      <c r="G10" s="47"/>
-      <c r="H10" s="47"/>
-      <c r="I10" s="47">
+      <c r="G10" s="43"/>
+      <c r="H10" s="43"/>
+      <c r="I10" s="43">
         <v>23</v>
       </c>
-      <c r="J10" s="47"/>
-      <c r="K10" s="47"/>
-      <c r="L10" s="47"/>
-      <c r="M10" s="47"/>
-      <c r="N10" s="47"/>
-      <c r="O10" s="47"/>
-      <c r="P10" s="47"/>
-      <c r="Q10" s="47"/>
-      <c r="R10" s="47"/>
-      <c r="S10" s="47"/>
-      <c r="T10" s="47"/>
-      <c r="U10" s="47">
+      <c r="J10" s="43"/>
+      <c r="K10" s="43"/>
+      <c r="L10" s="43"/>
+      <c r="M10" s="43"/>
+      <c r="N10" s="43"/>
+      <c r="O10" s="43"/>
+      <c r="P10" s="43"/>
+      <c r="Q10" s="43"/>
+      <c r="R10" s="43"/>
+      <c r="S10" s="43"/>
+      <c r="T10" s="43"/>
+      <c r="U10" s="43">
         <v>23</v>
       </c>
-      <c r="V10" s="47"/>
-      <c r="W10" s="47"/>
-      <c r="X10" s="47"/>
-      <c r="Y10" s="47"/>
-      <c r="Z10" s="47"/>
-      <c r="AA10" s="47"/>
-      <c r="AB10" s="47"/>
-      <c r="AC10" s="47"/>
-      <c r="AD10" s="48"/>
-      <c r="AE10" s="49">
+      <c r="V10" s="43"/>
+      <c r="W10" s="43"/>
+      <c r="X10" s="43"/>
+      <c r="Y10" s="43"/>
+      <c r="Z10" s="43"/>
+      <c r="AA10" s="43"/>
+      <c r="AB10" s="43"/>
+      <c r="AC10" s="43"/>
+      <c r="AD10" s="44"/>
+      <c r="AE10" s="45">
         <v>23</v>
       </c>
     </row>
     <row r="11" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A11" s="20" t="s">
+      <c r="A11" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="B11" s="46"/>
-      <c r="C11" s="47"/>
-      <c r="D11" s="47"/>
-      <c r="E11" s="47"/>
-      <c r="F11" s="47"/>
-      <c r="G11" s="47"/>
-      <c r="H11" s="47"/>
-      <c r="I11" s="47">
+      <c r="B11" s="42"/>
+      <c r="C11" s="43"/>
+      <c r="D11" s="43"/>
+      <c r="E11" s="43"/>
+      <c r="F11" s="43"/>
+      <c r="G11" s="43"/>
+      <c r="H11" s="43"/>
+      <c r="I11" s="43">
         <v>26</v>
       </c>
-      <c r="J11" s="47"/>
-      <c r="K11" s="47"/>
-      <c r="L11" s="47"/>
-      <c r="M11" s="47"/>
-      <c r="N11" s="47"/>
-      <c r="O11" s="47"/>
-      <c r="P11" s="47"/>
-      <c r="Q11" s="47"/>
-      <c r="R11" s="47"/>
-      <c r="S11" s="47"/>
-      <c r="T11" s="47"/>
-      <c r="U11" s="47">
+      <c r="J11" s="43"/>
+      <c r="K11" s="43"/>
+      <c r="L11" s="43"/>
+      <c r="M11" s="43"/>
+      <c r="N11" s="43"/>
+      <c r="O11" s="43"/>
+      <c r="P11" s="43"/>
+      <c r="Q11" s="43"/>
+      <c r="R11" s="43"/>
+      <c r="S11" s="43"/>
+      <c r="T11" s="43"/>
+      <c r="U11" s="43">
         <v>26</v>
       </c>
-      <c r="V11" s="47"/>
-      <c r="W11" s="47">
+      <c r="V11" s="43"/>
+      <c r="W11" s="43">
         <v>27</v>
       </c>
-      <c r="X11" s="47"/>
-      <c r="Y11" s="47"/>
-      <c r="Z11" s="47"/>
-      <c r="AA11" s="47"/>
-      <c r="AB11" s="47"/>
-      <c r="AC11" s="47"/>
-      <c r="AD11" s="48"/>
-      <c r="AE11" s="49">
+      <c r="X11" s="43"/>
+      <c r="Y11" s="43"/>
+      <c r="Z11" s="43"/>
+      <c r="AA11" s="43"/>
+      <c r="AB11" s="43"/>
+      <c r="AC11" s="43"/>
+      <c r="AD11" s="44"/>
+      <c r="AE11" s="45">
         <v>26</v>
       </c>
     </row>
     <row r="12" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A12" s="20" t="s">
+      <c r="A12" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="B12" s="46"/>
-      <c r="C12" s="47"/>
-      <c r="D12" s="47"/>
-      <c r="E12" s="47"/>
-      <c r="F12" s="47"/>
-      <c r="G12" s="47"/>
-      <c r="H12" s="47"/>
-      <c r="I12" s="47"/>
-      <c r="J12" s="47"/>
-      <c r="K12" s="47"/>
-      <c r="L12" s="47"/>
-      <c r="M12" s="47"/>
-      <c r="N12" s="47"/>
-      <c r="O12" s="47"/>
-      <c r="P12" s="47"/>
-      <c r="Q12" s="47"/>
-      <c r="R12" s="47"/>
-      <c r="S12" s="47"/>
-      <c r="T12" s="47"/>
-      <c r="U12" s="47"/>
-      <c r="V12" s="47"/>
-      <c r="W12" s="47"/>
-      <c r="X12" s="47"/>
-      <c r="Y12" s="47"/>
-      <c r="Z12" s="47">
+      <c r="B12" s="42"/>
+      <c r="C12" s="43"/>
+      <c r="D12" s="43"/>
+      <c r="E12" s="43"/>
+      <c r="F12" s="43"/>
+      <c r="G12" s="43"/>
+      <c r="H12" s="43"/>
+      <c r="I12" s="43"/>
+      <c r="J12" s="43"/>
+      <c r="K12" s="43"/>
+      <c r="L12" s="43"/>
+      <c r="M12" s="43"/>
+      <c r="N12" s="43"/>
+      <c r="O12" s="43"/>
+      <c r="P12" s="43"/>
+      <c r="Q12" s="43"/>
+      <c r="R12" s="43"/>
+      <c r="S12" s="43"/>
+      <c r="T12" s="43"/>
+      <c r="U12" s="43"/>
+      <c r="V12" s="43"/>
+      <c r="W12" s="43"/>
+      <c r="X12" s="43"/>
+      <c r="Y12" s="43"/>
+      <c r="Z12" s="43">
         <v>28</v>
       </c>
-      <c r="AA12" s="47"/>
-      <c r="AB12" s="47"/>
-      <c r="AC12" s="47"/>
-      <c r="AD12" s="48"/>
-      <c r="AE12" s="49"/>
+      <c r="AA12" s="43"/>
+      <c r="AB12" s="43"/>
+      <c r="AC12" s="43"/>
+      <c r="AD12" s="44"/>
+      <c r="AE12" s="45"/>
     </row>
     <row r="13" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A13" s="22" t="s">
+      <c r="A13" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="B13" s="50"/>
-      <c r="C13" s="51"/>
-      <c r="D13" s="51"/>
-      <c r="E13" s="51"/>
-      <c r="F13" s="51"/>
-      <c r="G13" s="51"/>
-      <c r="H13" s="51"/>
-      <c r="I13" s="51"/>
-      <c r="J13" s="51"/>
-      <c r="K13" s="51"/>
-      <c r="L13" s="51"/>
-      <c r="M13" s="51"/>
-      <c r="N13" s="51"/>
-      <c r="O13" s="51"/>
-      <c r="P13" s="51"/>
-      <c r="Q13" s="51"/>
-      <c r="R13" s="51"/>
-      <c r="S13" s="51"/>
-      <c r="T13" s="51"/>
-      <c r="U13" s="51"/>
-      <c r="V13" s="51"/>
-      <c r="W13" s="51"/>
-      <c r="X13" s="51"/>
-      <c r="Y13" s="51"/>
-      <c r="Z13" s="51"/>
-      <c r="AA13" s="51"/>
-      <c r="AB13" s="51"/>
-      <c r="AC13" s="51">
+      <c r="B13" s="42"/>
+      <c r="C13" s="43"/>
+      <c r="D13" s="43"/>
+      <c r="E13" s="43"/>
+      <c r="F13" s="43"/>
+      <c r="G13" s="43"/>
+      <c r="H13" s="43"/>
+      <c r="I13" s="43"/>
+      <c r="J13" s="43"/>
+      <c r="K13" s="43"/>
+      <c r="L13" s="43"/>
+      <c r="M13" s="43"/>
+      <c r="N13" s="43"/>
+      <c r="O13" s="43"/>
+      <c r="P13" s="43"/>
+      <c r="Q13" s="43"/>
+      <c r="R13" s="43"/>
+      <c r="S13" s="43"/>
+      <c r="T13" s="43"/>
+      <c r="U13" s="43"/>
+      <c r="V13" s="43"/>
+      <c r="W13" s="43"/>
+      <c r="X13" s="43"/>
+      <c r="Y13" s="43"/>
+      <c r="Z13" s="43"/>
+      <c r="AA13" s="43"/>
+      <c r="AB13" s="43"/>
+      <c r="AC13" s="43">
         <v>29</v>
       </c>
-      <c r="AD13" s="52"/>
-      <c r="AE13" s="53"/>
+      <c r="AD13" s="54"/>
+      <c r="AE13" s="45"/>
     </row>
     <row r="14" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A14" s="42"/>
-      <c r="B14" s="6"/>
-      <c r="C14" s="6"/>
-      <c r="D14" s="6"/>
-      <c r="E14" s="6"/>
-      <c r="F14" s="6"/>
-      <c r="G14" s="6"/>
-      <c r="H14" s="6"/>
-      <c r="I14" s="6"/>
-      <c r="J14" s="6"/>
-      <c r="K14" s="6"/>
-      <c r="L14" s="6"/>
-      <c r="M14" s="6"/>
-      <c r="N14" s="6"/>
-      <c r="O14" s="44"/>
-      <c r="P14" s="7"/>
-      <c r="S14" s="7"/>
+      <c r="A14" s="20" t="s">
+        <v>109</v>
+      </c>
+      <c r="B14" s="5">
+        <v>30</v>
+      </c>
+      <c r="C14" s="5">
+        <v>31</v>
+      </c>
+      <c r="D14" s="5">
+        <v>31</v>
+      </c>
+      <c r="E14" s="5">
+        <v>31</v>
+      </c>
+      <c r="F14" s="5">
+        <v>31</v>
+      </c>
+      <c r="G14" s="5">
+        <v>31</v>
+      </c>
+      <c r="H14" s="5"/>
+      <c r="I14" s="5"/>
+      <c r="J14" s="5"/>
+      <c r="K14" s="5"/>
+      <c r="L14" s="5"/>
+      <c r="M14" s="5"/>
+      <c r="N14" s="5"/>
+      <c r="O14" s="40"/>
+      <c r="P14" s="5"/>
+      <c r="Q14" s="1"/>
+      <c r="R14" s="1"/>
+      <c r="S14" s="5"/>
+      <c r="T14" s="1">
+        <v>31</v>
+      </c>
+      <c r="U14" s="1"/>
+      <c r="V14" s="1"/>
+      <c r="W14" s="1"/>
+      <c r="X14" s="1"/>
+      <c r="Y14" s="1"/>
+      <c r="Z14" s="1"/>
+      <c r="AA14" s="1"/>
+      <c r="AB14" s="1"/>
+      <c r="AC14" s="1"/>
+      <c r="AD14" s="1"/>
+      <c r="AE14" s="24"/>
+    </row>
+    <row r="15" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A15" s="20" t="s">
+        <v>77</v>
+      </c>
+      <c r="B15" s="5"/>
+      <c r="C15" s="5"/>
+      <c r="D15" s="5"/>
+      <c r="E15" s="5"/>
+      <c r="F15" s="5"/>
+      <c r="G15" s="5"/>
+      <c r="H15" s="5"/>
+      <c r="I15" s="5">
+        <v>42</v>
+      </c>
+      <c r="J15" s="5">
+        <v>32</v>
+      </c>
+      <c r="K15" s="5">
+        <v>33</v>
+      </c>
+      <c r="L15" s="5">
+        <v>34</v>
+      </c>
+      <c r="M15" s="5">
+        <v>35</v>
+      </c>
+      <c r="N15" s="5">
+        <v>36</v>
+      </c>
+      <c r="O15" s="5">
+        <v>37</v>
+      </c>
+      <c r="P15" s="5">
+        <v>38</v>
+      </c>
+      <c r="Q15" s="5">
+        <v>39</v>
+      </c>
+      <c r="R15" s="5">
+        <v>40</v>
+      </c>
+      <c r="S15" s="5">
+        <v>41</v>
+      </c>
+      <c r="T15" s="5"/>
+      <c r="U15" s="5"/>
+      <c r="V15" s="5"/>
+      <c r="W15" s="5"/>
+      <c r="X15" s="5"/>
+      <c r="Y15" s="5"/>
+      <c r="Z15" s="5"/>
+      <c r="AA15" s="5"/>
+      <c r="AB15" s="5"/>
+      <c r="AC15" s="5"/>
+      <c r="AD15" s="5"/>
+      <c r="AE15" s="24">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="16" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A16" s="20" t="s">
+        <v>124</v>
+      </c>
+      <c r="B16" s="1">
+        <v>44</v>
+      </c>
+      <c r="C16" s="1">
+        <v>43</v>
+      </c>
+      <c r="D16" s="1">
+        <v>43</v>
+      </c>
+      <c r="E16" s="1">
+        <v>43</v>
+      </c>
+      <c r="F16" s="1">
+        <v>43</v>
+      </c>
+      <c r="G16" s="1">
+        <v>43</v>
+      </c>
+      <c r="T16" s="1">
+        <v>43</v>
+      </c>
+      <c r="U16" s="1"/>
+      <c r="V16" s="1"/>
+      <c r="W16" s="1"/>
+      <c r="X16" s="1"/>
+      <c r="Y16" s="1"/>
+      <c r="Z16" s="1"/>
+      <c r="AA16" s="1"/>
+      <c r="AB16" s="1"/>
+      <c r="AC16" s="1"/>
+      <c r="AD16" s="1"/>
+      <c r="AE16" s="24"/>
+    </row>
+    <row r="17" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A17" s="27" t="s">
+        <v>128</v>
+      </c>
+      <c r="B17" s="17">
+        <v>46</v>
+      </c>
+      <c r="C17" s="17">
+        <v>46</v>
+      </c>
+      <c r="D17" s="17">
+        <v>46</v>
+      </c>
+      <c r="E17" s="17">
+        <v>46</v>
+      </c>
+      <c r="F17" s="17">
+        <v>46</v>
+      </c>
+      <c r="G17" s="17"/>
+      <c r="H17" s="17"/>
+      <c r="I17" s="17"/>
+      <c r="J17" s="17">
+        <v>45</v>
+      </c>
+      <c r="K17" s="17">
+        <v>45</v>
+      </c>
+      <c r="L17" s="17">
+        <v>45</v>
+      </c>
+      <c r="M17" s="17">
+        <v>45</v>
+      </c>
+      <c r="N17" s="17">
+        <v>45</v>
+      </c>
+      <c r="O17" s="17">
+        <v>45</v>
+      </c>
+      <c r="P17" s="17">
+        <v>45</v>
+      </c>
+      <c r="Q17" s="17">
+        <v>45</v>
+      </c>
+      <c r="R17" s="17">
+        <v>45</v>
+      </c>
+      <c r="S17" s="17">
+        <v>45</v>
+      </c>
+      <c r="T17" s="17">
+        <v>46</v>
+      </c>
+      <c r="U17" s="17"/>
+      <c r="V17" s="17"/>
+      <c r="W17" s="17"/>
+      <c r="X17" s="17"/>
+      <c r="Y17" s="17"/>
+      <c r="Z17" s="17"/>
+      <c r="AA17" s="17"/>
+      <c r="AB17" s="17"/>
+      <c r="AC17" s="17"/>
+      <c r="AD17" s="17"/>
+      <c r="AE17" s="55"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
@@ -1776,10 +2009,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B9B981D-AC8B-4430-B1E8-C28C34350FA5}">
-  <dimension ref="A1:AK42"/>
+  <dimension ref="A1:AK47"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1800,144 +2033,144 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A1" s="19"/>
-      <c r="B1" s="23" t="s">
+      <c r="A1" s="18"/>
+      <c r="B1" s="22" t="s">
         <v>37</v>
       </c>
-      <c r="C1" s="23" t="s">
+      <c r="C1" s="22" t="s">
         <v>41</v>
       </c>
-      <c r="D1" s="23" t="s">
+      <c r="D1" s="22" t="s">
         <v>46</v>
       </c>
-      <c r="E1" s="7"/>
-      <c r="F1" s="19"/>
-      <c r="G1" s="54" t="s">
+      <c r="E1" s="6"/>
+      <c r="F1" s="18"/>
+      <c r="G1" s="48" t="s">
         <v>61</v>
       </c>
-      <c r="H1" s="54"/>
-      <c r="I1" s="55"/>
-      <c r="J1" s="30" t="s">
+      <c r="H1" s="48"/>
+      <c r="I1" s="49"/>
+      <c r="J1" s="29" t="s">
         <v>48</v>
       </c>
-      <c r="K1" s="34"/>
-      <c r="L1" s="19"/>
-      <c r="M1" s="56" t="s">
-        <v>93</v>
-      </c>
-      <c r="N1" s="57"/>
-      <c r="O1" s="58"/>
-      <c r="P1" s="7"/>
-      <c r="Q1" s="7"/>
-      <c r="R1" s="7"/>
-      <c r="S1" s="7"/>
-      <c r="T1" s="7"/>
-      <c r="U1" s="7"/>
-      <c r="V1" s="7"/>
-      <c r="W1" s="7"/>
-      <c r="X1" s="7"/>
-      <c r="Y1" s="7"/>
-      <c r="Z1" s="7"/>
-      <c r="AA1" s="7"/>
-      <c r="AB1" s="7"/>
+      <c r="K1" s="33"/>
+      <c r="L1" s="18"/>
+      <c r="M1" s="50" t="s">
+        <v>92</v>
+      </c>
+      <c r="N1" s="51"/>
+      <c r="O1" s="52"/>
+      <c r="P1" s="6"/>
+      <c r="Q1" s="6"/>
+      <c r="R1" s="6"/>
+      <c r="S1" s="6"/>
+      <c r="T1" s="6"/>
+      <c r="U1" s="6"/>
+      <c r="V1" s="6"/>
+      <c r="W1" s="6"/>
+      <c r="X1" s="6"/>
+      <c r="Y1" s="6"/>
+      <c r="Z1" s="6"/>
+      <c r="AA1" s="6"/>
+      <c r="AB1" s="6"/>
     </row>
     <row r="2" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A2" s="20" t="s">
+      <c r="A2" s="53" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>36</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>100</v>
-      </c>
-      <c r="D2" s="24" t="s">
+        <v>97</v>
+      </c>
+      <c r="D2" s="23" t="s">
         <v>62</v>
       </c>
       <c r="E2" s="1"/>
-      <c r="F2" s="20">
+      <c r="F2" s="19">
         <v>1</v>
       </c>
-      <c r="G2" s="8" t="s">
+      <c r="G2" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="H2" s="8"/>
-      <c r="I2" s="15" t="s">
+      <c r="H2" s="7"/>
+      <c r="I2" s="14" t="s">
         <v>75</v>
       </c>
-      <c r="J2" s="13" t="s">
+      <c r="J2" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="K2" s="6"/>
+      <c r="K2" s="5"/>
       <c r="L2" s="4">
         <v>1</v>
       </c>
-      <c r="M2" s="35" t="s">
-        <v>90</v>
-      </c>
-      <c r="N2" s="6"/>
-      <c r="O2" s="10" t="s">
-        <v>86</v>
-      </c>
-      <c r="P2" s="6"/>
-      <c r="Q2" s="6"/>
-      <c r="R2" s="6"/>
-      <c r="S2" s="6"/>
-      <c r="T2" s="6"/>
-      <c r="U2" s="6"/>
-      <c r="V2" s="6"/>
-      <c r="W2" s="6"/>
-      <c r="X2" s="6"/>
-      <c r="Y2" s="6"/>
-      <c r="Z2" s="6"/>
-      <c r="AA2" s="6"/>
-      <c r="AB2" s="6"/>
-      <c r="AC2" s="7"/>
-      <c r="AD2" s="7"/>
-      <c r="AE2" s="7"/>
-      <c r="AF2" s="7"/>
-      <c r="AG2" s="7"/>
-      <c r="AH2" s="7"/>
-      <c r="AI2" s="7"/>
-      <c r="AJ2" s="7"/>
-      <c r="AK2" s="7"/>
+      <c r="M2" s="34" t="s">
+        <v>89</v>
+      </c>
+      <c r="N2" s="5"/>
+      <c r="O2" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="P2" s="5"/>
+      <c r="Q2" s="5"/>
+      <c r="R2" s="5"/>
+      <c r="S2" s="5"/>
+      <c r="T2" s="5"/>
+      <c r="U2" s="5"/>
+      <c r="V2" s="5"/>
+      <c r="W2" s="5"/>
+      <c r="X2" s="5"/>
+      <c r="Y2" s="5"/>
+      <c r="Z2" s="5"/>
+      <c r="AA2" s="5"/>
+      <c r="AB2" s="5"/>
+      <c r="AC2" s="6"/>
+      <c r="AD2" s="6"/>
+      <c r="AE2" s="6"/>
+      <c r="AF2" s="6"/>
+      <c r="AG2" s="6"/>
+      <c r="AH2" s="6"/>
+      <c r="AI2" s="6"/>
+      <c r="AJ2" s="6"/>
+      <c r="AK2" s="6"/>
     </row>
     <row r="3" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A3" s="20" t="s">
+      <c r="A3" s="19" t="s">
         <v>1</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>38</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>99</v>
-      </c>
-      <c r="D3" s="25" t="s">
-        <v>101</v>
+        <v>96</v>
+      </c>
+      <c r="D3" s="24" t="s">
+        <v>98</v>
       </c>
       <c r="E3" s="1"/>
-      <c r="F3" s="31">
+      <c r="F3" s="30">
         <v>2</v>
       </c>
-      <c r="G3" s="8" t="s">
+      <c r="G3" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="H3" s="7"/>
-      <c r="I3" s="32" t="s">
-        <v>76</v>
+      <c r="H3" s="6"/>
+      <c r="I3" s="31" t="s">
+        <v>130</v>
       </c>
       <c r="J3" s="4" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="L3" s="4">
         <v>2</v>
       </c>
-      <c r="M3" s="35" t="s">
-        <v>90</v>
-      </c>
-      <c r="N3" s="6"/>
-      <c r="O3" s="10" t="s">
-        <v>94</v>
+      <c r="M3" s="34" t="s">
+        <v>89</v>
+      </c>
+      <c r="N3" s="5"/>
+      <c r="O3" s="9" t="s">
+        <v>123</v>
       </c>
       <c r="P3" s="1"/>
       <c r="Q3" s="1"/>
@@ -1954,27 +2187,27 @@
       <c r="AB3" s="1"/>
     </row>
     <row r="4" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A4" s="20" t="s">
-        <v>85</v>
+      <c r="A4" s="19" t="s">
+        <v>84</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>36</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="D4" s="4" t="s">
         <v>47</v>
       </c>
       <c r="E4" s="1"/>
-      <c r="F4" s="20">
+      <c r="F4" s="19">
         <v>3</v>
       </c>
-      <c r="G4" s="8" t="s">
+      <c r="G4" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="H4" s="7"/>
-      <c r="I4" s="14" t="s">
+      <c r="H4" s="6"/>
+      <c r="I4" s="13" t="s">
         <v>13</v>
       </c>
       <c r="J4" s="4" t="s">
@@ -1983,12 +2216,12 @@
       <c r="L4" s="4">
         <v>3</v>
       </c>
-      <c r="M4" s="35" t="s">
-        <v>90</v>
-      </c>
-      <c r="N4" s="6"/>
-      <c r="O4" s="10" t="s">
-        <v>95</v>
+      <c r="M4" s="34" t="s">
+        <v>89</v>
+      </c>
+      <c r="N4" s="5"/>
+      <c r="O4" s="9" t="s">
+        <v>93</v>
       </c>
       <c r="P4" s="1"/>
       <c r="Q4" s="1"/>
@@ -2005,42 +2238,42 @@
       <c r="AB4" s="1"/>
     </row>
     <row r="5" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A5" s="20" t="s">
-        <v>86</v>
+      <c r="A5" s="19" t="s">
+        <v>85</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>38</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D5" s="4" t="s">
         <v>43</v>
       </c>
       <c r="E5" s="1"/>
-      <c r="F5" s="31">
+      <c r="F5" s="30">
         <v>4</v>
       </c>
-      <c r="G5" s="8" t="s">
+      <c r="G5" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="H5" s="8"/>
-      <c r="I5" s="10" t="s">
-        <v>77</v>
+      <c r="H5" s="7"/>
+      <c r="I5" s="9" t="s">
+        <v>76</v>
       </c>
       <c r="J5" s="4" t="s">
         <v>39</v>
       </c>
       <c r="K5" s="1"/>
-      <c r="L5" s="4">
+      <c r="L5" s="2">
         <v>4</v>
       </c>
-      <c r="M5" s="35" t="s">
-        <v>90</v>
-      </c>
-      <c r="N5" s="6"/>
-      <c r="O5" s="10" t="s">
-        <v>96</v>
+      <c r="M5" s="37" t="s">
+        <v>89</v>
+      </c>
+      <c r="N5" s="17"/>
+      <c r="O5" s="47" t="s">
+        <v>122</v>
       </c>
       <c r="P5" s="1"/>
       <c r="Q5" s="1"/>
@@ -2057,7 +2290,7 @@
       <c r="AB5" s="1"/>
     </row>
     <row r="6" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A6" s="20" t="s">
+      <c r="A6" s="19" t="s">
         <v>69</v>
       </c>
       <c r="B6" s="3" t="s">
@@ -2067,33 +2300,27 @@
         <v>47</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="E6" s="1"/>
-      <c r="F6" s="31">
+      <c r="F6" s="30">
         <v>5</v>
       </c>
-      <c r="G6" s="8" t="s">
+      <c r="G6" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="H6" s="8"/>
-      <c r="I6" s="10" t="s">
+      <c r="H6" s="7"/>
+      <c r="I6" s="9" t="s">
         <v>74</v>
       </c>
       <c r="J6" s="4" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="K6" s="1"/>
-      <c r="L6" s="4">
-        <v>5</v>
-      </c>
-      <c r="M6" s="35" t="s">
-        <v>91</v>
-      </c>
-      <c r="N6" s="6"/>
-      <c r="O6" s="10" t="s">
-        <v>97</v>
-      </c>
+      <c r="L6" s="5"/>
+      <c r="M6" s="7"/>
+      <c r="N6" s="5"/>
+      <c r="O6" s="10"/>
       <c r="P6" s="1"/>
       <c r="Q6" s="1"/>
       <c r="R6" s="1"/>
@@ -2109,42 +2336,36 @@
       <c r="AB6" s="1"/>
     </row>
     <row r="7" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A7" s="21" t="s">
+      <c r="A7" s="20" t="s">
         <v>73</v>
       </c>
       <c r="B7" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="C7" s="13" t="s">
+      <c r="C7" s="12" t="s">
         <v>47</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="E7" s="1"/>
-      <c r="F7" s="31">
+      <c r="F7" s="30">
         <v>6</v>
       </c>
-      <c r="G7" s="8" t="s">
+      <c r="G7" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="I7" s="14" t="s">
+      <c r="I7" s="13" t="s">
         <v>51</v>
       </c>
-      <c r="J7" s="25" t="s">
-        <v>101</v>
+      <c r="J7" s="24" t="s">
+        <v>98</v>
       </c>
       <c r="K7" s="1"/>
-      <c r="L7" s="4">
-        <v>6</v>
-      </c>
-      <c r="M7" s="35" t="s">
-        <v>91</v>
-      </c>
-      <c r="N7" s="6"/>
-      <c r="O7" s="10" t="s">
-        <v>68</v>
-      </c>
+      <c r="L7" s="5"/>
+      <c r="M7" s="7"/>
+      <c r="N7" s="5"/>
+      <c r="O7" s="10"/>
       <c r="P7" s="1"/>
       <c r="Q7" s="1"/>
       <c r="R7" s="1"/>
@@ -2160,43 +2381,36 @@
       <c r="AB7" s="1"/>
     </row>
     <row r="8" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A8" s="26" t="s">
+      <c r="A8" s="20" t="s">
         <v>65</v>
       </c>
-      <c r="B8" s="17" t="s">
+      <c r="B8" s="16" t="s">
         <v>36</v>
       </c>
-      <c r="C8" s="13" t="s">
+      <c r="C8" s="12" t="s">
         <v>42</v>
       </c>
       <c r="D8" s="4" t="s">
         <v>47</v>
       </c>
       <c r="E8" s="1"/>
-      <c r="F8" s="31">
+      <c r="F8" s="30">
         <v>7</v>
       </c>
-      <c r="G8" s="8" t="s">
+      <c r="G8" s="7" t="s">
         <v>49</v>
       </c>
       <c r="I8" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="J8" s="4" t="s">
         <v>44</v>
       </c>
       <c r="K8" s="1"/>
-      <c r="L8" s="4">
-        <v>7</v>
-      </c>
-      <c r="M8" s="35" t="s">
-        <v>92</v>
-      </c>
-      <c r="N8" s="6"/>
-      <c r="O8" s="10" t="str">
-        <f xml:space="preserve"> "+ &lt;expr_id&gt;"</f>
-        <v>+ &lt;expr_id&gt;</v>
-      </c>
+      <c r="L8" s="5"/>
+      <c r="M8" s="7"/>
+      <c r="N8" s="5"/>
+      <c r="O8" s="10"/>
       <c r="P8" s="1"/>
       <c r="Q8" s="1"/>
       <c r="R8" s="1"/>
@@ -2212,43 +2426,36 @@
       <c r="AB8" s="1"/>
     </row>
     <row r="9" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A9" s="20" t="s">
+      <c r="A9" s="19" t="s">
         <v>2</v>
       </c>
       <c r="B9" s="4" t="s">
         <v>38</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="E9" s="1"/>
-      <c r="F9" s="31">
+      <c r="F9" s="30">
         <v>8</v>
       </c>
-      <c r="G9" s="8" t="s">
+      <c r="G9" s="7" t="s">
         <v>49</v>
       </c>
       <c r="I9" t="s">
-        <v>82</v>
-      </c>
-      <c r="J9" s="16" t="s">
+        <v>81</v>
+      </c>
+      <c r="J9" s="15" t="s">
         <v>45</v>
       </c>
       <c r="K9" s="1"/>
-      <c r="L9" s="4">
-        <v>8</v>
-      </c>
-      <c r="M9" s="35" t="s">
-        <v>92</v>
-      </c>
-      <c r="N9" s="6"/>
-      <c r="O9" s="10" t="str">
-        <f xml:space="preserve"> "- &lt;expr_id&gt;"</f>
-        <v>- &lt;expr_id&gt;</v>
-      </c>
+      <c r="L9" s="5"/>
+      <c r="M9" s="7"/>
+      <c r="N9" s="5"/>
+      <c r="O9" s="10"/>
       <c r="P9" s="1"/>
       <c r="Q9" s="1"/>
       <c r="R9" s="1"/>
@@ -2264,43 +2471,36 @@
       <c r="AB9" s="1"/>
     </row>
     <row r="10" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A10" s="20" t="s">
+      <c r="A10" s="19" t="s">
         <v>3</v>
       </c>
       <c r="B10" s="4" t="s">
         <v>38</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="E10" s="1"/>
-      <c r="F10" s="31">
+      <c r="F10" s="30">
         <v>9</v>
       </c>
-      <c r="G10" s="8" t="s">
-        <v>79</v>
-      </c>
-      <c r="I10" s="10" t="s">
+      <c r="G10" s="7" t="s">
         <v>78</v>
       </c>
+      <c r="I10" s="9" t="s">
+        <v>77</v>
+      </c>
       <c r="J10" s="4" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="K10" s="1"/>
-      <c r="L10" s="4">
-        <v>9</v>
-      </c>
-      <c r="M10" s="35" t="s">
-        <v>92</v>
-      </c>
-      <c r="N10" s="6"/>
-      <c r="O10" s="10" t="str">
-        <f xml:space="preserve"> "/ &lt;expr_id&gt;"</f>
-        <v>/ &lt;expr_id&gt;</v>
-      </c>
+      <c r="L10" s="5"/>
+      <c r="M10" s="7"/>
+      <c r="N10" s="5"/>
+      <c r="O10" s="10"/>
       <c r="P10" s="1"/>
       <c r="Q10" s="1"/>
       <c r="R10" s="1"/>
@@ -2316,7 +2516,7 @@
       <c r="AB10" s="1"/>
     </row>
     <row r="11" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A11" s="20" t="s">
+      <c r="A11" s="19" t="s">
         <v>4</v>
       </c>
       <c r="B11" s="4" t="s">
@@ -2326,51 +2526,44 @@
         <v>43</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>104</v>
-      </c>
-      <c r="E11" s="6"/>
-      <c r="F11" s="31">
+        <v>101</v>
+      </c>
+      <c r="E11" s="5"/>
+      <c r="F11" s="30">
         <v>10</v>
       </c>
-      <c r="G11" s="8" t="s">
-        <v>79</v>
-      </c>
-      <c r="H11" s="8"/>
-      <c r="I11" s="12" t="str">
-        <f>"= &lt;expr&gt;"</f>
-        <v>= &lt;expr&gt;</v>
+      <c r="G11" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="H11" s="7"/>
+      <c r="I11" s="11" t="str">
+        <f>"= &lt;defvar&gt;"</f>
+        <v>= &lt;defvar&gt;</v>
       </c>
       <c r="J11" s="4" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="K11" s="1"/>
-      <c r="L11" s="4">
-        <v>10</v>
-      </c>
-      <c r="M11" s="35" t="s">
-        <v>92</v>
-      </c>
-      <c r="N11" s="6"/>
-      <c r="O11" s="10" t="str">
-        <f xml:space="preserve"> "* &lt;expr_id&gt;"</f>
-        <v>* &lt;expr_id&gt;</v>
-      </c>
-      <c r="P11" s="6"/>
-      <c r="Q11" s="6"/>
-      <c r="R11" s="6"/>
-      <c r="S11" s="6"/>
-      <c r="T11" s="6"/>
-      <c r="U11" s="6"/>
-      <c r="V11" s="6"/>
-      <c r="W11" s="6"/>
-      <c r="X11" s="6"/>
-      <c r="Y11" s="6"/>
-      <c r="Z11" s="6"/>
-      <c r="AA11" s="6"/>
-      <c r="AB11" s="6"/>
+      <c r="L11" s="5"/>
+      <c r="M11" s="7"/>
+      <c r="N11" s="5"/>
+      <c r="O11" s="10"/>
+      <c r="P11" s="5"/>
+      <c r="Q11" s="5"/>
+      <c r="R11" s="5"/>
+      <c r="S11" s="5"/>
+      <c r="T11" s="5"/>
+      <c r="U11" s="5"/>
+      <c r="V11" s="5"/>
+      <c r="W11" s="5"/>
+      <c r="X11" s="5"/>
+      <c r="Y11" s="5"/>
+      <c r="Z11" s="5"/>
+      <c r="AA11" s="5"/>
+      <c r="AB11" s="5"/>
     </row>
     <row r="12" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A12" s="20" t="s">
+      <c r="A12" s="19" t="s">
         <v>5</v>
       </c>
       <c r="B12" s="3" t="s">
@@ -2382,31 +2575,24 @@
       <c r="D12" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="E12" s="6"/>
-      <c r="F12" s="31">
+      <c r="E12" s="5"/>
+      <c r="F12" s="30">
         <v>11</v>
       </c>
-      <c r="G12" s="8" t="s">
-        <v>79</v>
-      </c>
-      <c r="H12" s="8"/>
-      <c r="I12" s="10" t="s">
+      <c r="G12" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="H12" s="7"/>
+      <c r="I12" s="9" t="s">
         <v>2</v>
       </c>
       <c r="J12" s="4" t="s">
-        <v>88</v>
-      </c>
-      <c r="L12" s="4">
-        <v>11</v>
-      </c>
-      <c r="M12" s="35" t="s">
-        <v>92</v>
-      </c>
-      <c r="N12" s="6"/>
-      <c r="O12" s="10" t="str">
-        <f xml:space="preserve"> "== &lt;expr_id&gt;"</f>
-        <v>== &lt;expr_id&gt;</v>
-      </c>
+        <v>87</v>
+      </c>
+      <c r="L12" s="5"/>
+      <c r="M12" s="7"/>
+      <c r="N12" s="5"/>
+      <c r="O12" s="10"/>
       <c r="P12" s="1"/>
       <c r="Q12" s="1"/>
       <c r="R12" s="1"/>
@@ -2422,43 +2608,36 @@
       <c r="AB12" s="1"/>
     </row>
     <row r="13" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A13" s="22" t="s">
+      <c r="A13" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="B13" s="5" t="s">
+      <c r="B13" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="C13" s="2" t="s">
+      <c r="C13" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="D13" s="4" t="s">
+      <c r="D13" s="24" t="s">
         <v>47</v>
       </c>
       <c r="E13" s="1"/>
-      <c r="F13" s="31">
+      <c r="F13" s="30">
         <v>12</v>
       </c>
-      <c r="G13" s="8" t="s">
-        <v>79</v>
-      </c>
-      <c r="H13" s="8"/>
-      <c r="I13" s="14" t="s">
+      <c r="G13" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="H13" s="7"/>
+      <c r="I13" s="13" t="s">
         <v>51</v>
       </c>
       <c r="J13" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="L13" s="4">
-        <v>12</v>
-      </c>
-      <c r="M13" s="35" t="s">
-        <v>92</v>
-      </c>
-      <c r="N13" s="6"/>
-      <c r="O13" s="10" t="str">
-        <f xml:space="preserve"> "!= &lt;expr_id&gt;"</f>
-        <v>!= &lt;expr_id&gt;</v>
-      </c>
+      <c r="L13" s="5"/>
+      <c r="M13" s="7"/>
+      <c r="N13" s="5"/>
+      <c r="O13" s="10"/>
       <c r="P13" s="1"/>
       <c r="Q13" s="1"/>
       <c r="R13" s="1"/>
@@ -2475,41 +2654,36 @@
     </row>
     <row r="14" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A14" s="20" t="s">
-        <v>7</v>
-      </c>
-      <c r="B14" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="B14" s="3" t="s">
         <v>36</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="D14" s="24"/>
+        <v>110</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>121</v>
+      </c>
       <c r="E14" s="1"/>
-      <c r="F14" s="31">
+      <c r="F14" s="30">
         <v>13</v>
       </c>
-      <c r="G14" s="8" t="s">
-        <v>80</v>
-      </c>
-      <c r="H14" s="7"/>
-      <c r="I14" s="12" t="s">
+      <c r="G14" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="H14" s="6"/>
+      <c r="I14" s="11" t="s">
         <v>8</v>
       </c>
       <c r="J14" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="K14" s="6"/>
-      <c r="L14" s="4">
-        <v>13</v>
-      </c>
-      <c r="M14" s="35" t="s">
-        <v>92</v>
-      </c>
-      <c r="N14" s="6"/>
-      <c r="O14" s="10" t="str">
-        <f xml:space="preserve"> "&lt; &lt;expr_id&gt;"</f>
-        <v>&lt; &lt;expr_id&gt;</v>
-      </c>
+      <c r="K14" s="5"/>
+      <c r="L14" s="5"/>
+      <c r="M14" s="7"/>
+      <c r="N14" s="5"/>
+      <c r="O14" s="10"/>
       <c r="P14" s="1"/>
       <c r="Q14" s="1"/>
       <c r="R14" s="1"/>
@@ -2526,41 +2700,36 @@
     </row>
     <row r="15" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A15" s="20" t="s">
-        <v>8</v>
-      </c>
-      <c r="B15" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="B15" s="3" t="s">
         <v>36</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="D15" s="4"/>
+        <v>106</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>100</v>
+      </c>
       <c r="E15" s="1"/>
-      <c r="F15" s="31">
+      <c r="F15" s="30">
         <v>14</v>
       </c>
-      <c r="G15" s="8" t="s">
-        <v>80</v>
-      </c>
-      <c r="H15" s="7"/>
-      <c r="I15" s="14" t="s">
+      <c r="G15" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="H15" s="6"/>
+      <c r="I15" s="13" t="s">
         <v>9</v>
       </c>
       <c r="J15" s="4" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="K15" s="1"/>
-      <c r="L15" s="4">
-        <v>14</v>
-      </c>
-      <c r="M15" s="35" t="s">
-        <v>92</v>
-      </c>
-      <c r="N15" s="6"/>
-      <c r="O15" s="10" t="str">
-        <f xml:space="preserve"> "&gt; &lt;expr_id&gt;"</f>
-        <v>&gt; &lt;expr_id&gt;</v>
-      </c>
+      <c r="L15" s="5"/>
+      <c r="M15" s="7"/>
+      <c r="N15" s="5"/>
+      <c r="O15" s="10"/>
       <c r="P15" s="1"/>
       <c r="Q15" s="1"/>
       <c r="R15" s="1"/>
@@ -2576,43 +2745,37 @@
       <c r="AB15" s="1"/>
     </row>
     <row r="16" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A16" s="20" t="s">
-        <v>9</v>
-      </c>
-      <c r="B16" s="4" t="s">
+      <c r="A16" s="19" t="s">
+        <v>124</v>
+      </c>
+      <c r="B16" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="C16" s="4" t="str">
-        <f>"{"&amp;A16&amp;"}"</f>
-        <v>{integer}</v>
-      </c>
-      <c r="D16" s="13"/>
+      <c r="C16" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>100</v>
+      </c>
       <c r="E16" s="1"/>
-      <c r="F16" s="31">
+      <c r="F16" s="30">
         <v>15</v>
       </c>
-      <c r="G16" s="8" t="s">
-        <v>80</v>
-      </c>
-      <c r="H16" s="7"/>
-      <c r="I16" s="12" t="s">
+      <c r="G16" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="H16" s="6"/>
+      <c r="I16" s="11" t="s">
         <v>11</v>
       </c>
       <c r="J16" s="4" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="K16" s="1"/>
-      <c r="L16" s="4">
-        <v>15</v>
-      </c>
-      <c r="M16" s="35" t="s">
-        <v>92</v>
-      </c>
-      <c r="N16" s="6"/>
-      <c r="O16" s="10" t="str">
-        <f xml:space="preserve"> "&lt;= &lt;expr_id&gt;"</f>
-        <v>&lt;= &lt;expr_id&gt;</v>
-      </c>
+      <c r="L16" s="5"/>
+      <c r="M16" s="7"/>
+      <c r="N16" s="5"/>
+      <c r="O16" s="10"/>
       <c r="P16" s="1"/>
       <c r="Q16" s="1"/>
       <c r="R16" s="1"/>
@@ -2628,43 +2791,37 @@
       <c r="AB16" s="1"/>
     </row>
     <row r="17" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A17" s="20" t="s">
+      <c r="A17" s="21" t="s">
+        <v>128</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="E17" s="1"/>
+      <c r="F17" s="30">
+        <v>16</v>
+      </c>
+      <c r="G17" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="H17" s="6"/>
+      <c r="I17" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="B17" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="C17" s="4" t="str">
-        <f t="shared" ref="C17:C42" si="0">"{"&amp;A17&amp;"}"</f>
-        <v>{string}</v>
-      </c>
-      <c r="D17" s="4"/>
-      <c r="E17" s="1"/>
-      <c r="F17" s="31">
-        <v>16</v>
-      </c>
-      <c r="G17" s="8" t="s">
-        <v>80</v>
-      </c>
-      <c r="H17" s="7"/>
-      <c r="I17" s="10" t="s">
-        <v>10</v>
-      </c>
       <c r="J17" s="4" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="K17" s="1"/>
-      <c r="L17" s="4">
-        <v>16</v>
-      </c>
-      <c r="M17" s="35" t="s">
-        <v>92</v>
-      </c>
-      <c r="N17" s="6"/>
-      <c r="O17" s="10" t="str">
-        <f xml:space="preserve"> "&gt;= &lt;expr_id&gt;"</f>
-        <v>&gt;= &lt;expr_id&gt;</v>
-      </c>
+      <c r="L17" s="5"/>
+      <c r="M17" s="7"/>
+      <c r="N17" s="5"/>
+      <c r="O17" s="10"/>
       <c r="P17" s="1"/>
       <c r="Q17" s="1"/>
       <c r="R17" s="1"/>
@@ -2680,42 +2837,35 @@
       <c r="AB17" s="1"/>
     </row>
     <row r="18" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A18" s="20" t="s">
-        <v>11</v>
+      <c r="A18" s="19" t="s">
+        <v>7</v>
       </c>
       <c r="B18" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="C18" s="4" t="str">
-        <f t="shared" si="0"/>
-        <v>{float}</v>
+      <c r="C18" s="4" t="s">
+        <v>39</v>
       </c>
       <c r="D18" s="4"/>
       <c r="E18" s="1"/>
-      <c r="F18" s="31">
+      <c r="F18" s="30">
         <v>17</v>
       </c>
-      <c r="G18" s="8" t="s">
+      <c r="G18" s="7" t="s">
         <v>70</v>
       </c>
-      <c r="H18" s="8"/>
-      <c r="I18" s="10" t="s">
+      <c r="H18" s="7"/>
+      <c r="I18" s="9" t="s">
         <v>72</v>
       </c>
       <c r="J18" s="4" t="s">
         <v>47</v>
       </c>
       <c r="K18" s="1"/>
-      <c r="L18" s="2">
-        <v>17</v>
-      </c>
-      <c r="M18" s="40" t="s">
-        <v>92</v>
-      </c>
-      <c r="N18" s="18"/>
-      <c r="O18" s="41" t="s">
-        <v>51</v>
-      </c>
+      <c r="L18" s="5"/>
+      <c r="M18" s="7"/>
+      <c r="N18" s="5"/>
+      <c r="O18" s="6"/>
       <c r="P18" s="1"/>
       <c r="Q18" s="1"/>
       <c r="R18" s="1"/>
@@ -2731,36 +2881,35 @@
       <c r="AB18" s="1"/>
     </row>
     <row r="19" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A19" s="20" t="s">
-        <v>14</v>
+      <c r="A19" s="19" t="s">
+        <v>8</v>
       </c>
       <c r="B19" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="C19" s="4" t="str">
-        <f t="shared" si="0"/>
-        <v>{not}</v>
+      <c r="C19" s="4" t="s">
+        <v>40</v>
       </c>
       <c r="D19" s="4"/>
       <c r="E19" s="1"/>
-      <c r="F19" s="31">
+      <c r="F19" s="30">
         <v>18</v>
       </c>
-      <c r="G19" s="8" t="s">
+      <c r="G19" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="H19" s="8"/>
-      <c r="I19" s="14" t="s">
+      <c r="H19" s="7"/>
+      <c r="I19" s="13" t="s">
         <v>51</v>
       </c>
       <c r="J19" s="4" t="s">
-        <v>102</v>
-      </c>
-      <c r="K19" s="39"/>
-      <c r="L19" s="6"/>
-      <c r="M19" s="8"/>
-      <c r="N19" s="6"/>
-      <c r="O19" s="6"/>
+        <v>99</v>
+      </c>
+      <c r="K19" s="36"/>
+      <c r="L19" s="5"/>
+      <c r="M19" s="7"/>
+      <c r="N19" s="5"/>
+      <c r="O19" s="5"/>
       <c r="P19" s="1"/>
       <c r="Q19" s="1"/>
       <c r="R19" s="1"/>
@@ -2776,36 +2925,36 @@
       <c r="AB19" s="1"/>
     </row>
     <row r="20" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A20" s="20" t="s">
-        <v>13</v>
+      <c r="A20" s="19" t="s">
+        <v>9</v>
       </c>
       <c r="B20" s="4" t="s">
         <v>36</v>
       </c>
       <c r="C20" s="4" t="str">
-        <f t="shared" si="0"/>
-        <v>{EOF}</v>
-      </c>
-      <c r="D20" s="4"/>
+        <f>"{"&amp;A20&amp;"}"</f>
+        <v>{integer}</v>
+      </c>
+      <c r="D20" s="12"/>
       <c r="E20" s="1"/>
-      <c r="F20" s="31">
+      <c r="F20" s="30">
         <v>19</v>
       </c>
-      <c r="G20" s="8" t="s">
+      <c r="G20" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="H20" s="7"/>
-      <c r="I20" s="12" t="s">
+      <c r="H20" s="6"/>
+      <c r="I20" s="11" t="s">
         <v>69</v>
       </c>
       <c r="J20" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="K20" s="39"/>
-      <c r="L20" s="6"/>
-      <c r="M20" s="8"/>
-      <c r="N20" s="6"/>
-      <c r="O20" s="6"/>
+      <c r="K20" s="36"/>
+      <c r="L20" s="5"/>
+      <c r="M20" s="7"/>
+      <c r="N20" s="5"/>
+      <c r="O20" s="5"/>
       <c r="P20" s="1"/>
       <c r="Q20" s="1"/>
       <c r="R20" s="1"/>
@@ -2821,36 +2970,36 @@
       <c r="AB20" s="1"/>
     </row>
     <row r="21" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A21" s="20" t="s">
-        <v>12</v>
+      <c r="A21" s="19" t="s">
+        <v>10</v>
       </c>
       <c r="B21" s="4" t="s">
         <v>36</v>
       </c>
       <c r="C21" s="4" t="str">
-        <f t="shared" si="0"/>
-        <v>{EOL}</v>
+        <f t="shared" ref="C21:C46" si="0">"{"&amp;A21&amp;"}"</f>
+        <v>{string}</v>
       </c>
       <c r="D21" s="4"/>
       <c r="E21" s="1"/>
-      <c r="F21" s="31">
+      <c r="F21" s="30">
         <v>20</v>
       </c>
-      <c r="G21" s="8" t="s">
+      <c r="G21" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="H21" s="8"/>
-      <c r="I21" s="10" t="s">
-        <v>83</v>
+      <c r="H21" s="7"/>
+      <c r="I21" s="9" t="s">
+        <v>82</v>
       </c>
       <c r="J21" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="K21" s="39"/>
-      <c r="L21" s="6"/>
-      <c r="M21" s="8"/>
-      <c r="N21" s="6"/>
-      <c r="O21" s="6"/>
+      <c r="K21" s="36"/>
+      <c r="L21" s="5"/>
+      <c r="M21" s="7"/>
+      <c r="N21" s="5"/>
+      <c r="O21" s="5"/>
       <c r="P21" s="1"/>
       <c r="Q21" s="1"/>
       <c r="R21" s="1"/>
@@ -2866,36 +3015,36 @@
       <c r="AB21" s="1"/>
     </row>
     <row r="22" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A22" s="20" t="s">
-        <v>15</v>
+      <c r="A22" s="19" t="s">
+        <v>11</v>
       </c>
       <c r="B22" s="4" t="s">
         <v>36</v>
       </c>
       <c r="C22" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>{+}</v>
+        <v>{float}</v>
       </c>
       <c r="D22" s="4"/>
       <c r="E22" s="1"/>
-      <c r="F22" s="31">
+      <c r="F22" s="30">
         <v>21</v>
       </c>
-      <c r="G22" s="8" t="s">
+      <c r="G22" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="H22" s="8"/>
-      <c r="I22" s="10" t="s">
+      <c r="H22" s="7"/>
+      <c r="I22" s="9" t="s">
         <v>64</v>
       </c>
       <c r="J22" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="K22" s="39"/>
-      <c r="L22" s="6"/>
-      <c r="M22" s="8"/>
-      <c r="N22" s="6"/>
-      <c r="O22" s="6"/>
+      <c r="K22" s="36"/>
+      <c r="L22" s="5"/>
+      <c r="M22" s="7"/>
+      <c r="N22" s="5"/>
+      <c r="O22" s="5"/>
       <c r="P22" s="1"/>
       <c r="Q22" s="1"/>
       <c r="R22" s="1"/>
@@ -2911,36 +3060,36 @@
       <c r="AB22" s="1"/>
     </row>
     <row r="23" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A23" s="20" t="s">
-        <v>16</v>
+      <c r="A23" s="19" t="s">
+        <v>14</v>
       </c>
       <c r="B23" s="4" t="s">
         <v>36</v>
       </c>
       <c r="C23" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>{-}</v>
+        <v>{not}</v>
       </c>
       <c r="D23" s="4"/>
       <c r="E23" s="1"/>
-      <c r="F23" s="31">
+      <c r="F23" s="30">
         <v>22</v>
       </c>
-      <c r="G23" s="8" t="s">
+      <c r="G23" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="H23" s="8"/>
-      <c r="I23" s="10" t="s">
+      <c r="H23" s="7"/>
+      <c r="I23" s="9" t="s">
         <v>3</v>
       </c>
       <c r="J23" s="4" t="s">
-        <v>87</v>
-      </c>
-      <c r="K23" s="39"/>
-      <c r="L23" s="6"/>
-      <c r="M23" s="8"/>
-      <c r="N23" s="6"/>
-      <c r="O23" s="6"/>
+        <v>86</v>
+      </c>
+      <c r="K23" s="36"/>
+      <c r="L23" s="5"/>
+      <c r="M23" s="7"/>
+      <c r="N23" s="5"/>
+      <c r="O23" s="5"/>
       <c r="P23" s="1"/>
       <c r="Q23" s="1"/>
       <c r="R23" s="1"/>
@@ -2956,36 +3105,36 @@
       <c r="AB23" s="1"/>
     </row>
     <row r="24" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A24" s="20" t="s">
-        <v>17</v>
+      <c r="A24" s="19" t="s">
+        <v>13</v>
       </c>
       <c r="B24" s="4" t="s">
         <v>36</v>
       </c>
       <c r="C24" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>{*}</v>
+        <v>{EOF}</v>
       </c>
       <c r="D24" s="4"/>
       <c r="E24" s="1"/>
-      <c r="F24" s="31">
+      <c r="F24" s="30">
         <v>23</v>
       </c>
-      <c r="G24" s="8" t="s">
+      <c r="G24" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="H24" s="8"/>
-      <c r="I24" s="10" t="s">
+      <c r="H24" s="7"/>
+      <c r="I24" s="9" t="s">
         <v>51</v>
       </c>
       <c r="J24" s="4" t="s">
-        <v>104</v>
-      </c>
-      <c r="K24" s="39"/>
-      <c r="L24" s="6"/>
-      <c r="M24" s="8"/>
-      <c r="N24" s="6"/>
-      <c r="O24" s="6"/>
+        <v>101</v>
+      </c>
+      <c r="K24" s="36"/>
+      <c r="L24" s="5"/>
+      <c r="M24" s="7"/>
+      <c r="N24" s="5"/>
+      <c r="O24" s="5"/>
       <c r="P24" s="1"/>
       <c r="Q24" s="1"/>
       <c r="R24" s="1"/>
@@ -3001,36 +3150,36 @@
       <c r="AB24" s="1"/>
     </row>
     <row r="25" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A25" s="20" t="s">
-        <v>18</v>
+      <c r="A25" s="19" t="s">
+        <v>12</v>
       </c>
       <c r="B25" s="4" t="s">
         <v>36</v>
       </c>
       <c r="C25" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>{/}</v>
+        <v>{EOL}</v>
       </c>
       <c r="D25" s="4"/>
       <c r="E25" s="1"/>
-      <c r="F25" s="31">
+      <c r="F25" s="30">
         <v>24</v>
       </c>
-      <c r="G25" s="8" t="s">
+      <c r="G25" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="H25" s="8"/>
-      <c r="I25" s="10" t="s">
-        <v>84</v>
+      <c r="H25" s="7"/>
+      <c r="I25" s="9" t="s">
+        <v>83</v>
       </c>
       <c r="J25" s="4" t="s">
-        <v>89</v>
-      </c>
-      <c r="K25" s="39"/>
-      <c r="L25" s="6"/>
-      <c r="M25" s="8"/>
-      <c r="N25" s="6"/>
-      <c r="O25" s="6"/>
+        <v>88</v>
+      </c>
+      <c r="K25" s="36"/>
+      <c r="L25" s="5"/>
+      <c r="M25" s="7"/>
+      <c r="N25" s="5"/>
+      <c r="O25" s="5"/>
       <c r="P25" s="1"/>
       <c r="Q25" s="1"/>
       <c r="R25" s="1"/>
@@ -3046,36 +3195,36 @@
       <c r="AB25" s="1"/>
     </row>
     <row r="26" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A26" s="27" t="s">
-        <v>19</v>
+      <c r="A26" s="19" t="s">
+        <v>15</v>
       </c>
       <c r="B26" s="4" t="s">
         <v>36</v>
       </c>
       <c r="C26" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>{==}</v>
+        <v>{+}</v>
       </c>
       <c r="D26" s="4"/>
       <c r="E26" s="1"/>
-      <c r="F26" s="31">
+      <c r="F26" s="30">
         <v>25</v>
       </c>
-      <c r="G26" s="8" t="s">
+      <c r="G26" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="H26" s="8"/>
-      <c r="I26" s="10" t="s">
+      <c r="H26" s="7"/>
+      <c r="I26" s="9" t="s">
         <v>57</v>
       </c>
       <c r="J26" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="K26" s="39"/>
-      <c r="L26" s="6"/>
-      <c r="M26" s="8"/>
-      <c r="N26" s="6"/>
-      <c r="O26" s="6"/>
+      <c r="K26" s="36"/>
+      <c r="L26" s="5"/>
+      <c r="M26" s="7"/>
+      <c r="N26" s="5"/>
+      <c r="O26" s="5"/>
       <c r="P26" s="1"/>
       <c r="Q26" s="1"/>
       <c r="R26" s="1"/>
@@ -3091,36 +3240,36 @@
       <c r="AB26" s="1"/>
     </row>
     <row r="27" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A27" s="20" t="s">
-        <v>20</v>
+      <c r="A27" s="19" t="s">
+        <v>16</v>
       </c>
       <c r="B27" s="4" t="s">
         <v>36</v>
       </c>
       <c r="C27" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>{!=}</v>
+        <v>{-}</v>
       </c>
       <c r="D27" s="4"/>
       <c r="E27" s="1"/>
-      <c r="F27" s="31">
+      <c r="F27" s="30">
         <v>26</v>
       </c>
-      <c r="G27" s="8" t="s">
+      <c r="G27" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="H27" s="8"/>
-      <c r="I27" s="10" t="s">
+      <c r="H27" s="7"/>
+      <c r="I27" s="9" t="s">
         <v>51</v>
       </c>
       <c r="J27" s="4" t="s">
-        <v>104</v>
-      </c>
-      <c r="K27" s="39"/>
-      <c r="L27" s="6"/>
-      <c r="M27" s="8"/>
-      <c r="N27" s="6"/>
-      <c r="O27" s="6"/>
+        <v>101</v>
+      </c>
+      <c r="K27" s="36"/>
+      <c r="L27" s="5"/>
+      <c r="M27" s="7"/>
+      <c r="N27" s="5"/>
+      <c r="O27" s="5"/>
       <c r="P27" s="1"/>
       <c r="Q27" s="1"/>
       <c r="R27" s="1"/>
@@ -3136,36 +3285,36 @@
       <c r="AB27" s="1"/>
     </row>
     <row r="28" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A28" s="20" t="s">
-        <v>21</v>
+      <c r="A28" s="19" t="s">
+        <v>17</v>
       </c>
       <c r="B28" s="4" t="s">
         <v>36</v>
       </c>
       <c r="C28" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>{&lt;}</v>
+        <v>{*}</v>
       </c>
       <c r="D28" s="4"/>
       <c r="E28" s="1"/>
-      <c r="F28" s="31">
+      <c r="F28" s="30">
         <v>27</v>
       </c>
-      <c r="G28" s="8" t="s">
+      <c r="G28" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="H28" s="8"/>
-      <c r="I28" s="10" t="s">
+      <c r="H28" s="7"/>
+      <c r="I28" s="9" t="s">
         <v>58</v>
       </c>
       <c r="J28" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="K28" s="39"/>
-      <c r="L28" s="6"/>
-      <c r="M28" s="8"/>
-      <c r="N28" s="6"/>
-      <c r="O28" s="6"/>
+      <c r="K28" s="36"/>
+      <c r="L28" s="5"/>
+      <c r="M28" s="7"/>
+      <c r="N28" s="5"/>
+      <c r="O28" s="5"/>
       <c r="P28" s="1"/>
       <c r="Q28" s="1"/>
       <c r="R28" s="1"/>
@@ -3181,36 +3330,36 @@
       <c r="AB28" s="1"/>
     </row>
     <row r="29" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A29" s="20" t="s">
-        <v>22</v>
+      <c r="A29" s="19" t="s">
+        <v>18</v>
       </c>
       <c r="B29" s="4" t="s">
         <v>36</v>
       </c>
       <c r="C29" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>{&gt;}</v>
+        <v>{/}</v>
       </c>
       <c r="D29" s="4"/>
       <c r="E29" s="1"/>
-      <c r="F29" s="31">
+      <c r="F29" s="30">
         <v>28</v>
       </c>
-      <c r="G29" s="35" t="s">
+      <c r="G29" s="34" t="s">
         <v>55</v>
       </c>
-      <c r="H29" s="8"/>
-      <c r="I29" s="10" t="s">
+      <c r="H29" s="7"/>
+      <c r="I29" s="9" t="s">
         <v>59</v>
       </c>
       <c r="J29" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="K29" s="39"/>
-      <c r="L29" s="6"/>
-      <c r="M29" s="8"/>
-      <c r="N29" s="6"/>
-      <c r="O29" s="6"/>
+      <c r="K29" s="36"/>
+      <c r="L29" s="5"/>
+      <c r="M29" s="7"/>
+      <c r="N29" s="5"/>
+      <c r="O29" s="5"/>
       <c r="P29" s="1"/>
       <c r="Q29" s="1"/>
       <c r="R29" s="1"/>
@@ -3226,36 +3375,36 @@
       <c r="AB29" s="1"/>
     </row>
     <row r="30" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A30" s="20" t="s">
-        <v>23</v>
+      <c r="A30" s="26" t="s">
+        <v>19</v>
       </c>
       <c r="B30" s="4" t="s">
         <v>36</v>
       </c>
       <c r="C30" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>{&lt;=}</v>
+        <v>{==}</v>
       </c>
       <c r="D30" s="4"/>
       <c r="E30" s="1"/>
-      <c r="F30" s="33">
+      <c r="F30" s="30">
         <v>29</v>
       </c>
-      <c r="G30" s="36" t="s">
+      <c r="G30" s="46" t="s">
         <v>56</v>
       </c>
-      <c r="H30" s="37"/>
-      <c r="I30" s="38" t="s">
+      <c r="H30" s="6"/>
+      <c r="I30" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="J30" s="2" t="s">
+      <c r="J30" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="K30" s="39"/>
-      <c r="L30" s="6"/>
-      <c r="M30" s="8"/>
-      <c r="N30" s="6"/>
-      <c r="O30" s="6"/>
+      <c r="K30" s="36"/>
+      <c r="L30" s="5"/>
+      <c r="M30" s="7"/>
+      <c r="N30" s="5"/>
+      <c r="O30" s="5"/>
       <c r="P30" s="1"/>
       <c r="Q30" s="1"/>
       <c r="R30" s="1"/>
@@ -3271,23 +3420,35 @@
       <c r="AB30" s="1"/>
     </row>
     <row r="31" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A31" s="20" t="s">
-        <v>24</v>
+      <c r="A31" s="19" t="s">
+        <v>20</v>
       </c>
       <c r="B31" s="4" t="s">
         <v>36</v>
       </c>
       <c r="C31" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>{&gt;=}</v>
+        <v>{!=}</v>
       </c>
       <c r="D31" s="4"/>
       <c r="E31" s="1"/>
+      <c r="F31" s="30">
+        <v>30</v>
+      </c>
+      <c r="G31" s="34" t="s">
+        <v>90</v>
+      </c>
+      <c r="I31" s="9" t="s">
+        <v>94</v>
+      </c>
+      <c r="J31" s="4" t="s">
+        <v>39</v>
+      </c>
       <c r="K31" s="1"/>
       <c r="L31" s="1"/>
       <c r="M31" s="1"/>
       <c r="N31" s="1"/>
-      <c r="O31" s="6"/>
+      <c r="O31" s="5"/>
       <c r="P31" s="1"/>
       <c r="Q31" s="1"/>
       <c r="R31" s="1"/>
@@ -3303,18 +3464,30 @@
       <c r="AB31" s="1"/>
     </row>
     <row r="32" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A32" s="20" t="s">
-        <v>25</v>
+      <c r="A32" s="19" t="s">
+        <v>21</v>
       </c>
       <c r="B32" s="4" t="s">
         <v>36</v>
       </c>
       <c r="C32" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>{(}</v>
+        <v>{&lt;}</v>
       </c>
       <c r="D32" s="4"/>
       <c r="E32" s="1"/>
+      <c r="F32" s="30">
+        <v>31</v>
+      </c>
+      <c r="G32" s="34" t="s">
+        <v>90</v>
+      </c>
+      <c r="I32" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="J32" s="4" t="s">
+        <v>105</v>
+      </c>
       <c r="K32" s="1"/>
       <c r="L32" s="1"/>
       <c r="M32" s="1"/>
@@ -3335,18 +3508,31 @@
       <c r="AB32" s="1"/>
     </row>
     <row r="33" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A33" s="20" t="s">
-        <v>26</v>
+      <c r="A33" s="19" t="s">
+        <v>22</v>
       </c>
       <c r="B33" s="4" t="s">
         <v>36</v>
       </c>
       <c r="C33" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>{)}</v>
+        <v>{&gt;}</v>
       </c>
       <c r="D33" s="4"/>
       <c r="E33" s="1"/>
+      <c r="F33" s="30">
+        <v>32</v>
+      </c>
+      <c r="G33" s="34" t="s">
+        <v>91</v>
+      </c>
+      <c r="I33" s="9" t="str">
+        <f xml:space="preserve"> "+ &lt;expr_id&gt;"</f>
+        <v>+ &lt;expr_id&gt;</v>
+      </c>
+      <c r="J33" s="4" t="s">
+        <v>111</v>
+      </c>
       <c r="K33" s="1"/>
       <c r="L33" s="1"/>
       <c r="M33" s="1"/>
@@ -3367,18 +3553,31 @@
       <c r="AB33" s="1"/>
     </row>
     <row r="34" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A34" s="20" t="s">
-        <v>29</v>
+      <c r="A34" s="19" t="s">
+        <v>23</v>
       </c>
       <c r="B34" s="4" t="s">
         <v>36</v>
       </c>
       <c r="C34" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>{=}</v>
+        <v>{&lt;=}</v>
       </c>
       <c r="D34" s="4"/>
       <c r="E34" s="1"/>
+      <c r="F34" s="30">
+        <v>33</v>
+      </c>
+      <c r="G34" s="34" t="s">
+        <v>91</v>
+      </c>
+      <c r="I34" s="9" t="str">
+        <f xml:space="preserve"> "- &lt;expr_id&gt;"</f>
+        <v>- &lt;expr_id&gt;</v>
+      </c>
+      <c r="J34" s="4" t="s">
+        <v>112</v>
+      </c>
       <c r="K34" s="1"/>
       <c r="L34" s="1"/>
       <c r="M34" s="1"/>
@@ -3399,18 +3598,31 @@
       <c r="AB34" s="1"/>
     </row>
     <row r="35" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A35" s="20" t="s">
-        <v>30</v>
+      <c r="A35" s="19" t="s">
+        <v>24</v>
       </c>
       <c r="B35" s="4" t="s">
         <v>36</v>
       </c>
       <c r="C35" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>{,}</v>
+        <v>{&gt;=}</v>
       </c>
       <c r="D35" s="4"/>
       <c r="E35" s="1"/>
+      <c r="F35" s="30">
+        <v>34</v>
+      </c>
+      <c r="G35" s="34" t="s">
+        <v>91</v>
+      </c>
+      <c r="I35" s="9" t="str">
+        <f xml:space="preserve"> "/ &lt;expr_id&gt;"</f>
+        <v>/ &lt;expr_id&gt;</v>
+      </c>
+      <c r="J35" s="4" t="s">
+        <v>113</v>
+      </c>
       <c r="K35" s="1"/>
       <c r="L35" s="1"/>
       <c r="M35" s="1"/>
@@ -3431,18 +3643,31 @@
       <c r="AB35" s="1"/>
     </row>
     <row r="36" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A36" s="20" t="s">
-        <v>27</v>
+      <c r="A36" s="19" t="s">
+        <v>25</v>
       </c>
       <c r="B36" s="4" t="s">
         <v>36</v>
       </c>
       <c r="C36" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>{def}</v>
+        <v>{(}</v>
       </c>
       <c r="D36" s="4"/>
       <c r="E36" s="1"/>
+      <c r="F36" s="30">
+        <v>35</v>
+      </c>
+      <c r="G36" s="34" t="s">
+        <v>91</v>
+      </c>
+      <c r="I36" s="9" t="str">
+        <f xml:space="preserve"> "* &lt;expr_id&gt;"</f>
+        <v>* &lt;expr_id&gt;</v>
+      </c>
+      <c r="J36" s="4" t="s">
+        <v>114</v>
+      </c>
       <c r="K36" s="1"/>
       <c r="L36" s="1"/>
       <c r="M36" s="1"/>
@@ -3463,18 +3688,31 @@
       <c r="AB36" s="1"/>
     </row>
     <row r="37" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A37" s="20" t="s">
-        <v>28</v>
+      <c r="A37" s="19" t="s">
+        <v>26</v>
       </c>
       <c r="B37" s="4" t="s">
         <v>36</v>
       </c>
       <c r="C37" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>{end}</v>
+        <v>{)}</v>
       </c>
       <c r="D37" s="4"/>
       <c r="E37" s="1"/>
+      <c r="F37" s="30">
+        <v>36</v>
+      </c>
+      <c r="G37" s="34" t="s">
+        <v>91</v>
+      </c>
+      <c r="I37" s="9" t="str">
+        <f xml:space="preserve"> "== &lt;expr_id&gt;"</f>
+        <v>== &lt;expr_id&gt;</v>
+      </c>
+      <c r="J37" s="4" t="s">
+        <v>115</v>
+      </c>
       <c r="K37" s="1"/>
       <c r="L37" s="1"/>
       <c r="M37" s="1"/>
@@ -3495,18 +3733,31 @@
       <c r="AB37" s="1"/>
     </row>
     <row r="38" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A38" s="20" t="s">
-        <v>32</v>
+      <c r="A38" s="19" t="s">
+        <v>29</v>
       </c>
       <c r="B38" s="4" t="s">
         <v>36</v>
       </c>
       <c r="C38" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>{if}</v>
+        <v>{=}</v>
       </c>
       <c r="D38" s="4"/>
       <c r="E38" s="1"/>
+      <c r="F38" s="30">
+        <v>37</v>
+      </c>
+      <c r="G38" s="34" t="s">
+        <v>91</v>
+      </c>
+      <c r="I38" s="9" t="str">
+        <f xml:space="preserve"> "!= &lt;expr_id&gt;"</f>
+        <v>!= &lt;expr_id&gt;</v>
+      </c>
+      <c r="J38" s="4" t="s">
+        <v>116</v>
+      </c>
       <c r="K38" s="1"/>
       <c r="L38" s="1"/>
       <c r="M38" s="1"/>
@@ -3527,23 +3778,32 @@
       <c r="AB38" s="1"/>
     </row>
     <row r="39" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A39" s="21" t="s">
-        <v>31</v>
+      <c r="A39" s="19" t="s">
+        <v>30</v>
       </c>
       <c r="B39" s="4" t="s">
         <v>36</v>
       </c>
       <c r="C39" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>{then}</v>
+        <v>{,}</v>
       </c>
       <c r="D39" s="4"/>
       <c r="E39" s="1"/>
-      <c r="F39" s="1"/>
-      <c r="G39" s="9"/>
-      <c r="H39" s="9"/>
-      <c r="I39" s="11"/>
-      <c r="J39" s="6"/>
+      <c r="F39" s="30">
+        <v>38</v>
+      </c>
+      <c r="G39" s="34" t="s">
+        <v>91</v>
+      </c>
+      <c r="H39" s="8"/>
+      <c r="I39" s="9" t="str">
+        <f xml:space="preserve"> "&lt; &lt;expr_id&gt;"</f>
+        <v>&lt; &lt;expr_id&gt;</v>
+      </c>
+      <c r="J39" s="4" t="s">
+        <v>117</v>
+      </c>
       <c r="K39" s="1"/>
       <c r="L39" s="1"/>
       <c r="M39" s="1"/>
@@ -3564,23 +3824,32 @@
       <c r="AB39" s="1"/>
     </row>
     <row r="40" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A40" s="21" t="s">
-        <v>33</v>
+      <c r="A40" s="19" t="s">
+        <v>27</v>
       </c>
       <c r="B40" s="4" t="s">
         <v>36</v>
       </c>
       <c r="C40" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>{else}</v>
+        <v>{def}</v>
       </c>
       <c r="D40" s="4"/>
       <c r="E40" s="1"/>
-      <c r="F40" s="1"/>
-      <c r="G40" s="9"/>
-      <c r="H40" s="9"/>
-      <c r="I40" s="11"/>
-      <c r="J40" s="6"/>
+      <c r="F40" s="30">
+        <v>39</v>
+      </c>
+      <c r="G40" s="34" t="s">
+        <v>91</v>
+      </c>
+      <c r="H40" s="8"/>
+      <c r="I40" s="9" t="str">
+        <f xml:space="preserve"> "&gt; &lt;expr_id&gt;"</f>
+        <v>&gt; &lt;expr_id&gt;</v>
+      </c>
+      <c r="J40" s="4" t="s">
+        <v>118</v>
+      </c>
       <c r="K40" s="1"/>
       <c r="L40" s="1"/>
       <c r="M40" s="1"/>
@@ -3601,23 +3870,32 @@
       <c r="AB40" s="1"/>
     </row>
     <row r="41" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A41" s="21" t="s">
-        <v>34</v>
+      <c r="A41" s="19" t="s">
+        <v>28</v>
       </c>
       <c r="B41" s="4" t="s">
         <v>36</v>
       </c>
       <c r="C41" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>{while}</v>
+        <v>{end}</v>
       </c>
       <c r="D41" s="4"/>
       <c r="E41" s="1"/>
-      <c r="F41" s="1"/>
-      <c r="G41" s="9"/>
-      <c r="H41" s="9"/>
-      <c r="I41" s="11"/>
-      <c r="J41" s="6"/>
+      <c r="F41" s="30">
+        <v>40</v>
+      </c>
+      <c r="G41" s="34" t="s">
+        <v>91</v>
+      </c>
+      <c r="H41" s="8"/>
+      <c r="I41" s="9" t="str">
+        <f xml:space="preserve"> "&lt;= &lt;expr_id&gt;"</f>
+        <v>&lt;= &lt;expr_id&gt;</v>
+      </c>
+      <c r="J41" s="4" t="s">
+        <v>119</v>
+      </c>
       <c r="K41" s="1"/>
       <c r="L41" s="1"/>
       <c r="M41" s="1"/>
@@ -3638,23 +3916,32 @@
       <c r="AB41" s="1"/>
     </row>
     <row r="42" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A42" s="28" t="s">
-        <v>35</v>
-      </c>
-      <c r="B42" s="2" t="s">
+      <c r="A42" s="19" t="s">
+        <v>32</v>
+      </c>
+      <c r="B42" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="C42" s="2" t="str">
+      <c r="C42" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>{do}</v>
-      </c>
-      <c r="D42" s="2"/>
-      <c r="E42" s="6"/>
-      <c r="F42" s="1"/>
-      <c r="G42" s="9"/>
-      <c r="H42" s="9"/>
-      <c r="I42" s="11"/>
-      <c r="J42" s="6"/>
+        <v>{if}</v>
+      </c>
+      <c r="D42" s="4"/>
+      <c r="E42" s="5"/>
+      <c r="F42" s="30">
+        <v>41</v>
+      </c>
+      <c r="G42" s="34" t="s">
+        <v>91</v>
+      </c>
+      <c r="H42" s="8"/>
+      <c r="I42" s="9" t="str">
+        <f xml:space="preserve"> "&gt;= &lt;expr_id&gt;"</f>
+        <v>&gt;= &lt;expr_id&gt;</v>
+      </c>
+      <c r="J42" s="4" t="s">
+        <v>120</v>
+      </c>
       <c r="K42" s="1"/>
       <c r="L42" s="1"/>
       <c r="M42" s="1"/>
@@ -3674,6 +3961,128 @@
       <c r="AA42" s="1"/>
       <c r="AB42" s="1"/>
     </row>
+    <row r="43" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A43" s="20" t="s">
+        <v>31</v>
+      </c>
+      <c r="B43" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C43" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>{then}</v>
+      </c>
+      <c r="D43" s="4"/>
+      <c r="F43" s="30">
+        <v>42</v>
+      </c>
+      <c r="G43" s="34" t="s">
+        <v>91</v>
+      </c>
+      <c r="H43" s="6"/>
+      <c r="I43" s="13" t="s">
+        <v>51</v>
+      </c>
+      <c r="J43" s="4" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="44" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A44" s="20" t="s">
+        <v>33</v>
+      </c>
+      <c r="B44" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C44" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>{else}</v>
+      </c>
+      <c r="D44" s="4"/>
+      <c r="E44" s="13"/>
+      <c r="F44" s="30">
+        <v>43</v>
+      </c>
+      <c r="G44" s="25" t="s">
+        <v>125</v>
+      </c>
+      <c r="H44" s="6"/>
+      <c r="I44" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="J44" s="4" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="45" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A45" s="20" t="s">
+        <v>34</v>
+      </c>
+      <c r="B45" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C45" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>{while}</v>
+      </c>
+      <c r="D45" s="4"/>
+      <c r="E45" s="13"/>
+      <c r="F45" s="30">
+        <v>44</v>
+      </c>
+      <c r="G45" s="25" t="s">
+        <v>125</v>
+      </c>
+      <c r="H45" s="6"/>
+      <c r="I45" s="13" t="s">
+        <v>127</v>
+      </c>
+      <c r="J45" s="24" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="46" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A46" s="27" t="s">
+        <v>35</v>
+      </c>
+      <c r="B46" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C46" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>{do}</v>
+      </c>
+      <c r="D46" s="2"/>
+      <c r="E46" s="13"/>
+      <c r="F46" s="30">
+        <v>45</v>
+      </c>
+      <c r="G46" s="25" t="s">
+        <v>126</v>
+      </c>
+      <c r="I46" s="13" t="s">
+        <v>77</v>
+      </c>
+      <c r="J46" s="4" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="47" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="E47" s="13"/>
+      <c r="F47" s="32">
+        <v>46</v>
+      </c>
+      <c r="G47" s="56" t="s">
+        <v>126</v>
+      </c>
+      <c r="H47" s="35"/>
+      <c r="I47" s="38" t="s">
+        <v>2</v>
+      </c>
+      <c r="J47" s="2" t="s">
+        <v>87</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="G1:I1"/>
@@ -3681,8 +4090,5 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
-  <ignoredErrors>
-    <ignoredError sqref="O9" formula="1"/>
-  </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Opraveny EOLy, funkční syntaktický analyzátor
</commit_message>
<xml_diff>
--- a/doc/LL tabulka.xlsx
+++ b/doc/LL tabulka.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\OneDrive\VUT_FIT_BIT\IFJ\Projekt\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="160" documentId="6_{9A5E4322-B6A2-4F6C-9661-AD2FA57F2F31}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{892EF6EB-727E-4D2B-8D85-FEE95D778E8A}"/>
+  <xr:revisionPtr revIDLastSave="307" documentId="6_{9A5E4322-B6A2-4F6C-9661-AD2FA57F2F31}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{1D85FAF0-2B37-4308-8B28-C7F86AAA8935}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12165" activeTab="1" xr2:uid="{C362D381-7D2B-4872-B2C9-60D26B6B778F}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12165" xr2:uid="{C362D381-7D2B-4872-B2C9-60D26B6B778F}"/>
   </bookViews>
   <sheets>
     <sheet name="LL tabulka prediktivní analýzy" sheetId="2" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="311" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="295" uniqueCount="125">
   <si>
     <t>&lt;prog&gt;</t>
   </si>
@@ -240,30 +240,6 @@
     <t>&lt;expr&gt;</t>
   </si>
   <si>
-    <t>&lt;new_line&gt;</t>
-  </si>
-  <si>
-    <t>&lt;new_line&gt;   -&gt;</t>
-  </si>
-  <si>
-    <t>&lt;new_line_n&gt;   -&gt;</t>
-  </si>
-  <si>
-    <t>EOL &lt;new_line_n&gt;</t>
-  </si>
-  <si>
-    <t>&lt;new_line_n&gt;</t>
-  </si>
-  <si>
-    <t>&lt;expr&gt; &lt;new_line&gt; &lt;body&gt;</t>
-  </si>
-  <si>
-    <t>&lt;def_func&gt; &lt;new_line&gt; &lt;prog&gt;</t>
-  </si>
-  <si>
-    <t>id &lt;body_id&gt; &lt;new_line&gt; &lt;body&gt;</t>
-  </si>
-  <si>
     <t>&lt;expr_o&gt;</t>
   </si>
   <si>
@@ -273,12 +249,6 @@
     <t>&lt;type&gt;   -&gt;</t>
   </si>
   <si>
-    <t>&lt;if&gt; &lt;newline&gt; &lt;body&gt;</t>
-  </si>
-  <si>
-    <t>&lt;while&gt; &lt;newline&gt; &lt;body&gt;</t>
-  </si>
-  <si>
     <t>def id ( &lt;params&gt; ) EOL &lt;body&gt; end</t>
   </si>
   <si>
@@ -321,18 +291,9 @@
     <t>{=, (, id, nil, integer, float, string, +, -, /, *, ==, !=, &lt;, &gt;, &lt;=, &gt;=}</t>
   </si>
   <si>
-    <t>{id, if, while, nil, integer, float, string, not, (}</t>
-  </si>
-  <si>
-    <t>{def, id, if, while, EOF, nil, integer, float, string, not, (}</t>
-  </si>
-  <si>
     <t>{end, else, $}</t>
   </si>
   <si>
-    <t>{def, id, if, while, EOF, nil, integer, float, string, not, (, $}</t>
-  </si>
-  <si>
     <t>{EOL, $}</t>
   </si>
   <si>
@@ -396,9 +357,6 @@
     <t>{&gt;=}</t>
   </si>
   <si>
-    <t>{EOL $}</t>
-  </si>
-  <si>
     <t>( &lt;expr_id&gt; )</t>
   </si>
   <si>
@@ -424,6 +382,30 @@
   </si>
   <si>
     <t>&lt;body&gt; &lt;prog&gt;</t>
+  </si>
+  <si>
+    <t>&lt;if&gt; EOL &lt;body&gt;</t>
+  </si>
+  <si>
+    <t>&lt;while&gt; EOL &lt;body&gt;</t>
+  </si>
+  <si>
+    <t>id &lt;body_id&gt; EOL &lt;body&gt;</t>
+  </si>
+  <si>
+    <t>&lt;expr&gt; EOL &lt;body&gt;</t>
+  </si>
+  <si>
+    <t>EOL &lt;body&gt;</t>
+  </si>
+  <si>
+    <t>{id, if, while, nil, integer, float, string, not, (, EOL}</t>
+  </si>
+  <si>
+    <t>{def, id, if, while, EOF, nil, integer, float, string, not, (, EOL}</t>
+  </si>
+  <si>
+    <t>&lt;def_func&gt; EOL &lt;prog&gt;</t>
   </si>
 </sst>
 </file>
@@ -763,21 +745,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
@@ -787,6 +754,21 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1102,10 +1084,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AC8D7845-686F-4A38-8521-27846C315129}">
-  <dimension ref="A1:AE17"/>
+  <dimension ref="A1:AE15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I17" sqref="I17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M29" sqref="M29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1206,7 +1188,7 @@
         <v>35</v>
       </c>
       <c r="AE1" s="39" t="s">
-        <v>108</v>
+        <v>95</v>
       </c>
     </row>
     <row r="2" spans="1:31" x14ac:dyDescent="0.25">
@@ -1234,7 +1216,9 @@
       <c r="H2" s="43">
         <v>3</v>
       </c>
-      <c r="I2" s="43"/>
+      <c r="I2" s="43">
+        <v>2</v>
+      </c>
       <c r="J2" s="43"/>
       <c r="K2" s="43"/>
       <c r="L2" s="43"/>
@@ -1289,7 +1273,9 @@
         <v>5</v>
       </c>
       <c r="H3" s="43"/>
-      <c r="I3" s="43"/>
+      <c r="I3" s="43">
+        <v>9</v>
+      </c>
       <c r="J3" s="43"/>
       <c r="K3" s="43"/>
       <c r="L3" s="43"/>
@@ -1327,64 +1313,64 @@
     </row>
     <row r="4" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A4" s="19" t="s">
-        <v>84</v>
+        <v>74</v>
       </c>
       <c r="B4" s="42">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C4" s="43">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D4" s="43">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E4" s="43">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F4" s="43">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G4" s="43"/>
       <c r="H4" s="43"/>
       <c r="I4" s="43">
+        <v>13</v>
+      </c>
+      <c r="J4" s="43">
+        <v>10</v>
+      </c>
+      <c r="K4" s="43">
+        <v>10</v>
+      </c>
+      <c r="L4" s="43">
+        <v>10</v>
+      </c>
+      <c r="M4" s="43">
+        <v>10</v>
+      </c>
+      <c r="N4" s="43">
+        <v>10</v>
+      </c>
+      <c r="O4" s="43">
+        <v>10</v>
+      </c>
+      <c r="P4" s="43">
+        <v>10</v>
+      </c>
+      <c r="Q4" s="43">
+        <v>10</v>
+      </c>
+      <c r="R4" s="43">
+        <v>10</v>
+      </c>
+      <c r="S4" s="43">
+        <v>10</v>
+      </c>
+      <c r="T4" s="43">
         <v>12</v>
-      </c>
-      <c r="J4" s="43">
-        <v>9</v>
-      </c>
-      <c r="K4" s="43">
-        <v>9</v>
-      </c>
-      <c r="L4" s="43">
-        <v>9</v>
-      </c>
-      <c r="M4" s="43">
-        <v>9</v>
-      </c>
-      <c r="N4" s="43">
-        <v>9</v>
-      </c>
-      <c r="O4" s="43">
-        <v>9</v>
-      </c>
-      <c r="P4" s="43">
-        <v>9</v>
-      </c>
-      <c r="Q4" s="43">
-        <v>9</v>
-      </c>
-      <c r="R4" s="43">
-        <v>9</v>
-      </c>
-      <c r="S4" s="43">
-        <v>9</v>
-      </c>
-      <c r="T4" s="43">
-        <v>11</v>
       </c>
       <c r="U4" s="43"/>
       <c r="V4" s="43">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="W4" s="43"/>
       <c r="X4" s="43"/>
@@ -1398,20 +1384,20 @@
     </row>
     <row r="5" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A5" s="19" t="s">
-        <v>85</v>
+        <v>75</v>
       </c>
       <c r="B5" s="42"/>
       <c r="C5" s="43">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D5" s="43">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E5" s="43">
+        <v>17</v>
+      </c>
+      <c r="F5" s="43">
         <v>16</v>
-      </c>
-      <c r="F5" s="43">
-        <v>15</v>
       </c>
       <c r="G5" s="43"/>
       <c r="H5" s="43"/>
@@ -1440,8 +1426,8 @@
       <c r="AE5" s="45"/>
     </row>
     <row r="6" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A6" s="19" t="s">
-        <v>69</v>
+      <c r="A6" s="20" t="s">
+        <v>65</v>
       </c>
       <c r="B6" s="42"/>
       <c r="C6" s="43"/>
@@ -1450,9 +1436,7 @@
       <c r="F6" s="43"/>
       <c r="G6" s="43"/>
       <c r="H6" s="43"/>
-      <c r="I6" s="43">
-        <v>17</v>
-      </c>
+      <c r="I6" s="43"/>
       <c r="J6" s="43"/>
       <c r="K6" s="43"/>
       <c r="L6" s="43"/>
@@ -1467,7 +1451,9 @@
       <c r="U6" s="43"/>
       <c r="V6" s="43"/>
       <c r="W6" s="43"/>
-      <c r="X6" s="43"/>
+      <c r="X6" s="43">
+        <v>18</v>
+      </c>
       <c r="Y6" s="43"/>
       <c r="Z6" s="43"/>
       <c r="AA6" s="43"/>
@@ -1477,33 +1463,27 @@
       <c r="AE6" s="45"/>
     </row>
     <row r="7" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A7" s="20" t="s">
-        <v>73</v>
+      <c r="A7" s="19" t="s">
+        <v>2</v>
       </c>
       <c r="B7" s="43">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C7" s="43">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="D7" s="43">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="E7" s="43">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="F7" s="43">
-        <v>18</v>
-      </c>
-      <c r="G7" s="43">
-        <v>18</v>
-      </c>
-      <c r="H7" s="43">
-        <v>18</v>
-      </c>
-      <c r="I7" s="43">
-        <v>19</v>
-      </c>
+        <v>20</v>
+      </c>
+      <c r="G7" s="43"/>
+      <c r="H7" s="43"/>
+      <c r="I7" s="43"/>
       <c r="J7" s="43"/>
       <c r="K7" s="43"/>
       <c r="L7" s="43"/>
@@ -1515,40 +1495,44 @@
       <c r="R7" s="43"/>
       <c r="S7" s="43"/>
       <c r="T7" s="43">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="U7" s="43"/>
       <c r="V7" s="43"/>
       <c r="W7" s="43"/>
-      <c r="X7" s="43">
-        <v>18</v>
-      </c>
+      <c r="X7" s="43"/>
       <c r="Y7" s="43"/>
-      <c r="Z7" s="43">
-        <v>18</v>
-      </c>
-      <c r="AA7" s="43">
-        <v>18</v>
-      </c>
+      <c r="Z7" s="43"/>
+      <c r="AA7" s="43"/>
       <c r="AB7" s="43"/>
       <c r="AC7" s="43"/>
       <c r="AD7" s="44"/>
-      <c r="AE7" s="45">
-        <v>18</v>
-      </c>
+      <c r="AE7" s="45"/>
     </row>
     <row r="8" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A8" s="20" t="s">
-        <v>65</v>
-      </c>
-      <c r="B8" s="42"/>
-      <c r="C8" s="43"/>
-      <c r="D8" s="43"/>
-      <c r="E8" s="43"/>
-      <c r="F8" s="43"/>
+      <c r="A8" s="19" t="s">
+        <v>3</v>
+      </c>
+      <c r="B8" s="42">
+        <v>23</v>
+      </c>
+      <c r="C8" s="43">
+        <v>22</v>
+      </c>
+      <c r="D8" s="43">
+        <v>22</v>
+      </c>
+      <c r="E8" s="43">
+        <v>22</v>
+      </c>
+      <c r="F8" s="43">
+        <v>22</v>
+      </c>
       <c r="G8" s="43"/>
       <c r="H8" s="43"/>
-      <c r="I8" s="43"/>
+      <c r="I8" s="43">
+        <v>24</v>
+      </c>
       <c r="J8" s="43"/>
       <c r="K8" s="43"/>
       <c r="L8" s="43"/>
@@ -1560,42 +1544,36 @@
       <c r="R8" s="43"/>
       <c r="S8" s="43"/>
       <c r="T8" s="43"/>
-      <c r="U8" s="43"/>
+      <c r="U8" s="43">
+        <v>21</v>
+      </c>
       <c r="V8" s="43"/>
       <c r="W8" s="43"/>
-      <c r="X8" s="43">
-        <v>20</v>
-      </c>
+      <c r="X8" s="43"/>
       <c r="Y8" s="43"/>
       <c r="Z8" s="43"/>
       <c r="AA8" s="43"/>
       <c r="AB8" s="43"/>
       <c r="AC8" s="43"/>
       <c r="AD8" s="44"/>
-      <c r="AE8" s="45"/>
+      <c r="AE8" s="45">
+        <v>21</v>
+      </c>
     </row>
     <row r="9" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A9" s="19" t="s">
-        <v>2</v>
-      </c>
-      <c r="B9" s="42">
-        <v>22</v>
-      </c>
-      <c r="C9" s="43">
-        <v>22</v>
-      </c>
-      <c r="D9" s="43">
-        <v>22</v>
-      </c>
-      <c r="E9" s="43">
-        <v>22</v>
-      </c>
-      <c r="F9" s="43">
-        <v>22</v>
-      </c>
+        <v>4</v>
+      </c>
+      <c r="B9" s="42"/>
+      <c r="C9" s="43"/>
+      <c r="D9" s="43"/>
+      <c r="E9" s="43"/>
+      <c r="F9" s="43"/>
       <c r="G9" s="43"/>
       <c r="H9" s="43"/>
-      <c r="I9" s="43"/>
+      <c r="I9" s="43">
+        <v>24</v>
+      </c>
       <c r="J9" s="43"/>
       <c r="K9" s="43"/>
       <c r="L9" s="43"/>
@@ -1606,12 +1584,14 @@
       <c r="Q9" s="43"/>
       <c r="R9" s="43"/>
       <c r="S9" s="43"/>
-      <c r="T9" s="43">
-        <v>21</v>
-      </c>
-      <c r="U9" s="43"/>
+      <c r="T9" s="43"/>
+      <c r="U9" s="43">
+        <v>24</v>
+      </c>
       <c r="V9" s="43"/>
-      <c r="W9" s="43"/>
+      <c r="W9" s="43">
+        <v>25</v>
+      </c>
       <c r="X9" s="43"/>
       <c r="Y9" s="43"/>
       <c r="Z9" s="43"/>
@@ -1619,32 +1599,22 @@
       <c r="AB9" s="43"/>
       <c r="AC9" s="43"/>
       <c r="AD9" s="44"/>
-      <c r="AE9" s="45"/>
+      <c r="AE9" s="45">
+        <v>24</v>
+      </c>
     </row>
     <row r="10" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A10" s="19" t="s">
-        <v>3</v>
-      </c>
-      <c r="B10" s="42">
-        <v>25</v>
-      </c>
-      <c r="C10" s="43">
-        <v>24</v>
-      </c>
-      <c r="D10" s="43">
-        <v>24</v>
-      </c>
-      <c r="E10" s="43">
-        <v>24</v>
-      </c>
-      <c r="F10" s="43">
-        <v>24</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="B10" s="42"/>
+      <c r="C10" s="43"/>
+      <c r="D10" s="43"/>
+      <c r="E10" s="43"/>
+      <c r="F10" s="43"/>
       <c r="G10" s="43"/>
       <c r="H10" s="43"/>
-      <c r="I10" s="43">
-        <v>23</v>
-      </c>
+      <c r="I10" s="43"/>
       <c r="J10" s="43"/>
       <c r="K10" s="43"/>
       <c r="L10" s="43"/>
@@ -1656,25 +1626,23 @@
       <c r="R10" s="43"/>
       <c r="S10" s="43"/>
       <c r="T10" s="43"/>
-      <c r="U10" s="43">
-        <v>23</v>
-      </c>
+      <c r="U10" s="43"/>
       <c r="V10" s="43"/>
       <c r="W10" s="43"/>
       <c r="X10" s="43"/>
       <c r="Y10" s="43"/>
-      <c r="Z10" s="43"/>
+      <c r="Z10" s="43">
+        <v>26</v>
+      </c>
       <c r="AA10" s="43"/>
       <c r="AB10" s="43"/>
       <c r="AC10" s="43"/>
       <c r="AD10" s="44"/>
-      <c r="AE10" s="45">
-        <v>23</v>
-      </c>
+      <c r="AE10" s="45"/>
     </row>
     <row r="11" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A11" s="19" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B11" s="42"/>
       <c r="C11" s="43"/>
@@ -1683,9 +1651,7 @@
       <c r="F11" s="43"/>
       <c r="G11" s="43"/>
       <c r="H11" s="43"/>
-      <c r="I11" s="43">
-        <v>26</v>
-      </c>
+      <c r="I11" s="43"/>
       <c r="J11" s="43"/>
       <c r="K11" s="43"/>
       <c r="L11" s="43"/>
@@ -1697,134 +1663,152 @@
       <c r="R11" s="43"/>
       <c r="S11" s="43"/>
       <c r="T11" s="43"/>
-      <c r="U11" s="43">
-        <v>26</v>
-      </c>
+      <c r="U11" s="43"/>
       <c r="V11" s="43"/>
-      <c r="W11" s="43">
-        <v>27</v>
-      </c>
+      <c r="W11" s="43"/>
       <c r="X11" s="43"/>
       <c r="Y11" s="43"/>
       <c r="Z11" s="43"/>
       <c r="AA11" s="43"/>
       <c r="AB11" s="43"/>
-      <c r="AC11" s="43"/>
-      <c r="AD11" s="44"/>
-      <c r="AE11" s="45">
-        <v>26</v>
-      </c>
+      <c r="AC11" s="43">
+        <v>27</v>
+      </c>
+      <c r="AD11" s="49"/>
+      <c r="AE11" s="45"/>
     </row>
     <row r="12" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A12" s="19" t="s">
-        <v>5</v>
-      </c>
-      <c r="B12" s="42"/>
-      <c r="C12" s="43"/>
-      <c r="D12" s="43"/>
-      <c r="E12" s="43"/>
-      <c r="F12" s="43"/>
-      <c r="G12" s="43"/>
-      <c r="H12" s="43"/>
-      <c r="I12" s="43"/>
-      <c r="J12" s="43"/>
-      <c r="K12" s="43"/>
-      <c r="L12" s="43"/>
-      <c r="M12" s="43"/>
-      <c r="N12" s="43"/>
-      <c r="O12" s="43"/>
-      <c r="P12" s="43"/>
-      <c r="Q12" s="43"/>
-      <c r="R12" s="43"/>
-      <c r="S12" s="43"/>
-      <c r="T12" s="43"/>
-      <c r="U12" s="43"/>
-      <c r="V12" s="43"/>
-      <c r="W12" s="43"/>
-      <c r="X12" s="43"/>
-      <c r="Y12" s="43"/>
-      <c r="Z12" s="43">
+      <c r="A12" s="20" t="s">
+        <v>96</v>
+      </c>
+      <c r="B12" s="5">
         <v>28</v>
       </c>
-      <c r="AA12" s="43"/>
-      <c r="AB12" s="43"/>
-      <c r="AC12" s="43"/>
-      <c r="AD12" s="44"/>
-      <c r="AE12" s="45"/>
+      <c r="C12" s="5">
+        <v>29</v>
+      </c>
+      <c r="D12" s="5">
+        <v>29</v>
+      </c>
+      <c r="E12" s="5">
+        <v>29</v>
+      </c>
+      <c r="F12" s="5">
+        <v>29</v>
+      </c>
+      <c r="G12" s="5">
+        <v>29</v>
+      </c>
+      <c r="H12" s="5"/>
+      <c r="I12" s="5"/>
+      <c r="J12" s="5"/>
+      <c r="K12" s="5"/>
+      <c r="L12" s="5"/>
+      <c r="M12" s="5"/>
+      <c r="N12" s="5"/>
+      <c r="O12" s="40"/>
+      <c r="P12" s="5"/>
+      <c r="Q12" s="1"/>
+      <c r="R12" s="1"/>
+      <c r="S12" s="5"/>
+      <c r="T12" s="1">
+        <v>29</v>
+      </c>
+      <c r="U12" s="1"/>
+      <c r="V12" s="1"/>
+      <c r="W12" s="1"/>
+      <c r="X12" s="1"/>
+      <c r="Y12" s="1"/>
+      <c r="Z12" s="1"/>
+      <c r="AA12" s="1"/>
+      <c r="AB12" s="1"/>
+      <c r="AC12" s="1"/>
+      <c r="AD12" s="1"/>
+      <c r="AE12" s="24"/>
     </row>
     <row r="13" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A13" s="19" t="s">
-        <v>6</v>
-      </c>
-      <c r="B13" s="42"/>
-      <c r="C13" s="43"/>
-      <c r="D13" s="43"/>
-      <c r="E13" s="43"/>
-      <c r="F13" s="43"/>
-      <c r="G13" s="43"/>
-      <c r="H13" s="43"/>
-      <c r="I13" s="43"/>
-      <c r="J13" s="43"/>
-      <c r="K13" s="43"/>
-      <c r="L13" s="43"/>
-      <c r="M13" s="43"/>
-      <c r="N13" s="43"/>
-      <c r="O13" s="43"/>
-      <c r="P13" s="43"/>
-      <c r="Q13" s="43"/>
-      <c r="R13" s="43"/>
-      <c r="S13" s="43"/>
-      <c r="T13" s="43"/>
-      <c r="U13" s="43"/>
-      <c r="V13" s="43"/>
-      <c r="W13" s="43"/>
-      <c r="X13" s="43"/>
-      <c r="Y13" s="43"/>
-      <c r="Z13" s="43"/>
-      <c r="AA13" s="43"/>
-      <c r="AB13" s="43"/>
-      <c r="AC13" s="43">
-        <v>29</v>
-      </c>
-      <c r="AD13" s="54"/>
-      <c r="AE13" s="45"/>
+      <c r="A13" s="20" t="s">
+        <v>69</v>
+      </c>
+      <c r="B13" s="5"/>
+      <c r="C13" s="5"/>
+      <c r="D13" s="5"/>
+      <c r="E13" s="5"/>
+      <c r="F13" s="5"/>
+      <c r="G13" s="5"/>
+      <c r="H13" s="5"/>
+      <c r="I13" s="5">
+        <v>40</v>
+      </c>
+      <c r="J13" s="5">
+        <v>30</v>
+      </c>
+      <c r="K13" s="5">
+        <v>31</v>
+      </c>
+      <c r="L13" s="5">
+        <v>32</v>
+      </c>
+      <c r="M13" s="5">
+        <v>33</v>
+      </c>
+      <c r="N13" s="5">
+        <v>34</v>
+      </c>
+      <c r="O13" s="5">
+        <v>35</v>
+      </c>
+      <c r="P13" s="5">
+        <v>36</v>
+      </c>
+      <c r="Q13" s="5">
+        <v>37</v>
+      </c>
+      <c r="R13" s="5">
+        <v>38</v>
+      </c>
+      <c r="S13" s="5">
+        <v>39</v>
+      </c>
+      <c r="T13" s="5"/>
+      <c r="U13" s="5"/>
+      <c r="V13" s="5"/>
+      <c r="W13" s="5"/>
+      <c r="X13" s="5"/>
+      <c r="Y13" s="5"/>
+      <c r="Z13" s="5"/>
+      <c r="AA13" s="5"/>
+      <c r="AB13" s="5"/>
+      <c r="AC13" s="5"/>
+      <c r="AD13" s="5"/>
+      <c r="AE13" s="24">
+        <v>40</v>
+      </c>
     </row>
     <row r="14" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A14" s="20" t="s">
-        <v>109</v>
-      </c>
-      <c r="B14" s="5">
-        <v>30</v>
-      </c>
-      <c r="C14" s="5">
-        <v>31</v>
-      </c>
-      <c r="D14" s="5">
-        <v>31</v>
-      </c>
-      <c r="E14" s="5">
-        <v>31</v>
-      </c>
-      <c r="F14" s="5">
-        <v>31</v>
-      </c>
-      <c r="G14" s="5">
-        <v>31</v>
-      </c>
-      <c r="H14" s="5"/>
-      <c r="I14" s="5"/>
-      <c r="J14" s="5"/>
-      <c r="K14" s="5"/>
-      <c r="L14" s="5"/>
-      <c r="M14" s="5"/>
-      <c r="N14" s="5"/>
-      <c r="O14" s="40"/>
-      <c r="P14" s="5"/>
-      <c r="Q14" s="1"/>
-      <c r="R14" s="1"/>
-      <c r="S14" s="5"/>
+        <v>110</v>
+      </c>
+      <c r="B14" s="1">
+        <v>42</v>
+      </c>
+      <c r="C14" s="1">
+        <v>41</v>
+      </c>
+      <c r="D14" s="1">
+        <v>41</v>
+      </c>
+      <c r="E14" s="1">
+        <v>41</v>
+      </c>
+      <c r="F14" s="1">
+        <v>41</v>
+      </c>
+      <c r="G14" s="1">
+        <v>41</v>
+      </c>
       <c r="T14" s="1">
-        <v>31</v>
+        <v>41</v>
       </c>
       <c r="U14" s="1"/>
       <c r="V14" s="1"/>
@@ -1839,167 +1823,71 @@
       <c r="AE14" s="24"/>
     </row>
     <row r="15" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A15" s="20" t="s">
-        <v>77</v>
-      </c>
-      <c r="B15" s="5"/>
-      <c r="C15" s="5"/>
-      <c r="D15" s="5"/>
-      <c r="E15" s="5"/>
-      <c r="F15" s="5"/>
-      <c r="G15" s="5"/>
-      <c r="H15" s="5"/>
-      <c r="I15" s="5">
-        <v>42</v>
-      </c>
-      <c r="J15" s="5">
-        <v>32</v>
-      </c>
-      <c r="K15" s="5">
-        <v>33</v>
-      </c>
-      <c r="L15" s="5">
-        <v>34</v>
-      </c>
-      <c r="M15" s="5">
-        <v>35</v>
-      </c>
-      <c r="N15" s="5">
-        <v>36</v>
-      </c>
-      <c r="O15" s="5">
-        <v>37</v>
-      </c>
-      <c r="P15" s="5">
-        <v>38</v>
-      </c>
-      <c r="Q15" s="5">
-        <v>39</v>
-      </c>
-      <c r="R15" s="5">
-        <v>40</v>
-      </c>
-      <c r="S15" s="5">
-        <v>41</v>
-      </c>
-      <c r="T15" s="5"/>
-      <c r="U15" s="5"/>
-      <c r="V15" s="5"/>
-      <c r="W15" s="5"/>
-      <c r="X15" s="5"/>
-      <c r="Y15" s="5"/>
-      <c r="Z15" s="5"/>
-      <c r="AA15" s="5"/>
-      <c r="AB15" s="5"/>
-      <c r="AC15" s="5"/>
-      <c r="AD15" s="5"/>
-      <c r="AE15" s="24">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="16" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A16" s="20" t="s">
-        <v>124</v>
-      </c>
-      <c r="B16" s="1">
+      <c r="A15" s="27" t="s">
+        <v>114</v>
+      </c>
+      <c r="B15" s="17">
         <v>44</v>
       </c>
-      <c r="C16" s="1">
+      <c r="C15" s="17">
+        <v>44</v>
+      </c>
+      <c r="D15" s="17">
+        <v>44</v>
+      </c>
+      <c r="E15" s="17">
+        <v>44</v>
+      </c>
+      <c r="F15" s="17">
+        <v>44</v>
+      </c>
+      <c r="G15" s="17"/>
+      <c r="H15" s="17"/>
+      <c r="I15" s="17"/>
+      <c r="J15" s="17">
         <v>43</v>
       </c>
-      <c r="D16" s="1">
+      <c r="K15" s="17">
         <v>43</v>
       </c>
-      <c r="E16" s="1">
+      <c r="L15" s="17">
         <v>43</v>
       </c>
-      <c r="F16" s="1">
+      <c r="M15" s="17">
         <v>43</v>
       </c>
-      <c r="G16" s="1">
+      <c r="N15" s="17">
         <v>43</v>
       </c>
-      <c r="T16" s="1">
+      <c r="O15" s="17">
         <v>43</v>
       </c>
-      <c r="U16" s="1"/>
-      <c r="V16" s="1"/>
-      <c r="W16" s="1"/>
-      <c r="X16" s="1"/>
-      <c r="Y16" s="1"/>
-      <c r="Z16" s="1"/>
-      <c r="AA16" s="1"/>
-      <c r="AB16" s="1"/>
-      <c r="AC16" s="1"/>
-      <c r="AD16" s="1"/>
-      <c r="AE16" s="24"/>
-    </row>
-    <row r="17" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A17" s="27" t="s">
-        <v>128</v>
-      </c>
-      <c r="B17" s="17">
-        <v>46</v>
-      </c>
-      <c r="C17" s="17">
-        <v>46</v>
-      </c>
-      <c r="D17" s="17">
-        <v>46</v>
-      </c>
-      <c r="E17" s="17">
-        <v>46</v>
-      </c>
-      <c r="F17" s="17">
-        <v>46</v>
-      </c>
-      <c r="G17" s="17"/>
-      <c r="H17" s="17"/>
-      <c r="I17" s="17"/>
-      <c r="J17" s="17">
-        <v>45</v>
-      </c>
-      <c r="K17" s="17">
-        <v>45</v>
-      </c>
-      <c r="L17" s="17">
-        <v>45</v>
-      </c>
-      <c r="M17" s="17">
-        <v>45</v>
-      </c>
-      <c r="N17" s="17">
-        <v>45</v>
-      </c>
-      <c r="O17" s="17">
-        <v>45</v>
-      </c>
-      <c r="P17" s="17">
-        <v>45</v>
-      </c>
-      <c r="Q17" s="17">
-        <v>45</v>
-      </c>
-      <c r="R17" s="17">
-        <v>45</v>
-      </c>
-      <c r="S17" s="17">
-        <v>45</v>
-      </c>
-      <c r="T17" s="17">
-        <v>46</v>
-      </c>
-      <c r="U17" s="17"/>
-      <c r="V17" s="17"/>
-      <c r="W17" s="17"/>
-      <c r="X17" s="17"/>
-      <c r="Y17" s="17"/>
-      <c r="Z17" s="17"/>
-      <c r="AA17" s="17"/>
-      <c r="AB17" s="17"/>
-      <c r="AC17" s="17"/>
-      <c r="AD17" s="17"/>
-      <c r="AE17" s="55"/>
+      <c r="P15" s="17">
+        <v>43</v>
+      </c>
+      <c r="Q15" s="17">
+        <v>43</v>
+      </c>
+      <c r="R15" s="17">
+        <v>43</v>
+      </c>
+      <c r="S15" s="17">
+        <v>43</v>
+      </c>
+      <c r="T15" s="17">
+        <v>44</v>
+      </c>
+      <c r="U15" s="17"/>
+      <c r="V15" s="17"/>
+      <c r="W15" s="17"/>
+      <c r="X15" s="17"/>
+      <c r="Y15" s="17"/>
+      <c r="Z15" s="17"/>
+      <c r="AA15" s="17"/>
+      <c r="AB15" s="17"/>
+      <c r="AC15" s="17"/>
+      <c r="AD15" s="17"/>
+      <c r="AE15" s="50"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
@@ -2011,8 +1899,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B9B981D-AC8B-4430-B1E8-C28C34350FA5}">
   <dimension ref="A1:AK47"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+    <sheetView topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D36" sqref="D36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2045,21 +1933,21 @@
       </c>
       <c r="E1" s="6"/>
       <c r="F1" s="18"/>
-      <c r="G1" s="48" t="s">
+      <c r="G1" s="52" t="s">
         <v>61</v>
       </c>
-      <c r="H1" s="48"/>
-      <c r="I1" s="49"/>
+      <c r="H1" s="52"/>
+      <c r="I1" s="53"/>
       <c r="J1" s="29" t="s">
         <v>48</v>
       </c>
       <c r="K1" s="33"/>
       <c r="L1" s="18"/>
-      <c r="M1" s="50" t="s">
-        <v>92</v>
-      </c>
-      <c r="N1" s="51"/>
-      <c r="O1" s="52"/>
+      <c r="M1" s="54" t="s">
+        <v>82</v>
+      </c>
+      <c r="N1" s="55"/>
+      <c r="O1" s="56"/>
       <c r="P1" s="6"/>
       <c r="Q1" s="6"/>
       <c r="R1" s="6"/>
@@ -2075,14 +1963,14 @@
       <c r="AB1" s="6"/>
     </row>
     <row r="2" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A2" s="53" t="s">
+      <c r="A2" s="48" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>36</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>97</v>
+        <v>123</v>
       </c>
       <c r="D2" s="23" t="s">
         <v>62</v>
@@ -2096,7 +1984,7 @@
       </c>
       <c r="H2" s="7"/>
       <c r="I2" s="14" t="s">
-        <v>75</v>
+        <v>124</v>
       </c>
       <c r="J2" s="12" t="s">
         <v>42</v>
@@ -2106,11 +1994,11 @@
         <v>1</v>
       </c>
       <c r="M2" s="34" t="s">
-        <v>89</v>
+        <v>79</v>
       </c>
       <c r="N2" s="5"/>
       <c r="O2" s="9" t="s">
-        <v>85</v>
+        <v>75</v>
       </c>
       <c r="P2" s="5"/>
       <c r="Q2" s="5"/>
@@ -2143,10 +2031,10 @@
         <v>38</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>96</v>
+        <v>122</v>
       </c>
       <c r="D3" s="24" t="s">
-        <v>98</v>
+        <v>86</v>
       </c>
       <c r="E3" s="1"/>
       <c r="F3" s="30">
@@ -2157,20 +2045,20 @@
       </c>
       <c r="H3" s="6"/>
       <c r="I3" s="31" t="s">
-        <v>130</v>
+        <v>116</v>
       </c>
       <c r="J3" s="4" t="s">
-        <v>96</v>
+        <v>122</v>
       </c>
       <c r="L3" s="4">
         <v>2</v>
       </c>
       <c r="M3" s="34" t="s">
-        <v>89</v>
+        <v>79</v>
       </c>
       <c r="N3" s="5"/>
       <c r="O3" s="9" t="s">
-        <v>123</v>
+        <v>109</v>
       </c>
       <c r="P3" s="1"/>
       <c r="Q3" s="1"/>
@@ -2188,13 +2076,13 @@
     </row>
     <row r="4" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A4" s="19" t="s">
-        <v>84</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>36</v>
+        <v>74</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>38</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>95</v>
+        <v>85</v>
       </c>
       <c r="D4" s="4" t="s">
         <v>47</v>
@@ -2217,11 +2105,11 @@
         <v>3</v>
       </c>
       <c r="M4" s="34" t="s">
-        <v>89</v>
+        <v>79</v>
       </c>
       <c r="N4" s="5"/>
       <c r="O4" s="9" t="s">
-        <v>93</v>
+        <v>83</v>
       </c>
       <c r="P4" s="1"/>
       <c r="Q4" s="1"/>
@@ -2239,13 +2127,13 @@
     </row>
     <row r="5" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A5" s="19" t="s">
-        <v>85</v>
+        <v>75</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>38</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>88</v>
+        <v>78</v>
       </c>
       <c r="D5" s="4" t="s">
         <v>43</v>
@@ -2259,7 +2147,7 @@
       </c>
       <c r="H5" s="7"/>
       <c r="I5" s="9" t="s">
-        <v>76</v>
+        <v>119</v>
       </c>
       <c r="J5" s="4" t="s">
         <v>39</v>
@@ -2269,11 +2157,11 @@
         <v>4</v>
       </c>
       <c r="M5" s="37" t="s">
-        <v>89</v>
+        <v>79</v>
       </c>
       <c r="N5" s="17"/>
       <c r="O5" s="47" t="s">
-        <v>122</v>
+        <v>108</v>
       </c>
       <c r="P5" s="1"/>
       <c r="Q5" s="1"/>
@@ -2290,17 +2178,17 @@
       <c r="AB5" s="1"/>
     </row>
     <row r="6" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A6" s="19" t="s">
-        <v>69</v>
-      </c>
-      <c r="B6" s="3" t="s">
+      <c r="A6" s="20" t="s">
+        <v>65</v>
+      </c>
+      <c r="B6" s="16" t="s">
         <v>36</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="C6" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="D6" s="4" t="s">
         <v>47</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>99</v>
       </c>
       <c r="E6" s="1"/>
       <c r="F6" s="30">
@@ -2311,10 +2199,10 @@
       </c>
       <c r="H6" s="7"/>
       <c r="I6" s="9" t="s">
-        <v>74</v>
+        <v>120</v>
       </c>
       <c r="J6" s="4" t="s">
-        <v>105</v>
+        <v>92</v>
       </c>
       <c r="K6" s="1"/>
       <c r="L6" s="5"/>
@@ -2336,17 +2224,17 @@
       <c r="AB6" s="1"/>
     </row>
     <row r="7" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A7" s="20" t="s">
-        <v>73</v>
+      <c r="A7" s="19" t="s">
+        <v>2</v>
       </c>
       <c r="B7" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="C7" s="12" t="s">
-        <v>47</v>
+      <c r="C7" s="4" t="s">
+        <v>77</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>99</v>
+        <v>87</v>
       </c>
       <c r="E7" s="1"/>
       <c r="F7" s="30">
@@ -2359,7 +2247,7 @@
         <v>51</v>
       </c>
       <c r="J7" s="24" t="s">
-        <v>98</v>
+        <v>86</v>
       </c>
       <c r="K7" s="1"/>
       <c r="L7" s="5"/>
@@ -2381,17 +2269,17 @@
       <c r="AB7" s="1"/>
     </row>
     <row r="8" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A8" s="20" t="s">
-        <v>65</v>
-      </c>
-      <c r="B8" s="16" t="s">
-        <v>36</v>
-      </c>
-      <c r="C8" s="12" t="s">
-        <v>42</v>
+      <c r="A8" s="19" t="s">
+        <v>3</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>76</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>47</v>
+        <v>88</v>
       </c>
       <c r="E8" s="1"/>
       <c r="F8" s="30">
@@ -2401,7 +2289,7 @@
         <v>49</v>
       </c>
       <c r="I8" t="s">
-        <v>80</v>
+        <v>117</v>
       </c>
       <c r="J8" s="4" t="s">
         <v>44</v>
@@ -2427,16 +2315,16 @@
     </row>
     <row r="9" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A9" s="19" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B9" s="4" t="s">
         <v>38</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>87</v>
+        <v>43</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>100</v>
+        <v>88</v>
       </c>
       <c r="E9" s="1"/>
       <c r="F9" s="30">
@@ -2446,7 +2334,7 @@
         <v>49</v>
       </c>
       <c r="I9" t="s">
-        <v>81</v>
+        <v>118</v>
       </c>
       <c r="J9" s="15" t="s">
         <v>45</v>
@@ -2472,29 +2360,29 @@
     </row>
     <row r="10" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A10" s="19" t="s">
-        <v>3</v>
-      </c>
-      <c r="B10" s="4" t="s">
-        <v>38</v>
+        <v>5</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>36</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>86</v>
+        <v>44</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>101</v>
+        <v>47</v>
       </c>
       <c r="E10" s="1"/>
       <c r="F10" s="30">
         <v>9</v>
       </c>
       <c r="G10" s="7" t="s">
-        <v>78</v>
-      </c>
-      <c r="I10" s="9" t="s">
-        <v>77</v>
+        <v>49</v>
+      </c>
+      <c r="I10" s="13" t="s">
+        <v>121</v>
       </c>
       <c r="J10" s="4" t="s">
-        <v>106</v>
+        <v>47</v>
       </c>
       <c r="K10" s="1"/>
       <c r="L10" s="5"/>
@@ -2517,31 +2405,29 @@
     </row>
     <row r="11" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A11" s="19" t="s">
-        <v>4</v>
-      </c>
-      <c r="B11" s="4" t="s">
-        <v>38</v>
+        <v>6</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>36</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="D11" s="4" t="s">
-        <v>101</v>
+        <v>45</v>
+      </c>
+      <c r="D11" s="24" t="s">
+        <v>47</v>
       </c>
       <c r="E11" s="5"/>
       <c r="F11" s="30">
         <v>10</v>
       </c>
       <c r="G11" s="7" t="s">
-        <v>78</v>
-      </c>
-      <c r="H11" s="7"/>
-      <c r="I11" s="11" t="str">
-        <f>"= &lt;defvar&gt;"</f>
-        <v>= &lt;defvar&gt;</v>
+        <v>70</v>
+      </c>
+      <c r="I11" s="9" t="s">
+        <v>69</v>
       </c>
       <c r="J11" s="4" t="s">
-        <v>107</v>
+        <v>93</v>
       </c>
       <c r="K11" s="1"/>
       <c r="L11" s="5"/>
@@ -2563,31 +2449,32 @@
       <c r="AB11" s="5"/>
     </row>
     <row r="12" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A12" s="19" t="s">
-        <v>5</v>
+      <c r="A12" s="20" t="s">
+        <v>96</v>
       </c>
       <c r="B12" s="3" t="s">
         <v>36</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>44</v>
+        <v>97</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>47</v>
+        <v>87</v>
       </c>
       <c r="E12" s="5"/>
       <c r="F12" s="30">
         <v>11</v>
       </c>
       <c r="G12" s="7" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="H12" s="7"/>
-      <c r="I12" s="9" t="s">
-        <v>2</v>
+      <c r="I12" s="11" t="str">
+        <f>"= &lt;defvar&gt;"</f>
+        <v>= &lt;defvar&gt;</v>
       </c>
       <c r="J12" s="4" t="s">
-        <v>87</v>
+        <v>94</v>
       </c>
       <c r="L12" s="5"/>
       <c r="M12" s="7"/>
@@ -2608,31 +2495,31 @@
       <c r="AB12" s="1"/>
     </row>
     <row r="13" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A13" s="19" t="s">
-        <v>6</v>
+      <c r="A13" s="20" t="s">
+        <v>69</v>
       </c>
       <c r="B13" s="3" t="s">
         <v>36</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="D13" s="24" t="s">
-        <v>47</v>
+        <v>93</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>87</v>
       </c>
       <c r="E13" s="1"/>
       <c r="F13" s="30">
         <v>12</v>
       </c>
       <c r="G13" s="7" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="H13" s="7"/>
-      <c r="I13" s="13" t="s">
-        <v>51</v>
+      <c r="I13" s="9" t="s">
+        <v>2</v>
       </c>
       <c r="J13" s="4" t="s">
-        <v>47</v>
+        <v>77</v>
       </c>
       <c r="L13" s="5"/>
       <c r="M13" s="7"/>
@@ -2653,31 +2540,31 @@
       <c r="AB13" s="1"/>
     </row>
     <row r="14" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A14" s="20" t="s">
-        <v>109</v>
+      <c r="A14" s="19" t="s">
+        <v>110</v>
       </c>
       <c r="B14" s="3" t="s">
         <v>36</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>110</v>
+        <v>97</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>121</v>
+        <v>87</v>
       </c>
       <c r="E14" s="1"/>
       <c r="F14" s="30">
         <v>13</v>
       </c>
       <c r="G14" s="7" t="s">
-        <v>79</v>
-      </c>
-      <c r="H14" s="6"/>
-      <c r="I14" s="11" t="s">
-        <v>8</v>
+        <v>70</v>
+      </c>
+      <c r="H14" s="7"/>
+      <c r="I14" s="13" t="s">
+        <v>51</v>
       </c>
       <c r="J14" s="4" t="s">
-        <v>40</v>
+        <v>47</v>
       </c>
       <c r="K14" s="5"/>
       <c r="L14" s="5"/>
@@ -2699,31 +2586,31 @@
       <c r="AB14" s="1"/>
     </row>
     <row r="15" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A15" s="20" t="s">
-        <v>77</v>
-      </c>
-      <c r="B15" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="C15" s="4" t="s">
-        <v>106</v>
-      </c>
-      <c r="D15" s="4" t="s">
-        <v>100</v>
+      <c r="A15" s="21" t="s">
+        <v>114</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>87</v>
       </c>
       <c r="E15" s="1"/>
       <c r="F15" s="30">
         <v>14</v>
       </c>
       <c r="G15" s="7" t="s">
-        <v>79</v>
+        <v>71</v>
       </c>
       <c r="H15" s="6"/>
-      <c r="I15" s="13" t="s">
-        <v>9</v>
+      <c r="I15" s="11" t="s">
+        <v>8</v>
       </c>
       <c r="J15" s="4" t="s">
-        <v>102</v>
+        <v>40</v>
       </c>
       <c r="K15" s="1"/>
       <c r="L15" s="5"/>
@@ -2746,30 +2633,28 @@
     </row>
     <row r="16" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A16" s="19" t="s">
-        <v>124</v>
-      </c>
-      <c r="B16" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B16" s="4" t="s">
         <v>36</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>110</v>
-      </c>
-      <c r="D16" s="4" t="s">
-        <v>100</v>
-      </c>
+        <v>39</v>
+      </c>
+      <c r="D16" s="4"/>
       <c r="E16" s="1"/>
       <c r="F16" s="30">
         <v>15</v>
       </c>
       <c r="G16" s="7" t="s">
-        <v>79</v>
+        <v>71</v>
       </c>
       <c r="H16" s="6"/>
-      <c r="I16" s="11" t="s">
-        <v>11</v>
+      <c r="I16" s="13" t="s">
+        <v>9</v>
       </c>
       <c r="J16" s="4" t="s">
-        <v>103</v>
+        <v>89</v>
       </c>
       <c r="K16" s="1"/>
       <c r="L16" s="5"/>
@@ -2791,31 +2676,29 @@
       <c r="AB16" s="1"/>
     </row>
     <row r="17" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A17" s="21" t="s">
-        <v>128</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="D17" s="2" t="s">
-        <v>100</v>
-      </c>
+      <c r="A17" s="19" t="s">
+        <v>8</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="D17" s="4"/>
       <c r="E17" s="1"/>
       <c r="F17" s="30">
         <v>16</v>
       </c>
       <c r="G17" s="7" t="s">
-        <v>79</v>
+        <v>71</v>
       </c>
       <c r="H17" s="6"/>
-      <c r="I17" s="9" t="s">
-        <v>10</v>
+      <c r="I17" s="11" t="s">
+        <v>11</v>
       </c>
       <c r="J17" s="4" t="s">
-        <v>104</v>
+        <v>90</v>
       </c>
       <c r="K17" s="1"/>
       <c r="L17" s="5"/>
@@ -2838,28 +2721,29 @@
     </row>
     <row r="18" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A18" s="19" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B18" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="C18" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="D18" s="4"/>
+      <c r="C18" s="4" t="str">
+        <f>"{"&amp;A18&amp;"}"</f>
+        <v>{integer}</v>
+      </c>
+      <c r="D18" s="12"/>
       <c r="E18" s="1"/>
       <c r="F18" s="30">
         <v>17</v>
       </c>
       <c r="G18" s="7" t="s">
-        <v>70</v>
-      </c>
-      <c r="H18" s="7"/>
+        <v>71</v>
+      </c>
+      <c r="H18" s="6"/>
       <c r="I18" s="9" t="s">
-        <v>72</v>
+        <v>10</v>
       </c>
       <c r="J18" s="4" t="s">
-        <v>47</v>
+        <v>91</v>
       </c>
       <c r="K18" s="1"/>
       <c r="L18" s="5"/>
@@ -2882,13 +2766,14 @@
     </row>
     <row r="19" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A19" s="19" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B19" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="C19" s="4" t="s">
-        <v>40</v>
+      <c r="C19" s="4" t="str">
+        <f t="shared" ref="C19:C44" si="0">"{"&amp;A19&amp;"}"</f>
+        <v>{string}</v>
       </c>
       <c r="D19" s="4"/>
       <c r="E19" s="1"/>
@@ -2896,14 +2781,14 @@
         <v>18</v>
       </c>
       <c r="G19" s="7" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="H19" s="7"/>
-      <c r="I19" s="13" t="s">
-        <v>51</v>
+      <c r="I19" s="9" t="s">
+        <v>72</v>
       </c>
       <c r="J19" s="4" t="s">
-        <v>99</v>
+        <v>42</v>
       </c>
       <c r="K19" s="36"/>
       <c r="L19" s="5"/>
@@ -2926,29 +2811,29 @@
     </row>
     <row r="20" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A20" s="19" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B20" s="4" t="s">
         <v>36</v>
       </c>
       <c r="C20" s="4" t="str">
-        <f>"{"&amp;A20&amp;"}"</f>
-        <v>{integer}</v>
-      </c>
-      <c r="D20" s="12"/>
+        <f t="shared" si="0"/>
+        <v>{float}</v>
+      </c>
+      <c r="D20" s="4"/>
       <c r="E20" s="1"/>
       <c r="F20" s="30">
         <v>19</v>
       </c>
       <c r="G20" s="7" t="s">
-        <v>71</v>
-      </c>
-      <c r="H20" s="6"/>
-      <c r="I20" s="11" t="s">
-        <v>69</v>
+        <v>52</v>
+      </c>
+      <c r="H20" s="7"/>
+      <c r="I20" s="9" t="s">
+        <v>64</v>
       </c>
       <c r="J20" s="4" t="s">
-        <v>47</v>
+        <v>67</v>
       </c>
       <c r="K20" s="36"/>
       <c r="L20" s="5"/>
@@ -2971,14 +2856,14 @@
     </row>
     <row r="21" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A21" s="19" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="B21" s="4" t="s">
         <v>36</v>
       </c>
       <c r="C21" s="4" t="str">
-        <f t="shared" ref="C21:C46" si="0">"{"&amp;A21&amp;"}"</f>
-        <v>{string}</v>
+        <f t="shared" si="0"/>
+        <v>{not}</v>
       </c>
       <c r="D21" s="4"/>
       <c r="E21" s="1"/>
@@ -2986,14 +2871,14 @@
         <v>20</v>
       </c>
       <c r="G21" s="7" t="s">
-        <v>63</v>
+        <v>52</v>
       </c>
       <c r="H21" s="7"/>
       <c r="I21" s="9" t="s">
-        <v>82</v>
+        <v>3</v>
       </c>
       <c r="J21" s="4" t="s">
-        <v>42</v>
+        <v>76</v>
       </c>
       <c r="K21" s="36"/>
       <c r="L21" s="5"/>
@@ -3016,14 +2901,14 @@
     </row>
     <row r="22" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A22" s="19" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B22" s="4" t="s">
         <v>36</v>
       </c>
       <c r="C22" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>{float}</v>
+        <v>{EOF}</v>
       </c>
       <c r="D22" s="4"/>
       <c r="E22" s="1"/>
@@ -3031,14 +2916,14 @@
         <v>21</v>
       </c>
       <c r="G22" s="7" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="H22" s="7"/>
       <c r="I22" s="9" t="s">
-        <v>64</v>
+        <v>51</v>
       </c>
       <c r="J22" s="4" t="s">
-        <v>67</v>
+        <v>88</v>
       </c>
       <c r="K22" s="36"/>
       <c r="L22" s="5"/>
@@ -3061,14 +2946,14 @@
     </row>
     <row r="23" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A23" s="19" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B23" s="4" t="s">
         <v>36</v>
       </c>
       <c r="C23" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>{not}</v>
+        <v>{EOL}</v>
       </c>
       <c r="D23" s="4"/>
       <c r="E23" s="1"/>
@@ -3076,14 +2961,14 @@
         <v>22</v>
       </c>
       <c r="G23" s="7" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="H23" s="7"/>
       <c r="I23" s="9" t="s">
-        <v>3</v>
+        <v>73</v>
       </c>
       <c r="J23" s="4" t="s">
-        <v>86</v>
+        <v>78</v>
       </c>
       <c r="K23" s="36"/>
       <c r="L23" s="5"/>
@@ -3106,14 +2991,14 @@
     </row>
     <row r="24" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A24" s="19" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B24" s="4" t="s">
         <v>36</v>
       </c>
       <c r="C24" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>{EOF}</v>
+        <v>{+}</v>
       </c>
       <c r="D24" s="4"/>
       <c r="E24" s="1"/>
@@ -3125,10 +3010,10 @@
       </c>
       <c r="H24" s="7"/>
       <c r="I24" s="9" t="s">
-        <v>51</v>
+        <v>57</v>
       </c>
       <c r="J24" s="4" t="s">
-        <v>101</v>
+        <v>39</v>
       </c>
       <c r="K24" s="36"/>
       <c r="L24" s="5"/>
@@ -3151,14 +3036,14 @@
     </row>
     <row r="25" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A25" s="19" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="B25" s="4" t="s">
         <v>36</v>
       </c>
       <c r="C25" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>{EOL}</v>
+        <v>{-}</v>
       </c>
       <c r="D25" s="4"/>
       <c r="E25" s="1"/>
@@ -3166,11 +3051,11 @@
         <v>24</v>
       </c>
       <c r="G25" s="7" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="H25" s="7"/>
       <c r="I25" s="9" t="s">
-        <v>83</v>
+        <v>51</v>
       </c>
       <c r="J25" s="4" t="s">
         <v>88</v>
@@ -3196,14 +3081,14 @@
     </row>
     <row r="26" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A26" s="19" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B26" s="4" t="s">
         <v>36</v>
       </c>
       <c r="C26" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>{+}</v>
+        <v>{*}</v>
       </c>
       <c r="D26" s="4"/>
       <c r="E26" s="1"/>
@@ -3211,14 +3096,14 @@
         <v>25</v>
       </c>
       <c r="G26" s="7" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="H26" s="7"/>
       <c r="I26" s="9" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="J26" s="4" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="K26" s="36"/>
       <c r="L26" s="5"/>
@@ -3241,29 +3126,29 @@
     </row>
     <row r="27" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A27" s="19" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B27" s="4" t="s">
         <v>36</v>
       </c>
       <c r="C27" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>{-}</v>
+        <v>{/}</v>
       </c>
       <c r="D27" s="4"/>
       <c r="E27" s="1"/>
       <c r="F27" s="30">
         <v>26</v>
       </c>
-      <c r="G27" s="7" t="s">
-        <v>54</v>
+      <c r="G27" s="34" t="s">
+        <v>55</v>
       </c>
       <c r="H27" s="7"/>
       <c r="I27" s="9" t="s">
-        <v>51</v>
+        <v>59</v>
       </c>
       <c r="J27" s="4" t="s">
-        <v>101</v>
+        <v>44</v>
       </c>
       <c r="K27" s="36"/>
       <c r="L27" s="5"/>
@@ -3285,30 +3170,30 @@
       <c r="AB27" s="1"/>
     </row>
     <row r="28" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A28" s="19" t="s">
-        <v>17</v>
+      <c r="A28" s="26" t="s">
+        <v>19</v>
       </c>
       <c r="B28" s="4" t="s">
         <v>36</v>
       </c>
       <c r="C28" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>{*}</v>
+        <v>{==}</v>
       </c>
       <c r="D28" s="4"/>
       <c r="E28" s="1"/>
       <c r="F28" s="30">
         <v>27</v>
       </c>
-      <c r="G28" s="7" t="s">
-        <v>54</v>
-      </c>
-      <c r="H28" s="7"/>
-      <c r="I28" s="9" t="s">
-        <v>58</v>
+      <c r="G28" s="46" t="s">
+        <v>56</v>
+      </c>
+      <c r="H28" s="6"/>
+      <c r="I28" s="11" t="s">
+        <v>60</v>
       </c>
       <c r="J28" s="4" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="K28" s="36"/>
       <c r="L28" s="5"/>
@@ -3331,14 +3216,14 @@
     </row>
     <row r="29" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A29" s="19" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B29" s="4" t="s">
         <v>36</v>
       </c>
       <c r="C29" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>{/}</v>
+        <v>{!=}</v>
       </c>
       <c r="D29" s="4"/>
       <c r="E29" s="1"/>
@@ -3346,14 +3231,13 @@
         <v>28</v>
       </c>
       <c r="G29" s="34" t="s">
-        <v>55</v>
-      </c>
-      <c r="H29" s="7"/>
+        <v>80</v>
+      </c>
       <c r="I29" s="9" t="s">
-        <v>59</v>
+        <v>84</v>
       </c>
       <c r="J29" s="4" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="K29" s="36"/>
       <c r="L29" s="5"/>
@@ -3375,30 +3259,29 @@
       <c r="AB29" s="1"/>
     </row>
     <row r="30" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A30" s="26" t="s">
-        <v>19</v>
+      <c r="A30" s="19" t="s">
+        <v>21</v>
       </c>
       <c r="B30" s="4" t="s">
         <v>36</v>
       </c>
       <c r="C30" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>{==}</v>
+        <v>{&lt;}</v>
       </c>
       <c r="D30" s="4"/>
       <c r="E30" s="1"/>
       <c r="F30" s="30">
         <v>29</v>
       </c>
-      <c r="G30" s="46" t="s">
-        <v>56</v>
-      </c>
-      <c r="H30" s="6"/>
-      <c r="I30" s="11" t="s">
-        <v>60</v>
+      <c r="G30" s="34" t="s">
+        <v>80</v>
+      </c>
+      <c r="I30" s="9" t="s">
+        <v>68</v>
       </c>
       <c r="J30" s="4" t="s">
-        <v>45</v>
+        <v>92</v>
       </c>
       <c r="K30" s="36"/>
       <c r="L30" s="5"/>
@@ -3421,14 +3304,14 @@
     </row>
     <row r="31" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A31" s="19" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B31" s="4" t="s">
         <v>36</v>
       </c>
       <c r="C31" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>{!=}</v>
+        <v>{&gt;}</v>
       </c>
       <c r="D31" s="4"/>
       <c r="E31" s="1"/>
@@ -3436,13 +3319,14 @@
         <v>30</v>
       </c>
       <c r="G31" s="34" t="s">
-        <v>90</v>
-      </c>
-      <c r="I31" s="9" t="s">
-        <v>94</v>
+        <v>81</v>
+      </c>
+      <c r="I31" s="9" t="str">
+        <f xml:space="preserve"> "+ &lt;expr_id&gt;"</f>
+        <v>+ &lt;expr_id&gt;</v>
       </c>
       <c r="J31" s="4" t="s">
-        <v>39</v>
+        <v>98</v>
       </c>
       <c r="K31" s="1"/>
       <c r="L31" s="1"/>
@@ -3465,14 +3349,14 @@
     </row>
     <row r="32" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A32" s="19" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B32" s="4" t="s">
         <v>36</v>
       </c>
       <c r="C32" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>{&lt;}</v>
+        <v>{&lt;=}</v>
       </c>
       <c r="D32" s="4"/>
       <c r="E32" s="1"/>
@@ -3480,13 +3364,14 @@
         <v>31</v>
       </c>
       <c r="G32" s="34" t="s">
-        <v>90</v>
-      </c>
-      <c r="I32" s="9" t="s">
-        <v>68</v>
+        <v>81</v>
+      </c>
+      <c r="I32" s="9" t="str">
+        <f xml:space="preserve"> "- &lt;expr_id&gt;"</f>
+        <v>- &lt;expr_id&gt;</v>
       </c>
       <c r="J32" s="4" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="K32" s="1"/>
       <c r="L32" s="1"/>
@@ -3509,14 +3394,14 @@
     </row>
     <row r="33" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A33" s="19" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B33" s="4" t="s">
         <v>36</v>
       </c>
       <c r="C33" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>{&gt;}</v>
+        <v>{&gt;=}</v>
       </c>
       <c r="D33" s="4"/>
       <c r="E33" s="1"/>
@@ -3524,14 +3409,14 @@
         <v>32</v>
       </c>
       <c r="G33" s="34" t="s">
-        <v>91</v>
+        <v>81</v>
       </c>
       <c r="I33" s="9" t="str">
-        <f xml:space="preserve"> "+ &lt;expr_id&gt;"</f>
-        <v>+ &lt;expr_id&gt;</v>
+        <f xml:space="preserve"> "/ &lt;expr_id&gt;"</f>
+        <v>/ &lt;expr_id&gt;</v>
       </c>
       <c r="J33" s="4" t="s">
-        <v>111</v>
+        <v>100</v>
       </c>
       <c r="K33" s="1"/>
       <c r="L33" s="1"/>
@@ -3554,14 +3439,14 @@
     </row>
     <row r="34" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A34" s="19" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B34" s="4" t="s">
         <v>36</v>
       </c>
       <c r="C34" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>{&lt;=}</v>
+        <v>{(}</v>
       </c>
       <c r="D34" s="4"/>
       <c r="E34" s="1"/>
@@ -3569,14 +3454,14 @@
         <v>33</v>
       </c>
       <c r="G34" s="34" t="s">
-        <v>91</v>
+        <v>81</v>
       </c>
       <c r="I34" s="9" t="str">
-        <f xml:space="preserve"> "- &lt;expr_id&gt;"</f>
-        <v>- &lt;expr_id&gt;</v>
+        <f xml:space="preserve"> "* &lt;expr_id&gt;"</f>
+        <v>* &lt;expr_id&gt;</v>
       </c>
       <c r="J34" s="4" t="s">
-        <v>112</v>
+        <v>101</v>
       </c>
       <c r="K34" s="1"/>
       <c r="L34" s="1"/>
@@ -3599,14 +3484,14 @@
     </row>
     <row r="35" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A35" s="19" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B35" s="4" t="s">
         <v>36</v>
       </c>
       <c r="C35" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>{&gt;=}</v>
+        <v>{)}</v>
       </c>
       <c r="D35" s="4"/>
       <c r="E35" s="1"/>
@@ -3614,14 +3499,14 @@
         <v>34</v>
       </c>
       <c r="G35" s="34" t="s">
-        <v>91</v>
+        <v>81</v>
       </c>
       <c r="I35" s="9" t="str">
-        <f xml:space="preserve"> "/ &lt;expr_id&gt;"</f>
-        <v>/ &lt;expr_id&gt;</v>
+        <f xml:space="preserve"> "== &lt;expr_id&gt;"</f>
+        <v>== &lt;expr_id&gt;</v>
       </c>
       <c r="J35" s="4" t="s">
-        <v>113</v>
+        <v>102</v>
       </c>
       <c r="K35" s="1"/>
       <c r="L35" s="1"/>
@@ -3644,14 +3529,14 @@
     </row>
     <row r="36" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A36" s="19" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="B36" s="4" t="s">
         <v>36</v>
       </c>
       <c r="C36" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>{(}</v>
+        <v>{=}</v>
       </c>
       <c r="D36" s="4"/>
       <c r="E36" s="1"/>
@@ -3659,14 +3544,14 @@
         <v>35</v>
       </c>
       <c r="G36" s="34" t="s">
-        <v>91</v>
+        <v>81</v>
       </c>
       <c r="I36" s="9" t="str">
-        <f xml:space="preserve"> "* &lt;expr_id&gt;"</f>
-        <v>* &lt;expr_id&gt;</v>
+        <f xml:space="preserve"> "!= &lt;expr_id&gt;"</f>
+        <v>!= &lt;expr_id&gt;</v>
       </c>
       <c r="J36" s="4" t="s">
-        <v>114</v>
+        <v>103</v>
       </c>
       <c r="K36" s="1"/>
       <c r="L36" s="1"/>
@@ -3689,14 +3574,14 @@
     </row>
     <row r="37" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A37" s="19" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="B37" s="4" t="s">
         <v>36</v>
       </c>
       <c r="C37" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>{)}</v>
+        <v>{,}</v>
       </c>
       <c r="D37" s="4"/>
       <c r="E37" s="1"/>
@@ -3704,14 +3589,15 @@
         <v>36</v>
       </c>
       <c r="G37" s="34" t="s">
-        <v>91</v>
-      </c>
+        <v>81</v>
+      </c>
+      <c r="H37" s="8"/>
       <c r="I37" s="9" t="str">
-        <f xml:space="preserve"> "== &lt;expr_id&gt;"</f>
-        <v>== &lt;expr_id&gt;</v>
+        <f xml:space="preserve"> "&lt; &lt;expr_id&gt;"</f>
+        <v>&lt; &lt;expr_id&gt;</v>
       </c>
       <c r="J37" s="4" t="s">
-        <v>115</v>
+        <v>104</v>
       </c>
       <c r="K37" s="1"/>
       <c r="L37" s="1"/>
@@ -3734,14 +3620,14 @@
     </row>
     <row r="38" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A38" s="19" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B38" s="4" t="s">
         <v>36</v>
       </c>
       <c r="C38" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>{=}</v>
+        <v>{def}</v>
       </c>
       <c r="D38" s="4"/>
       <c r="E38" s="1"/>
@@ -3749,14 +3635,15 @@
         <v>37</v>
       </c>
       <c r="G38" s="34" t="s">
-        <v>91</v>
-      </c>
+        <v>81</v>
+      </c>
+      <c r="H38" s="8"/>
       <c r="I38" s="9" t="str">
-        <f xml:space="preserve"> "!= &lt;expr_id&gt;"</f>
-        <v>!= &lt;expr_id&gt;</v>
+        <f xml:space="preserve"> "&gt; &lt;expr_id&gt;"</f>
+        <v>&gt; &lt;expr_id&gt;</v>
       </c>
       <c r="J38" s="4" t="s">
-        <v>116</v>
+        <v>105</v>
       </c>
       <c r="K38" s="1"/>
       <c r="L38" s="1"/>
@@ -3779,14 +3666,14 @@
     </row>
     <row r="39" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A39" s="19" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B39" s="4" t="s">
         <v>36</v>
       </c>
       <c r="C39" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>{,}</v>
+        <v>{end}</v>
       </c>
       <c r="D39" s="4"/>
       <c r="E39" s="1"/>
@@ -3794,15 +3681,15 @@
         <v>38</v>
       </c>
       <c r="G39" s="34" t="s">
-        <v>91</v>
+        <v>81</v>
       </c>
       <c r="H39" s="8"/>
       <c r="I39" s="9" t="str">
-        <f xml:space="preserve"> "&lt; &lt;expr_id&gt;"</f>
-        <v>&lt; &lt;expr_id&gt;</v>
+        <f xml:space="preserve"> "&lt;= &lt;expr_id&gt;"</f>
+        <v>&lt;= &lt;expr_id&gt;</v>
       </c>
       <c r="J39" s="4" t="s">
-        <v>117</v>
+        <v>106</v>
       </c>
       <c r="K39" s="1"/>
       <c r="L39" s="1"/>
@@ -3825,14 +3712,14 @@
     </row>
     <row r="40" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A40" s="19" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="B40" s="4" t="s">
         <v>36</v>
       </c>
       <c r="C40" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>{def}</v>
+        <v>{if}</v>
       </c>
       <c r="D40" s="4"/>
       <c r="E40" s="1"/>
@@ -3840,15 +3727,15 @@
         <v>39</v>
       </c>
       <c r="G40" s="34" t="s">
-        <v>91</v>
+        <v>81</v>
       </c>
       <c r="H40" s="8"/>
       <c r="I40" s="9" t="str">
-        <f xml:space="preserve"> "&gt; &lt;expr_id&gt;"</f>
-        <v>&gt; &lt;expr_id&gt;</v>
+        <f xml:space="preserve"> "&gt;= &lt;expr_id&gt;"</f>
+        <v>&gt;= &lt;expr_id&gt;</v>
       </c>
       <c r="J40" s="4" t="s">
-        <v>118</v>
+        <v>107</v>
       </c>
       <c r="K40" s="1"/>
       <c r="L40" s="1"/>
@@ -3870,15 +3757,15 @@
       <c r="AB40" s="1"/>
     </row>
     <row r="41" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A41" s="19" t="s">
-        <v>28</v>
+      <c r="A41" s="20" t="s">
+        <v>31</v>
       </c>
       <c r="B41" s="4" t="s">
         <v>36</v>
       </c>
       <c r="C41" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>{end}</v>
+        <v>{then}</v>
       </c>
       <c r="D41" s="4"/>
       <c r="E41" s="1"/>
@@ -3886,15 +3773,14 @@
         <v>40</v>
       </c>
       <c r="G41" s="34" t="s">
-        <v>91</v>
-      </c>
-      <c r="H41" s="8"/>
-      <c r="I41" s="9" t="str">
-        <f xml:space="preserve"> "&lt;= &lt;expr_id&gt;"</f>
-        <v>&lt;= &lt;expr_id&gt;</v>
+        <v>81</v>
+      </c>
+      <c r="H41" s="6"/>
+      <c r="I41" s="13" t="s">
+        <v>51</v>
       </c>
       <c r="J41" s="4" t="s">
-        <v>119</v>
+        <v>87</v>
       </c>
       <c r="K41" s="1"/>
       <c r="L41" s="1"/>
@@ -3916,31 +3802,30 @@
       <c r="AB41" s="1"/>
     </row>
     <row r="42" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A42" s="19" t="s">
-        <v>32</v>
+      <c r="A42" s="20" t="s">
+        <v>33</v>
       </c>
       <c r="B42" s="4" t="s">
         <v>36</v>
       </c>
       <c r="C42" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>{if}</v>
+        <v>{else}</v>
       </c>
       <c r="D42" s="4"/>
       <c r="E42" s="5"/>
       <c r="F42" s="30">
         <v>41</v>
       </c>
-      <c r="G42" s="34" t="s">
-        <v>91</v>
-      </c>
-      <c r="H42" s="8"/>
-      <c r="I42" s="9" t="str">
-        <f xml:space="preserve"> "&gt;= &lt;expr_id&gt;"</f>
-        <v>&gt;= &lt;expr_id&gt;</v>
+      <c r="G42" s="25" t="s">
+        <v>111</v>
+      </c>
+      <c r="H42" s="6"/>
+      <c r="I42" s="13" t="s">
+        <v>68</v>
       </c>
       <c r="J42" s="4" t="s">
-        <v>120</v>
+        <v>92</v>
       </c>
       <c r="K42" s="1"/>
       <c r="L42" s="1"/>
@@ -3963,125 +3848,77 @@
     </row>
     <row r="43" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A43" s="20" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="B43" s="4" t="s">
         <v>36</v>
       </c>
       <c r="C43" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>{then}</v>
+        <v>{while}</v>
       </c>
       <c r="D43" s="4"/>
       <c r="F43" s="30">
         <v>42</v>
       </c>
-      <c r="G43" s="34" t="s">
-        <v>91</v>
+      <c r="G43" s="25" t="s">
+        <v>111</v>
       </c>
       <c r="H43" s="6"/>
       <c r="I43" s="13" t="s">
-        <v>51</v>
-      </c>
-      <c r="J43" s="4" t="s">
-        <v>100</v>
+        <v>113</v>
+      </c>
+      <c r="J43" s="24" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="44" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A44" s="20" t="s">
-        <v>33</v>
-      </c>
-      <c r="B44" s="4" t="s">
+      <c r="A44" s="27" t="s">
+        <v>35</v>
+      </c>
+      <c r="B44" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="C44" s="4" t="str">
+      <c r="C44" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>{else}</v>
-      </c>
-      <c r="D44" s="4"/>
+        <v>{do}</v>
+      </c>
+      <c r="D44" s="2"/>
       <c r="E44" s="13"/>
       <c r="F44" s="30">
         <v>43</v>
       </c>
       <c r="G44" s="25" t="s">
-        <v>125</v>
-      </c>
-      <c r="H44" s="6"/>
+        <v>112</v>
+      </c>
       <c r="I44" s="13" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="J44" s="4" t="s">
-        <v>105</v>
+        <v>93</v>
       </c>
     </row>
     <row r="45" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A45" s="20" t="s">
-        <v>34</v>
-      </c>
-      <c r="B45" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="C45" s="4" t="str">
-        <f t="shared" si="0"/>
-        <v>{while}</v>
-      </c>
-      <c r="D45" s="4"/>
       <c r="E45" s="13"/>
-      <c r="F45" s="30">
+      <c r="F45" s="32">
         <v>44</v>
       </c>
-      <c r="G45" s="25" t="s">
-        <v>125</v>
-      </c>
-      <c r="H45" s="6"/>
-      <c r="I45" s="13" t="s">
-        <v>127</v>
-      </c>
-      <c r="J45" s="24" t="s">
-        <v>39</v>
+      <c r="G45" s="51" t="s">
+        <v>112</v>
+      </c>
+      <c r="H45" s="35"/>
+      <c r="I45" s="38" t="s">
+        <v>2</v>
+      </c>
+      <c r="J45" s="2" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="46" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A46" s="27" t="s">
-        <v>35</v>
-      </c>
-      <c r="B46" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="C46" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>{do}</v>
-      </c>
-      <c r="D46" s="2"/>
-      <c r="E46" s="13"/>
-      <c r="F46" s="30">
-        <v>45</v>
-      </c>
-      <c r="G46" s="25" t="s">
-        <v>126</v>
-      </c>
-      <c r="I46" s="13" t="s">
-        <v>77</v>
-      </c>
-      <c r="J46" s="4" t="s">
-        <v>106</v>
-      </c>
+      <c r="E46" s="6"/>
     </row>
     <row r="47" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="E47" s="13"/>
-      <c r="F47" s="32">
-        <v>46</v>
-      </c>
-      <c r="G47" s="56" t="s">
-        <v>126</v>
-      </c>
-      <c r="H47" s="35"/>
-      <c r="I47" s="38" t="s">
-        <v>2</v>
-      </c>
-      <c r="J47" s="2" t="s">
-        <v>87</v>
-      </c>
+      <c r="E47" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>

<commit_message>
Upravená gramatika, přepsán podle ní parser, přesunutí testů, upravena LL tabulka
</commit_message>
<xml_diff>
--- a/doc/LL tabulka.xlsx
+++ b/doc/LL tabulka.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\OneDrive\VUT_FIT_BIT\IFJ\Projekt\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="307" documentId="6_{9A5E4322-B6A2-4F6C-9661-AD2FA57F2F31}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{1D85FAF0-2B37-4308-8B28-C7F86AAA8935}"/>
+  <xr:revisionPtr revIDLastSave="677" documentId="6_{9A5E4322-B6A2-4F6C-9661-AD2FA57F2F31}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{92E189F2-0B14-4D39-BA58-5D86189C9FB2}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12165" xr2:uid="{C362D381-7D2B-4872-B2C9-60D26B6B778F}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12165" activeTab="1" xr2:uid="{C362D381-7D2B-4872-B2C9-60D26B6B778F}"/>
   </bookViews>
   <sheets>
     <sheet name="LL tabulka prediktivní analýzy" sheetId="2" r:id="rId1"/>
@@ -24,6 +24,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="295" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="297" uniqueCount="122">
   <si>
     <t>&lt;prog&gt;</t>
   </si>
@@ -207,9 +208,6 @@
     <t>id &lt;params_n&gt;</t>
   </si>
   <si>
-    <t>, &lt;params&gt;</t>
-  </si>
-  <si>
     <t>if &lt;expr&gt; then EOL &lt;body&gt; else EOL &lt;body&gt; end</t>
   </si>
   <si>
@@ -261,15 +259,6 @@
     <t>&lt;type&gt;</t>
   </si>
   <si>
-    <t>{id, nil, integer, float, string}</t>
-  </si>
-  <si>
-    <t>{(, id, nil, integer, float, string}</t>
-  </si>
-  <si>
-    <t>{nil, integer, float, string}</t>
-  </si>
-  <si>
     <t>&lt;expr&gt;   -&gt;</t>
   </si>
   <si>
@@ -288,9 +277,6 @@
     <t>id &lt;expr_o&gt;</t>
   </si>
   <si>
-    <t>{=, (, id, nil, integer, float, string, +, -, /, *, ==, !=, &lt;, &gt;, &lt;=, &gt;=}</t>
-  </si>
-  <si>
     <t>{end, else, $}</t>
   </si>
   <si>
@@ -309,9 +295,6 @@
     <t>{string}</t>
   </si>
   <si>
-    <t>{nil, integer, float, string, not, (}</t>
-  </si>
-  <si>
     <t>{+, -, /, *, ==, !=, &lt;, &gt;, &lt;=, &gt;=}</t>
   </si>
   <si>
@@ -321,42 +304,6 @@
     <t>$</t>
   </si>
   <si>
-    <t>&lt;expr_id&gt;</t>
-  </si>
-  <si>
-    <t>{id, nil, integer, float, string, (, not}</t>
-  </si>
-  <si>
-    <t>{+}</t>
-  </si>
-  <si>
-    <t>{-}</t>
-  </si>
-  <si>
-    <t>{/}</t>
-  </si>
-  <si>
-    <t>{*}</t>
-  </si>
-  <si>
-    <t>{==}</t>
-  </si>
-  <si>
-    <t>{!=}</t>
-  </si>
-  <si>
-    <t>{&lt;}</t>
-  </si>
-  <si>
-    <t>{&gt;}</t>
-  </si>
-  <si>
-    <t>{&lt;=}</t>
-  </si>
-  <si>
-    <t>{&gt;=}</t>
-  </si>
-  <si>
     <t>( &lt;expr_id&gt; )</t>
   </si>
   <si>
@@ -378,9 +325,6 @@
     <t>&lt;def_var_id&gt;</t>
   </si>
   <si>
-    <t>{(, id, nil, integer, float, string, +, -, /, *, ==, !=, &lt;, &gt;, &lt;=, &gt;=}</t>
-  </si>
-  <si>
     <t>&lt;body&gt; &lt;prog&gt;</t>
   </si>
   <si>
@@ -399,20 +343,68 @@
     <t>EOL &lt;body&gt;</t>
   </si>
   <si>
-    <t>{id, if, while, nil, integer, float, string, not, (, EOL}</t>
-  </si>
-  <si>
-    <t>{def, id, if, while, EOF, nil, integer, float, string, not, (, EOL}</t>
-  </si>
-  <si>
     <t>&lt;def_func&gt; EOL &lt;prog&gt;</t>
+  </si>
+  <si>
+    <t>&lt;type_id&gt;   -&gt;</t>
+  </si>
+  <si>
+    <t>, &lt;type_id&gt; &lt;params_n&gt;</t>
+  </si>
+  <si>
+    <t>&lt;type_id&gt;</t>
+  </si>
+  <si>
+    <t>{,, $}</t>
+  </si>
+  <si>
+    <t>true</t>
+  </si>
+  <si>
+    <t>false</t>
+  </si>
+  <si>
+    <t>{=, (, id, nil, integer, float, string, true, false, +, -, /, *, ==, !=, &lt;, &gt;, &lt;=, &gt;=}</t>
+  </si>
+  <si>
+    <t>{nil, integer, float, string, true, false}</t>
+  </si>
+  <si>
+    <t>{id, nil, integer, float, string, true, false}</t>
+  </si>
+  <si>
+    <t>{(, id, nil, integer, float, string, true, false}</t>
+  </si>
+  <si>
+    <t>{(, id, nil, integer, float, string, true, false, +, -, /, *, ==, !=, &lt;, &gt;, &lt;=, &gt;=}</t>
+  </si>
+  <si>
+    <t>{true}</t>
+  </si>
+  <si>
+    <t>{false}</t>
+  </si>
+  <si>
+    <t>{nil, integer, float, string, true, false, not, +, -, (}</t>
+  </si>
+  <si>
+    <t>{nil, integer, float, string, true, false, not, +, - (}</t>
+  </si>
+  <si>
+    <t>{def, id, if, while, EOF, nil, integer, float, string, true, false not, +, -, (, EOL}</t>
+  </si>
+  <si>
+    <t>{id, if, while, nil, integer, float, string, true, false, not, +, -, (, EOL}</t>
+  </si>
+  <si>
+    <t>{id, nil, integer, float, string, true, false, (, not, +, -}</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -437,14 +429,6 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="238"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="238"/>
@@ -459,7 +443,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="14">
+  <borders count="15">
     <border>
       <left/>
       <right/>
@@ -616,11 +600,20 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="57">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -647,9 +640,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -660,7 +650,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -697,9 +687,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -707,7 +694,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
@@ -720,25 +706,15 @@
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
@@ -748,13 +724,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -769,6 +750,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1084,10 +1068,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AC8D7845-686F-4A38-8521-27846C315129}">
-  <dimension ref="A1:AE15"/>
+  <dimension ref="A1:AG14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M29" sqref="M29"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K24" sqref="K24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1095,684 +1079,737 @@
     <col min="1" max="1" width="14.7109375" customWidth="1"/>
     <col min="2" max="2" width="6.7109375" customWidth="1"/>
     <col min="3" max="15" width="6.7109375" style="1" customWidth="1"/>
-    <col min="16" max="31" width="6.7109375" customWidth="1"/>
+    <col min="16" max="33" width="6.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A1" s="18"/>
-      <c r="B1" s="22" t="s">
+    <row r="1" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A1" s="17"/>
+      <c r="B1" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="C1" s="22" t="s">
+      <c r="C1" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="D1" s="22" t="s">
+      <c r="D1" s="21" t="s">
         <v>9</v>
       </c>
-      <c r="E1" s="22" t="s">
+      <c r="E1" s="21" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1" s="21" t="s">
         <v>10</v>
       </c>
-      <c r="F1" s="22" t="s">
+      <c r="G1" s="21" t="s">
+        <v>108</v>
+      </c>
+      <c r="H1" s="27" t="s">
+        <v>109</v>
+      </c>
+      <c r="I1" s="21" t="s">
+        <v>14</v>
+      </c>
+      <c r="J1" s="21" t="s">
+        <v>13</v>
+      </c>
+      <c r="K1" s="21" t="s">
+        <v>12</v>
+      </c>
+      <c r="L1" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="M1" s="21" t="s">
+        <v>16</v>
+      </c>
+      <c r="N1" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="O1" s="21" t="s">
+        <v>18</v>
+      </c>
+      <c r="P1" s="36" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q1" s="21" t="s">
+        <v>20</v>
+      </c>
+      <c r="R1" s="21" t="s">
+        <v>21</v>
+      </c>
+      <c r="S1" s="21" t="s">
+        <v>22</v>
+      </c>
+      <c r="T1" s="21" t="s">
+        <v>23</v>
+      </c>
+      <c r="U1" s="21" t="s">
+        <v>24</v>
+      </c>
+      <c r="V1" s="21" t="s">
+        <v>25</v>
+      </c>
+      <c r="W1" s="21" t="s">
+        <v>26</v>
+      </c>
+      <c r="X1" s="21" t="s">
+        <v>29</v>
+      </c>
+      <c r="Y1" s="21" t="s">
+        <v>30</v>
+      </c>
+      <c r="Z1" s="21" t="s">
+        <v>27</v>
+      </c>
+      <c r="AA1" s="21" t="s">
+        <v>28</v>
+      </c>
+      <c r="AB1" s="21" t="s">
+        <v>32</v>
+      </c>
+      <c r="AC1" s="27" t="s">
+        <v>31</v>
+      </c>
+      <c r="AD1" s="27" t="s">
+        <v>33</v>
+      </c>
+      <c r="AE1" s="27" t="s">
+        <v>34</v>
+      </c>
+      <c r="AF1" s="27" t="s">
+        <v>35</v>
+      </c>
+      <c r="AG1" s="27" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="2" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A2" s="18" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="37">
+        <v>2</v>
+      </c>
+      <c r="C2" s="38">
+        <v>2</v>
+      </c>
+      <c r="D2" s="38">
+        <v>2</v>
+      </c>
+      <c r="E2" s="38">
+        <v>2</v>
+      </c>
+      <c r="F2" s="38">
+        <v>2</v>
+      </c>
+      <c r="G2" s="38">
+        <v>2</v>
+      </c>
+      <c r="H2" s="1">
+        <v>2</v>
+      </c>
+      <c r="I2" s="38">
+        <v>2</v>
+      </c>
+      <c r="J2" s="38">
+        <v>3</v>
+      </c>
+      <c r="K2" s="38">
+        <v>2</v>
+      </c>
+      <c r="L2" s="38">
+        <v>2</v>
+      </c>
+      <c r="M2" s="38">
+        <v>2</v>
+      </c>
+      <c r="N2" s="38"/>
+      <c r="O2" s="38"/>
+      <c r="P2" s="38"/>
+      <c r="Q2" s="38"/>
+      <c r="R2" s="38"/>
+      <c r="S2" s="38"/>
+      <c r="T2" s="38"/>
+      <c r="U2" s="38"/>
+      <c r="V2" s="38">
+        <v>2</v>
+      </c>
+      <c r="W2" s="38"/>
+      <c r="X2" s="38"/>
+      <c r="Y2" s="38"/>
+      <c r="Z2" s="38">
+        <v>1</v>
+      </c>
+      <c r="AA2" s="38"/>
+      <c r="AB2" s="38">
+        <v>2</v>
+      </c>
+      <c r="AC2" s="38"/>
+      <c r="AD2" s="38"/>
+      <c r="AE2" s="38">
+        <v>2</v>
+      </c>
+      <c r="AF2" s="45"/>
+      <c r="AG2" s="44"/>
+    </row>
+    <row r="3" spans="1:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="37">
+        <v>4</v>
+      </c>
+      <c r="C3" s="38">
+        <v>5</v>
+      </c>
+      <c r="D3" s="38">
+        <v>5</v>
+      </c>
+      <c r="E3" s="38">
+        <v>5</v>
+      </c>
+      <c r="F3" s="38">
+        <v>5</v>
+      </c>
+      <c r="G3" s="38">
+        <v>5</v>
+      </c>
+      <c r="H3" s="1">
+        <v>5</v>
+      </c>
+      <c r="I3" s="38">
+        <v>5</v>
+      </c>
+      <c r="J3" s="38"/>
+      <c r="K3" s="38">
+        <v>9</v>
+      </c>
+      <c r="L3" s="38">
+        <v>5</v>
+      </c>
+      <c r="M3" s="38">
+        <v>5</v>
+      </c>
+      <c r="N3" s="38"/>
+      <c r="O3" s="38"/>
+      <c r="P3" s="38"/>
+      <c r="Q3" s="38"/>
+      <c r="R3" s="38"/>
+      <c r="S3" s="38"/>
+      <c r="T3" s="38"/>
+      <c r="U3" s="38"/>
+      <c r="V3" s="38">
+        <v>5</v>
+      </c>
+      <c r="W3" s="38"/>
+      <c r="X3" s="38"/>
+      <c r="Y3" s="38"/>
+      <c r="Z3" s="38"/>
+      <c r="AA3" s="38">
+        <v>6</v>
+      </c>
+      <c r="AB3" s="38">
+        <v>7</v>
+      </c>
+      <c r="AC3" s="38"/>
+      <c r="AD3" s="38">
+        <v>6</v>
+      </c>
+      <c r="AE3" s="38">
+        <v>8</v>
+      </c>
+      <c r="AF3" s="38"/>
+      <c r="AG3" s="23">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A4" s="18" t="s">
+        <v>73</v>
+      </c>
+      <c r="B4" s="38">
+        <v>12</v>
+      </c>
+      <c r="C4" s="38">
+        <v>12</v>
+      </c>
+      <c r="D4" s="38">
+        <v>12</v>
+      </c>
+      <c r="E4" s="38">
+        <v>12</v>
+      </c>
+      <c r="F4" s="38">
+        <v>12</v>
+      </c>
+      <c r="G4" s="38">
+        <v>12</v>
+      </c>
+      <c r="I4" s="38"/>
+      <c r="J4" s="38"/>
+      <c r="K4" s="38">
+        <v>13</v>
+      </c>
+      <c r="L4" s="38">
+        <v>10</v>
+      </c>
+      <c r="M4" s="38">
+        <v>10</v>
+      </c>
+      <c r="N4" s="38">
+        <v>10</v>
+      </c>
+      <c r="O4" s="38">
+        <v>10</v>
+      </c>
+      <c r="P4" s="38">
+        <v>10</v>
+      </c>
+      <c r="Q4" s="38">
+        <v>10</v>
+      </c>
+      <c r="R4" s="38">
+        <v>10</v>
+      </c>
+      <c r="S4" s="38">
+        <v>10</v>
+      </c>
+      <c r="T4" s="38">
+        <v>10</v>
+      </c>
+      <c r="U4" s="38">
+        <v>10</v>
+      </c>
+      <c r="V4" s="38">
+        <v>12</v>
+      </c>
+      <c r="W4" s="38"/>
+      <c r="X4" s="38">
         <v>11</v>
       </c>
-      <c r="G1" s="22" t="s">
+      <c r="Y4" s="38"/>
+      <c r="Z4" s="38"/>
+      <c r="AA4" s="38"/>
+      <c r="AB4" s="38"/>
+      <c r="AC4" s="38"/>
+      <c r="AD4" s="38"/>
+      <c r="AE4" s="38"/>
+      <c r="AF4" s="38"/>
+      <c r="AG4" s="23"/>
+    </row>
+    <row r="5" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A5" s="18" t="s">
+        <v>74</v>
+      </c>
+      <c r="B5" s="37"/>
+      <c r="C5" s="38">
         <v>14</v>
       </c>
-      <c r="H1" s="22" t="s">
-        <v>13</v>
-      </c>
-      <c r="I1" s="22" t="s">
-        <v>12</v>
-      </c>
-      <c r="J1" s="22" t="s">
+      <c r="D5" s="38">
         <v>15</v>
       </c>
-      <c r="K1" s="22" t="s">
+      <c r="E5" s="38">
         <v>16</v>
       </c>
-      <c r="L1" s="22" t="s">
+      <c r="F5" s="38">
         <v>17</v>
       </c>
-      <c r="M1" s="22" t="s">
+      <c r="G5" s="38">
         <v>18</v>
       </c>
-      <c r="N1" s="41" t="s">
+      <c r="H5" s="1">
         <v>19</v>
       </c>
-      <c r="O1" s="22" t="s">
+      <c r="I5" s="38"/>
+      <c r="J5" s="38"/>
+      <c r="K5" s="38"/>
+      <c r="L5" s="38"/>
+      <c r="M5" s="38"/>
+      <c r="N5" s="38"/>
+      <c r="O5" s="38"/>
+      <c r="P5" s="38"/>
+      <c r="Q5" s="38"/>
+      <c r="R5" s="38"/>
+      <c r="S5" s="38"/>
+      <c r="T5" s="38"/>
+      <c r="U5" s="38"/>
+      <c r="V5" s="38"/>
+      <c r="W5" s="38"/>
+      <c r="X5" s="38"/>
+      <c r="Y5" s="38"/>
+      <c r="Z5" s="38"/>
+      <c r="AA5" s="38"/>
+      <c r="AB5" s="38"/>
+      <c r="AC5" s="38"/>
+      <c r="AD5" s="38"/>
+      <c r="AE5" s="38"/>
+      <c r="AF5" s="38"/>
+      <c r="AG5" s="23"/>
+    </row>
+    <row r="6" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A6" s="19" t="s">
+        <v>106</v>
+      </c>
+      <c r="B6" s="5">
+        <v>21</v>
+      </c>
+      <c r="C6" s="5">
         <v>20</v>
       </c>
-      <c r="P1" s="22" t="s">
-        <v>21</v>
-      </c>
-      <c r="Q1" s="22" t="s">
+      <c r="D6" s="5">
+        <v>20</v>
+      </c>
+      <c r="E6" s="5">
+        <v>20</v>
+      </c>
+      <c r="F6" s="5">
+        <v>20</v>
+      </c>
+      <c r="G6" s="5">
+        <v>20</v>
+      </c>
+      <c r="H6" s="1">
+        <v>20</v>
+      </c>
+      <c r="I6" s="5"/>
+      <c r="J6" s="5"/>
+      <c r="K6" s="5"/>
+      <c r="L6" s="5"/>
+      <c r="M6" s="5"/>
+      <c r="N6" s="5"/>
+      <c r="O6" s="5"/>
+      <c r="P6" s="5"/>
+      <c r="Q6" s="5"/>
+      <c r="R6" s="5"/>
+      <c r="S6" s="5"/>
+      <c r="T6" s="5"/>
+      <c r="U6" s="5"/>
+      <c r="V6" s="5"/>
+      <c r="W6" s="5"/>
+      <c r="X6" s="5"/>
+      <c r="Y6" s="5"/>
+      <c r="Z6" s="5"/>
+      <c r="AA6" s="5"/>
+      <c r="AB6" s="5"/>
+      <c r="AC6" s="5"/>
+      <c r="AD6" s="5"/>
+      <c r="AE6" s="5"/>
+      <c r="AF6" s="5"/>
+      <c r="AG6" s="23"/>
+    </row>
+    <row r="7" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A7" s="19" t="s">
+        <v>64</v>
+      </c>
+      <c r="B7" s="37"/>
+      <c r="C7" s="38"/>
+      <c r="D7" s="38"/>
+      <c r="E7" s="38"/>
+      <c r="F7" s="38"/>
+      <c r="G7" s="38"/>
+      <c r="I7" s="38"/>
+      <c r="J7" s="38"/>
+      <c r="K7" s="38"/>
+      <c r="L7" s="38"/>
+      <c r="M7" s="38"/>
+      <c r="N7" s="38"/>
+      <c r="O7" s="38"/>
+      <c r="P7" s="38"/>
+      <c r="Q7" s="38"/>
+      <c r="R7" s="38"/>
+      <c r="S7" s="38"/>
+      <c r="T7" s="38"/>
+      <c r="U7" s="38"/>
+      <c r="V7" s="38"/>
+      <c r="W7" s="38"/>
+      <c r="X7" s="38"/>
+      <c r="Y7" s="38"/>
+      <c r="Z7" s="38">
         <v>22</v>
       </c>
-      <c r="R1" s="22" t="s">
+      <c r="AA7" s="38"/>
+      <c r="AB7" s="38"/>
+      <c r="AC7" s="38"/>
+      <c r="AD7" s="38"/>
+      <c r="AE7" s="38"/>
+      <c r="AF7" s="38"/>
+      <c r="AG7" s="23"/>
+    </row>
+    <row r="8" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A8" s="18" t="s">
+        <v>2</v>
+      </c>
+      <c r="B8" s="38">
+        <v>24</v>
+      </c>
+      <c r="C8" s="38">
+        <v>24</v>
+      </c>
+      <c r="D8" s="38">
+        <v>24</v>
+      </c>
+      <c r="E8" s="38">
+        <v>24</v>
+      </c>
+      <c r="F8" s="38">
+        <v>24</v>
+      </c>
+      <c r="G8" s="38">
+        <v>24</v>
+      </c>
+      <c r="H8" s="38">
+        <v>24</v>
+      </c>
+      <c r="I8" s="38"/>
+      <c r="J8" s="38"/>
+      <c r="K8" s="38"/>
+      <c r="L8" s="38"/>
+      <c r="M8" s="38"/>
+      <c r="N8" s="38"/>
+      <c r="O8" s="38"/>
+      <c r="P8" s="38"/>
+      <c r="Q8" s="38"/>
+      <c r="R8" s="38"/>
+      <c r="S8" s="38"/>
+      <c r="T8" s="38"/>
+      <c r="U8" s="38"/>
+      <c r="V8" s="38">
         <v>23</v>
       </c>
-      <c r="S1" s="28" t="s">
-        <v>24</v>
-      </c>
-      <c r="T1" s="22" t="s">
+      <c r="W8" s="38"/>
+      <c r="X8" s="38"/>
+      <c r="Y8" s="38"/>
+      <c r="Z8" s="38"/>
+      <c r="AA8" s="38"/>
+      <c r="AB8" s="38"/>
+      <c r="AC8" s="38"/>
+      <c r="AD8" s="38"/>
+      <c r="AE8" s="38"/>
+      <c r="AF8" s="38"/>
+      <c r="AG8" s="23"/>
+    </row>
+    <row r="9" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A9" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="B9" s="37">
+        <v>27</v>
+      </c>
+      <c r="C9" s="38">
+        <v>26</v>
+      </c>
+      <c r="D9" s="38">
+        <v>26</v>
+      </c>
+      <c r="E9" s="38">
+        <v>26</v>
+      </c>
+      <c r="F9" s="38">
+        <v>26</v>
+      </c>
+      <c r="G9" s="38">
+        <v>26</v>
+      </c>
+      <c r="H9" s="1">
+        <v>26</v>
+      </c>
+      <c r="I9" s="38"/>
+      <c r="J9" s="38"/>
+      <c r="K9" s="38">
         <v>25</v>
       </c>
-      <c r="U1" s="22" t="s">
-        <v>26</v>
-      </c>
-      <c r="V1" s="22" t="s">
+      <c r="L9" s="38"/>
+      <c r="M9" s="38"/>
+      <c r="N9" s="38"/>
+      <c r="O9" s="38"/>
+      <c r="P9" s="38"/>
+      <c r="Q9" s="38"/>
+      <c r="R9" s="38"/>
+      <c r="S9" s="38"/>
+      <c r="T9" s="38"/>
+      <c r="U9" s="38"/>
+      <c r="V9" s="38"/>
+      <c r="W9" s="38">
+        <v>25</v>
+      </c>
+      <c r="X9" s="38"/>
+      <c r="Y9" s="38"/>
+      <c r="Z9" s="38"/>
+      <c r="AA9" s="38"/>
+      <c r="AB9" s="38"/>
+      <c r="AC9" s="38"/>
+      <c r="AD9" s="38"/>
+      <c r="AE9" s="38"/>
+      <c r="AF9" s="38"/>
+      <c r="AG9" s="23">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="10" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A10" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="B10" s="37"/>
+      <c r="C10" s="38"/>
+      <c r="D10" s="38"/>
+      <c r="E10" s="38"/>
+      <c r="F10" s="38"/>
+      <c r="G10" s="38"/>
+      <c r="I10" s="38"/>
+      <c r="J10" s="38"/>
+      <c r="K10" s="38">
+        <v>28</v>
+      </c>
+      <c r="L10" s="38"/>
+      <c r="M10" s="38"/>
+      <c r="N10" s="38"/>
+      <c r="O10" s="38"/>
+      <c r="P10" s="38"/>
+      <c r="Q10" s="38"/>
+      <c r="R10" s="38"/>
+      <c r="S10" s="38"/>
+      <c r="T10" s="38"/>
+      <c r="U10" s="38"/>
+      <c r="V10" s="38"/>
+      <c r="W10" s="38">
+        <v>28</v>
+      </c>
+      <c r="X10" s="38"/>
+      <c r="Y10" s="38">
         <v>29</v>
       </c>
-      <c r="W1" s="22" t="s">
+      <c r="Z10" s="38"/>
+      <c r="AA10" s="38"/>
+      <c r="AB10" s="38"/>
+      <c r="AC10" s="38"/>
+      <c r="AD10" s="38"/>
+      <c r="AE10" s="38"/>
+      <c r="AF10" s="38"/>
+      <c r="AG10" s="23">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="11" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A11" s="18" t="s">
+        <v>5</v>
+      </c>
+      <c r="B11" s="37"/>
+      <c r="C11" s="38"/>
+      <c r="D11" s="38"/>
+      <c r="E11" s="38"/>
+      <c r="F11" s="38"/>
+      <c r="G11" s="38"/>
+      <c r="I11" s="38"/>
+      <c r="J11" s="38"/>
+      <c r="K11" s="38"/>
+      <c r="L11" s="38"/>
+      <c r="M11" s="38"/>
+      <c r="N11" s="38"/>
+      <c r="O11" s="38"/>
+      <c r="P11" s="38"/>
+      <c r="Q11" s="38"/>
+      <c r="R11" s="38"/>
+      <c r="S11" s="38"/>
+      <c r="T11" s="38"/>
+      <c r="U11" s="38"/>
+      <c r="V11" s="38"/>
+      <c r="W11" s="38"/>
+      <c r="X11" s="38"/>
+      <c r="Y11" s="38"/>
+      <c r="Z11" s="38"/>
+      <c r="AA11" s="38"/>
+      <c r="AB11" s="38">
         <v>30</v>
       </c>
-      <c r="X1" s="22" t="s">
-        <v>27</v>
-      </c>
-      <c r="Y1" s="22" t="s">
-        <v>28</v>
-      </c>
-      <c r="Z1" s="22" t="s">
+      <c r="AC11" s="38"/>
+      <c r="AD11" s="38"/>
+      <c r="AE11" s="38"/>
+      <c r="AF11" s="38"/>
+      <c r="AG11" s="23"/>
+    </row>
+    <row r="12" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A12" s="18" t="s">
+        <v>6</v>
+      </c>
+      <c r="B12" s="37"/>
+      <c r="C12" s="38"/>
+      <c r="D12" s="38"/>
+      <c r="E12" s="38"/>
+      <c r="F12" s="38"/>
+      <c r="G12" s="38"/>
+      <c r="I12" s="38"/>
+      <c r="J12" s="38"/>
+      <c r="K12" s="38"/>
+      <c r="L12" s="38"/>
+      <c r="M12" s="38"/>
+      <c r="N12" s="38"/>
+      <c r="O12" s="38"/>
+      <c r="P12" s="38"/>
+      <c r="Q12" s="38"/>
+      <c r="R12" s="38"/>
+      <c r="S12" s="38"/>
+      <c r="T12" s="38"/>
+      <c r="U12" s="38"/>
+      <c r="V12" s="38"/>
+      <c r="W12" s="38"/>
+      <c r="X12" s="38"/>
+      <c r="Y12" s="38"/>
+      <c r="Z12" s="38"/>
+      <c r="AA12" s="38"/>
+      <c r="AB12" s="38"/>
+      <c r="AC12" s="38"/>
+      <c r="AD12" s="38"/>
+      <c r="AE12" s="38">
+        <v>31</v>
+      </c>
+      <c r="AF12" s="38"/>
+      <c r="AG12" s="23"/>
+    </row>
+    <row r="13" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A13" s="19" t="s">
+        <v>92</v>
+      </c>
+      <c r="B13" s="5">
+        <v>33</v>
+      </c>
+      <c r="C13" s="5">
         <v>32</v>
       </c>
-      <c r="AA1" s="29" t="s">
-        <v>31</v>
-      </c>
-      <c r="AB1" s="29" t="s">
-        <v>33</v>
-      </c>
-      <c r="AC1" s="29" t="s">
-        <v>34</v>
-      </c>
-      <c r="AD1" s="29" t="s">
-        <v>35</v>
-      </c>
-      <c r="AE1" s="39" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="2" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A2" s="19" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="42">
-        <v>2</v>
-      </c>
-      <c r="C2" s="43">
-        <v>2</v>
-      </c>
-      <c r="D2" s="43">
-        <v>2</v>
-      </c>
-      <c r="E2" s="43">
-        <v>2</v>
-      </c>
-      <c r="F2" s="43">
-        <v>2</v>
-      </c>
-      <c r="G2" s="43">
-        <v>2</v>
-      </c>
-      <c r="H2" s="43">
-        <v>3</v>
-      </c>
-      <c r="I2" s="43">
-        <v>2</v>
-      </c>
-      <c r="J2" s="43"/>
-      <c r="K2" s="43"/>
-      <c r="L2" s="43"/>
-      <c r="M2" s="43"/>
-      <c r="N2" s="43"/>
-      <c r="O2" s="43"/>
-      <c r="P2" s="43"/>
-      <c r="Q2" s="43"/>
-      <c r="R2" s="43"/>
-      <c r="S2" s="43"/>
-      <c r="T2" s="43">
-        <v>2</v>
-      </c>
-      <c r="U2" s="43"/>
-      <c r="V2" s="43"/>
-      <c r="W2" s="43"/>
-      <c r="X2" s="43">
-        <v>1</v>
-      </c>
-      <c r="Y2" s="43"/>
-      <c r="Z2" s="43">
-        <v>2</v>
-      </c>
-      <c r="AA2" s="43"/>
-      <c r="AB2" s="43"/>
-      <c r="AC2" s="43">
-        <v>2</v>
-      </c>
-      <c r="AD2" s="44"/>
-      <c r="AE2" s="45"/>
-    </row>
-    <row r="3" spans="1:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="19" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" s="42">
-        <v>4</v>
-      </c>
-      <c r="C3" s="43">
-        <v>5</v>
-      </c>
-      <c r="D3" s="43">
-        <v>5</v>
-      </c>
-      <c r="E3" s="43">
-        <v>5</v>
-      </c>
-      <c r="F3" s="43">
-        <v>5</v>
-      </c>
-      <c r="G3" s="43">
-        <v>5</v>
-      </c>
-      <c r="H3" s="43"/>
-      <c r="I3" s="43">
-        <v>9</v>
-      </c>
-      <c r="J3" s="43"/>
-      <c r="K3" s="43"/>
-      <c r="L3" s="43"/>
-      <c r="M3" s="43"/>
-      <c r="N3" s="43"/>
-      <c r="O3" s="43"/>
-      <c r="P3" s="43"/>
-      <c r="Q3" s="43"/>
-      <c r="R3" s="43"/>
-      <c r="S3" s="43"/>
-      <c r="T3" s="43">
-        <v>5</v>
-      </c>
-      <c r="U3" s="43"/>
-      <c r="V3" s="43"/>
-      <c r="W3" s="43"/>
-      <c r="X3" s="43"/>
-      <c r="Y3" s="43">
-        <v>6</v>
-      </c>
-      <c r="Z3" s="43">
-        <v>7</v>
-      </c>
-      <c r="AA3" s="43"/>
-      <c r="AB3" s="43">
-        <v>6</v>
-      </c>
-      <c r="AC3" s="43">
-        <v>8</v>
-      </c>
-      <c r="AD3" s="44"/>
-      <c r="AE3" s="45">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A4" s="19" t="s">
-        <v>74</v>
-      </c>
-      <c r="B4" s="42">
-        <v>12</v>
-      </c>
-      <c r="C4" s="43">
-        <v>12</v>
-      </c>
-      <c r="D4" s="43">
-        <v>12</v>
-      </c>
-      <c r="E4" s="43">
-        <v>12</v>
-      </c>
-      <c r="F4" s="43">
-        <v>12</v>
-      </c>
-      <c r="G4" s="43"/>
-      <c r="H4" s="43"/>
-      <c r="I4" s="43">
-        <v>13</v>
-      </c>
-      <c r="J4" s="43">
-        <v>10</v>
-      </c>
-      <c r="K4" s="43">
-        <v>10</v>
-      </c>
-      <c r="L4" s="43">
-        <v>10</v>
-      </c>
-      <c r="M4" s="43">
-        <v>10</v>
-      </c>
-      <c r="N4" s="43">
-        <v>10</v>
-      </c>
-      <c r="O4" s="43">
-        <v>10</v>
-      </c>
-      <c r="P4" s="43">
-        <v>10</v>
-      </c>
-      <c r="Q4" s="43">
-        <v>10</v>
-      </c>
-      <c r="R4" s="43">
-        <v>10</v>
-      </c>
-      <c r="S4" s="43">
-        <v>10</v>
-      </c>
-      <c r="T4" s="43">
-        <v>12</v>
-      </c>
-      <c r="U4" s="43"/>
-      <c r="V4" s="43">
-        <v>11</v>
-      </c>
-      <c r="W4" s="43"/>
-      <c r="X4" s="43"/>
-      <c r="Y4" s="43"/>
-      <c r="Z4" s="43"/>
-      <c r="AA4" s="43"/>
-      <c r="AB4" s="43"/>
-      <c r="AC4" s="43"/>
-      <c r="AD4" s="44"/>
-      <c r="AE4" s="45"/>
-    </row>
-    <row r="5" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A5" s="19" t="s">
-        <v>75</v>
-      </c>
-      <c r="B5" s="42"/>
-      <c r="C5" s="43">
-        <v>14</v>
-      </c>
-      <c r="D5" s="43">
-        <v>15</v>
-      </c>
-      <c r="E5" s="43">
-        <v>17</v>
-      </c>
-      <c r="F5" s="43">
-        <v>16</v>
-      </c>
-      <c r="G5" s="43"/>
-      <c r="H5" s="43"/>
-      <c r="I5" s="43"/>
-      <c r="J5" s="43"/>
-      <c r="K5" s="43"/>
-      <c r="L5" s="43"/>
-      <c r="M5" s="43"/>
-      <c r="N5" s="43"/>
-      <c r="O5" s="43"/>
-      <c r="P5" s="43"/>
-      <c r="Q5" s="43"/>
-      <c r="R5" s="43"/>
-      <c r="S5" s="43"/>
-      <c r="T5" s="43"/>
-      <c r="U5" s="43"/>
-      <c r="V5" s="43"/>
-      <c r="W5" s="43"/>
-      <c r="X5" s="43"/>
-      <c r="Y5" s="43"/>
-      <c r="Z5" s="43"/>
-      <c r="AA5" s="43"/>
-      <c r="AB5" s="43"/>
-      <c r="AC5" s="43"/>
-      <c r="AD5" s="44"/>
-      <c r="AE5" s="45"/>
-    </row>
-    <row r="6" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A6" s="20" t="s">
-        <v>65</v>
-      </c>
-      <c r="B6" s="42"/>
-      <c r="C6" s="43"/>
-      <c r="D6" s="43"/>
-      <c r="E6" s="43"/>
-      <c r="F6" s="43"/>
-      <c r="G6" s="43"/>
-      <c r="H6" s="43"/>
-      <c r="I6" s="43"/>
-      <c r="J6" s="43"/>
-      <c r="K6" s="43"/>
-      <c r="L6" s="43"/>
-      <c r="M6" s="43"/>
-      <c r="N6" s="43"/>
-      <c r="O6" s="43"/>
-      <c r="P6" s="43"/>
-      <c r="Q6" s="43"/>
-      <c r="R6" s="43"/>
-      <c r="S6" s="43"/>
-      <c r="T6" s="43"/>
-      <c r="U6" s="43"/>
-      <c r="V6" s="43"/>
-      <c r="W6" s="43"/>
-      <c r="X6" s="43">
-        <v>18</v>
-      </c>
-      <c r="Y6" s="43"/>
-      <c r="Z6" s="43"/>
-      <c r="AA6" s="43"/>
-      <c r="AB6" s="43"/>
-      <c r="AC6" s="43"/>
-      <c r="AD6" s="44"/>
-      <c r="AE6" s="45"/>
-    </row>
-    <row r="7" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A7" s="19" t="s">
-        <v>2</v>
-      </c>
-      <c r="B7" s="43">
-        <v>20</v>
-      </c>
-      <c r="C7" s="43">
-        <v>20</v>
-      </c>
-      <c r="D7" s="43">
-        <v>20</v>
-      </c>
-      <c r="E7" s="43">
-        <v>20</v>
-      </c>
-      <c r="F7" s="43">
-        <v>20</v>
-      </c>
-      <c r="G7" s="43"/>
-      <c r="H7" s="43"/>
-      <c r="I7" s="43"/>
-      <c r="J7" s="43"/>
-      <c r="K7" s="43"/>
-      <c r="L7" s="43"/>
-      <c r="M7" s="43"/>
-      <c r="N7" s="43"/>
-      <c r="O7" s="43"/>
-      <c r="P7" s="43"/>
-      <c r="Q7" s="43"/>
-      <c r="R7" s="43"/>
-      <c r="S7" s="43"/>
-      <c r="T7" s="43">
-        <v>19</v>
-      </c>
-      <c r="U7" s="43"/>
-      <c r="V7" s="43"/>
-      <c r="W7" s="43"/>
-      <c r="X7" s="43"/>
-      <c r="Y7" s="43"/>
-      <c r="Z7" s="43"/>
-      <c r="AA7" s="43"/>
-      <c r="AB7" s="43"/>
-      <c r="AC7" s="43"/>
-      <c r="AD7" s="44"/>
-      <c r="AE7" s="45"/>
-    </row>
-    <row r="8" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A8" s="19" t="s">
-        <v>3</v>
-      </c>
-      <c r="B8" s="42">
-        <v>23</v>
-      </c>
-      <c r="C8" s="43">
-        <v>22</v>
-      </c>
-      <c r="D8" s="43">
-        <v>22</v>
-      </c>
-      <c r="E8" s="43">
-        <v>22</v>
-      </c>
-      <c r="F8" s="43">
-        <v>22</v>
-      </c>
-      <c r="G8" s="43"/>
-      <c r="H8" s="43"/>
-      <c r="I8" s="43">
-        <v>24</v>
-      </c>
-      <c r="J8" s="43"/>
-      <c r="K8" s="43"/>
-      <c r="L8" s="43"/>
-      <c r="M8" s="43"/>
-      <c r="N8" s="43"/>
-      <c r="O8" s="43"/>
-      <c r="P8" s="43"/>
-      <c r="Q8" s="43"/>
-      <c r="R8" s="43"/>
-      <c r="S8" s="43"/>
-      <c r="T8" s="43"/>
-      <c r="U8" s="43">
-        <v>21</v>
-      </c>
-      <c r="V8" s="43"/>
-      <c r="W8" s="43"/>
-      <c r="X8" s="43"/>
-      <c r="Y8" s="43"/>
-      <c r="Z8" s="43"/>
-      <c r="AA8" s="43"/>
-      <c r="AB8" s="43"/>
-      <c r="AC8" s="43"/>
-      <c r="AD8" s="44"/>
-      <c r="AE8" s="45">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="9" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A9" s="19" t="s">
-        <v>4</v>
-      </c>
-      <c r="B9" s="42"/>
-      <c r="C9" s="43"/>
-      <c r="D9" s="43"/>
-      <c r="E9" s="43"/>
-      <c r="F9" s="43"/>
-      <c r="G9" s="43"/>
-      <c r="H9" s="43"/>
-      <c r="I9" s="43">
-        <v>24</v>
-      </c>
-      <c r="J9" s="43"/>
-      <c r="K9" s="43"/>
-      <c r="L9" s="43"/>
-      <c r="M9" s="43"/>
-      <c r="N9" s="43"/>
-      <c r="O9" s="43"/>
-      <c r="P9" s="43"/>
-      <c r="Q9" s="43"/>
-      <c r="R9" s="43"/>
-      <c r="S9" s="43"/>
-      <c r="T9" s="43"/>
-      <c r="U9" s="43">
-        <v>24</v>
-      </c>
-      <c r="V9" s="43"/>
-      <c r="W9" s="43">
-        <v>25</v>
-      </c>
-      <c r="X9" s="43"/>
-      <c r="Y9" s="43"/>
-      <c r="Z9" s="43"/>
-      <c r="AA9" s="43"/>
-      <c r="AB9" s="43"/>
-      <c r="AC9" s="43"/>
-      <c r="AD9" s="44"/>
-      <c r="AE9" s="45">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="10" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A10" s="19" t="s">
-        <v>5</v>
-      </c>
-      <c r="B10" s="42"/>
-      <c r="C10" s="43"/>
-      <c r="D10" s="43"/>
-      <c r="E10" s="43"/>
-      <c r="F10" s="43"/>
-      <c r="G10" s="43"/>
-      <c r="H10" s="43"/>
-      <c r="I10" s="43"/>
-      <c r="J10" s="43"/>
-      <c r="K10" s="43"/>
-      <c r="L10" s="43"/>
-      <c r="M10" s="43"/>
-      <c r="N10" s="43"/>
-      <c r="O10" s="43"/>
-      <c r="P10" s="43"/>
-      <c r="Q10" s="43"/>
-      <c r="R10" s="43"/>
-      <c r="S10" s="43"/>
-      <c r="T10" s="43"/>
-      <c r="U10" s="43"/>
-      <c r="V10" s="43"/>
-      <c r="W10" s="43"/>
-      <c r="X10" s="43"/>
-      <c r="Y10" s="43"/>
-      <c r="Z10" s="43">
-        <v>26</v>
-      </c>
-      <c r="AA10" s="43"/>
-      <c r="AB10" s="43"/>
-      <c r="AC10" s="43"/>
-      <c r="AD10" s="44"/>
-      <c r="AE10" s="45"/>
-    </row>
-    <row r="11" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A11" s="19" t="s">
-        <v>6</v>
-      </c>
-      <c r="B11" s="42"/>
-      <c r="C11" s="43"/>
-      <c r="D11" s="43"/>
-      <c r="E11" s="43"/>
-      <c r="F11" s="43"/>
-      <c r="G11" s="43"/>
-      <c r="H11" s="43"/>
-      <c r="I11" s="43"/>
-      <c r="J11" s="43"/>
-      <c r="K11" s="43"/>
-      <c r="L11" s="43"/>
-      <c r="M11" s="43"/>
-      <c r="N11" s="43"/>
-      <c r="O11" s="43"/>
-      <c r="P11" s="43"/>
-      <c r="Q11" s="43"/>
-      <c r="R11" s="43"/>
-      <c r="S11" s="43"/>
-      <c r="T11" s="43"/>
-      <c r="U11" s="43"/>
-      <c r="V11" s="43"/>
-      <c r="W11" s="43"/>
-      <c r="X11" s="43"/>
-      <c r="Y11" s="43"/>
-      <c r="Z11" s="43"/>
-      <c r="AA11" s="43"/>
-      <c r="AB11" s="43"/>
-      <c r="AC11" s="43">
-        <v>27</v>
-      </c>
-      <c r="AD11" s="49"/>
-      <c r="AE11" s="45"/>
-    </row>
-    <row r="12" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A12" s="20" t="s">
-        <v>96</v>
-      </c>
-      <c r="B12" s="5">
-        <v>28</v>
-      </c>
-      <c r="C12" s="5">
-        <v>29</v>
-      </c>
-      <c r="D12" s="5">
-        <v>29</v>
-      </c>
-      <c r="E12" s="5">
-        <v>29</v>
-      </c>
-      <c r="F12" s="5">
-        <v>29</v>
-      </c>
-      <c r="G12" s="5">
-        <v>29</v>
-      </c>
-      <c r="H12" s="5"/>
-      <c r="I12" s="5"/>
-      <c r="J12" s="5"/>
-      <c r="K12" s="5"/>
-      <c r="L12" s="5"/>
-      <c r="M12" s="5"/>
-      <c r="N12" s="5"/>
-      <c r="O12" s="40"/>
-      <c r="P12" s="5"/>
-      <c r="Q12" s="1"/>
-      <c r="R12" s="1"/>
-      <c r="S12" s="5"/>
-      <c r="T12" s="1">
-        <v>29</v>
-      </c>
-      <c r="U12" s="1"/>
-      <c r="V12" s="1"/>
-      <c r="W12" s="1"/>
-      <c r="X12" s="1"/>
-      <c r="Y12" s="1"/>
-      <c r="Z12" s="1"/>
-      <c r="AA12" s="1"/>
-      <c r="AB12" s="1"/>
-      <c r="AC12" s="1"/>
-      <c r="AD12" s="1"/>
-      <c r="AE12" s="24"/>
-    </row>
-    <row r="13" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A13" s="20" t="s">
-        <v>69</v>
-      </c>
-      <c r="B13" s="5"/>
-      <c r="C13" s="5"/>
-      <c r="D13" s="5"/>
-      <c r="E13" s="5"/>
-      <c r="F13" s="5"/>
-      <c r="G13" s="5"/>
-      <c r="H13" s="5"/>
+      <c r="D13" s="5">
+        <v>32</v>
+      </c>
+      <c r="E13" s="5">
+        <v>32</v>
+      </c>
+      <c r="F13" s="5">
+        <v>32</v>
+      </c>
+      <c r="G13" s="5">
+        <v>32</v>
+      </c>
+      <c r="H13" s="1">
+        <v>32</v>
+      </c>
       <c r="I13" s="5">
-        <v>40</v>
-      </c>
-      <c r="J13" s="5">
-        <v>30</v>
-      </c>
-      <c r="K13" s="5">
-        <v>31</v>
-      </c>
+        <v>32</v>
+      </c>
+      <c r="J13" s="5"/>
+      <c r="K13" s="5"/>
       <c r="L13" s="5">
         <v>32</v>
       </c>
       <c r="M13" s="5">
-        <v>33</v>
-      </c>
-      <c r="N13" s="5">
-        <v>34</v>
-      </c>
-      <c r="O13" s="5">
-        <v>35</v>
-      </c>
-      <c r="P13" s="5">
-        <v>36</v>
-      </c>
-      <c r="Q13" s="5">
-        <v>37</v>
-      </c>
-      <c r="R13" s="5">
-        <v>38</v>
-      </c>
-      <c r="S13" s="5">
-        <v>39</v>
-      </c>
+        <v>32</v>
+      </c>
+      <c r="N13" s="5"/>
+      <c r="O13" s="5"/>
+      <c r="P13" s="5"/>
+      <c r="Q13" s="5"/>
+      <c r="R13" s="5"/>
+      <c r="S13" s="5"/>
       <c r="T13" s="5"/>
       <c r="U13" s="5"/>
-      <c r="V13" s="5"/>
+      <c r="V13" s="5">
+        <v>32</v>
+      </c>
       <c r="W13" s="5"/>
       <c r="X13" s="5"/>
       <c r="Y13" s="5"/>
@@ -1781,113 +1818,82 @@
       <c r="AB13" s="5"/>
       <c r="AC13" s="5"/>
       <c r="AD13" s="5"/>
-      <c r="AE13" s="24">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="14" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A14" s="20" t="s">
-        <v>110</v>
-      </c>
-      <c r="B14" s="1">
-        <v>42</v>
-      </c>
-      <c r="C14" s="1">
-        <v>41</v>
-      </c>
-      <c r="D14" s="1">
-        <v>41</v>
-      </c>
-      <c r="E14" s="1">
-        <v>41</v>
-      </c>
-      <c r="F14" s="1">
-        <v>41</v>
-      </c>
-      <c r="G14" s="1">
-        <v>41</v>
-      </c>
-      <c r="T14" s="1">
-        <v>41</v>
-      </c>
-      <c r="U14" s="1"/>
-      <c r="V14" s="1"/>
-      <c r="W14" s="1"/>
-      <c r="X14" s="1"/>
-      <c r="Y14" s="1"/>
-      <c r="Z14" s="1"/>
-      <c r="AA14" s="1"/>
-      <c r="AB14" s="1"/>
-      <c r="AC14" s="1"/>
-      <c r="AD14" s="1"/>
-      <c r="AE14" s="24"/>
-    </row>
-    <row r="15" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A15" s="27" t="s">
-        <v>114</v>
-      </c>
-      <c r="B15" s="17">
-        <v>44</v>
-      </c>
-      <c r="C15" s="17">
-        <v>44</v>
-      </c>
-      <c r="D15" s="17">
-        <v>44</v>
-      </c>
-      <c r="E15" s="17">
-        <v>44</v>
-      </c>
-      <c r="F15" s="17">
-        <v>44</v>
-      </c>
-      <c r="G15" s="17"/>
-      <c r="H15" s="17"/>
-      <c r="I15" s="17"/>
-      <c r="J15" s="17">
-        <v>43</v>
-      </c>
-      <c r="K15" s="17">
-        <v>43</v>
-      </c>
-      <c r="L15" s="17">
-        <v>43</v>
-      </c>
-      <c r="M15" s="17">
-        <v>43</v>
-      </c>
-      <c r="N15" s="17">
-        <v>43</v>
-      </c>
-      <c r="O15" s="17">
-        <v>43</v>
-      </c>
-      <c r="P15" s="17">
-        <v>43</v>
-      </c>
-      <c r="Q15" s="17">
-        <v>43</v>
-      </c>
-      <c r="R15" s="17">
-        <v>43</v>
-      </c>
-      <c r="S15" s="17">
-        <v>43</v>
-      </c>
-      <c r="T15" s="17">
-        <v>44</v>
-      </c>
-      <c r="U15" s="17"/>
-      <c r="V15" s="17"/>
-      <c r="W15" s="17"/>
-      <c r="X15" s="17"/>
-      <c r="Y15" s="17"/>
-      <c r="Z15" s="17"/>
-      <c r="AA15" s="17"/>
-      <c r="AB15" s="17"/>
-      <c r="AC15" s="17"/>
-      <c r="AD15" s="17"/>
-      <c r="AE15" s="50"/>
+      <c r="AE13" s="5"/>
+      <c r="AF13" s="5"/>
+      <c r="AG13" s="23"/>
+    </row>
+    <row r="14" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A14" s="26" t="s">
+        <v>96</v>
+      </c>
+      <c r="B14" s="16">
+        <v>35</v>
+      </c>
+      <c r="C14" s="16">
+        <v>35</v>
+      </c>
+      <c r="D14" s="16">
+        <v>35</v>
+      </c>
+      <c r="E14" s="16">
+        <v>35</v>
+      </c>
+      <c r="F14" s="16">
+        <v>35</v>
+      </c>
+      <c r="G14" s="16">
+        <v>35</v>
+      </c>
+      <c r="H14" s="16">
+        <v>35</v>
+      </c>
+      <c r="I14" s="16"/>
+      <c r="J14" s="16"/>
+      <c r="K14" s="16"/>
+      <c r="L14" s="16">
+        <v>34</v>
+      </c>
+      <c r="M14" s="16">
+        <v>34</v>
+      </c>
+      <c r="N14" s="16">
+        <v>34</v>
+      </c>
+      <c r="O14" s="16">
+        <v>34</v>
+      </c>
+      <c r="P14" s="16">
+        <v>34</v>
+      </c>
+      <c r="Q14" s="16">
+        <v>34</v>
+      </c>
+      <c r="R14" s="16">
+        <v>34</v>
+      </c>
+      <c r="S14" s="16">
+        <v>34</v>
+      </c>
+      <c r="T14" s="16">
+        <v>34</v>
+      </c>
+      <c r="U14" s="16">
+        <v>34</v>
+      </c>
+      <c r="V14" s="16">
+        <v>35</v>
+      </c>
+      <c r="W14" s="16"/>
+      <c r="X14" s="16"/>
+      <c r="Y14" s="16"/>
+      <c r="Z14" s="16"/>
+      <c r="AA14" s="16"/>
+      <c r="AB14" s="16"/>
+      <c r="AC14" s="16"/>
+      <c r="AD14" s="16"/>
+      <c r="AE14" s="16"/>
+      <c r="AF14" s="16"/>
+      <c r="AG14" s="42"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
@@ -1899,21 +1905,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B9B981D-AC8B-4430-B1E8-C28C34350FA5}">
   <dimension ref="A1:AK47"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D36" sqref="D36"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14" customWidth="1"/>
     <col min="2" max="2" width="6" customWidth="1"/>
-    <col min="3" max="3" width="56" customWidth="1"/>
-    <col min="4" max="4" width="50.7109375" customWidth="1"/>
+    <col min="3" max="3" width="65.5703125" customWidth="1"/>
+    <col min="4" max="4" width="13.5703125" customWidth="1"/>
     <col min="5" max="6" width="3.42578125" customWidth="1"/>
     <col min="7" max="7" width="17.42578125" customWidth="1"/>
     <col min="8" max="8" width="2.140625" customWidth="1"/>
     <col min="9" max="9" width="43.42578125" customWidth="1"/>
-    <col min="10" max="10" width="51.140625" customWidth="1"/>
+    <col min="10" max="10" width="57.85546875" customWidth="1"/>
+    <col min="11" max="11" width="3.42578125" customWidth="1"/>
     <col min="12" max="12" width="3.5703125" customWidth="1"/>
     <col min="13" max="13" width="13.5703125" customWidth="1"/>
     <col min="14" max="14" width="2.42578125" customWidth="1"/>
@@ -1921,33 +1928,33 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A1" s="18"/>
-      <c r="B1" s="22" t="s">
+      <c r="A1" s="17"/>
+      <c r="B1" s="21" t="s">
         <v>37</v>
       </c>
-      <c r="C1" s="22" t="s">
+      <c r="C1" s="21" t="s">
         <v>41</v>
       </c>
-      <c r="D1" s="22" t="s">
+      <c r="D1" s="21" t="s">
         <v>46</v>
       </c>
       <c r="E1" s="6"/>
-      <c r="F1" s="18"/>
-      <c r="G1" s="52" t="s">
-        <v>61</v>
-      </c>
-      <c r="H1" s="52"/>
-      <c r="I1" s="53"/>
-      <c r="J1" s="29" t="s">
+      <c r="F1" s="17"/>
+      <c r="G1" s="46" t="s">
+        <v>60</v>
+      </c>
+      <c r="H1" s="46"/>
+      <c r="I1" s="47"/>
+      <c r="J1" s="27" t="s">
         <v>48</v>
       </c>
-      <c r="K1" s="33"/>
-      <c r="L1" s="18"/>
-      <c r="M1" s="54" t="s">
-        <v>82</v>
-      </c>
-      <c r="N1" s="55"/>
-      <c r="O1" s="56"/>
+      <c r="K1" s="30"/>
+      <c r="L1" s="17"/>
+      <c r="M1" s="48" t="s">
+        <v>78</v>
+      </c>
+      <c r="N1" s="49"/>
+      <c r="O1" s="50"/>
       <c r="P1" s="6"/>
       <c r="Q1" s="6"/>
       <c r="R1" s="6"/>
@@ -1963,42 +1970,42 @@
       <c r="AB1" s="6"/>
     </row>
     <row r="2" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A2" s="48" t="s">
+      <c r="A2" s="41" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>36</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>123</v>
-      </c>
-      <c r="D2" s="23" t="s">
-        <v>62</v>
+        <v>119</v>
+      </c>
+      <c r="D2" s="22" t="s">
+        <v>61</v>
       </c>
       <c r="E2" s="1"/>
-      <c r="F2" s="19">
+      <c r="F2" s="18">
         <v>1</v>
       </c>
       <c r="G2" s="7" t="s">
         <v>50</v>
       </c>
       <c r="H2" s="7"/>
-      <c r="I2" s="14" t="s">
-        <v>124</v>
-      </c>
-      <c r="J2" s="12" t="s">
+      <c r="I2" s="13" t="s">
+        <v>103</v>
+      </c>
+      <c r="J2" s="11" t="s">
         <v>42</v>
       </c>
       <c r="K2" s="5"/>
       <c r="L2" s="4">
         <v>1</v>
       </c>
-      <c r="M2" s="34" t="s">
-        <v>79</v>
+      <c r="M2" s="31" t="s">
+        <v>75</v>
       </c>
       <c r="N2" s="5"/>
       <c r="O2" s="9" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="P2" s="5"/>
       <c r="Q2" s="5"/>
@@ -2024,43 +2031,43 @@
       <c r="AK2" s="6"/>
     </row>
     <row r="3" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A3" s="19" t="s">
+      <c r="A3" s="18" t="s">
         <v>1</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>38</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>122</v>
-      </c>
-      <c r="D3" s="24" t="s">
-        <v>86</v>
+        <v>120</v>
+      </c>
+      <c r="D3" s="23" t="s">
+        <v>81</v>
       </c>
       <c r="E3" s="1"/>
-      <c r="F3" s="30">
+      <c r="F3" s="28">
         <v>2</v>
       </c>
       <c r="G3" s="7" t="s">
         <v>50</v>
       </c>
       <c r="H3" s="6"/>
-      <c r="I3" s="31" t="s">
-        <v>116</v>
+      <c r="I3" s="29" t="s">
+        <v>97</v>
       </c>
       <c r="J3" s="4" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="L3" s="4">
         <v>2</v>
       </c>
-      <c r="M3" s="34" t="s">
-        <v>79</v>
+      <c r="M3" s="31" t="s">
+        <v>75</v>
       </c>
       <c r="N3" s="5"/>
-      <c r="O3" s="9" t="s">
-        <v>109</v>
-      </c>
-      <c r="P3" s="1"/>
+      <c r="O3" s="51" t="s">
+        <v>91</v>
+      </c>
+      <c r="P3" s="33"/>
       <c r="Q3" s="1"/>
       <c r="R3" s="1"/>
       <c r="S3" s="1"/>
@@ -2075,43 +2082,43 @@
       <c r="AB3" s="1"/>
     </row>
     <row r="4" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A4" s="19" t="s">
-        <v>74</v>
+      <c r="A4" s="18" t="s">
+        <v>73</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>38</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>85</v>
+        <v>110</v>
       </c>
       <c r="D4" s="4" t="s">
         <v>47</v>
       </c>
       <c r="E4" s="1"/>
-      <c r="F4" s="19">
+      <c r="F4" s="18">
         <v>3</v>
       </c>
       <c r="G4" s="7" t="s">
         <v>50</v>
       </c>
       <c r="H4" s="6"/>
-      <c r="I4" s="13" t="s">
+      <c r="I4" s="12" t="s">
         <v>13</v>
       </c>
       <c r="J4" s="4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="L4" s="4">
         <v>3</v>
       </c>
-      <c r="M4" s="34" t="s">
-        <v>79</v>
-      </c>
-      <c r="N4" s="5"/>
-      <c r="O4" s="9" t="s">
-        <v>83</v>
-      </c>
-      <c r="P4" s="1"/>
+      <c r="M4" s="31" t="s">
+        <v>75</v>
+      </c>
+      <c r="O4" t="str">
+        <f>"+ &lt;expr_id&gt;"</f>
+        <v>+ &lt;expr_id&gt;</v>
+      </c>
+      <c r="P4" s="33"/>
       <c r="Q4" s="1"/>
       <c r="R4" s="1"/>
       <c r="S4" s="1"/>
@@ -2126,20 +2133,20 @@
       <c r="AB4" s="1"/>
     </row>
     <row r="5" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A5" s="19" t="s">
-        <v>75</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>38</v>
+      <c r="A5" s="18" t="s">
+        <v>74</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>36</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>78</v>
+        <v>111</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>43</v>
+        <v>107</v>
       </c>
       <c r="E5" s="1"/>
-      <c r="F5" s="30">
+      <c r="F5" s="28">
         <v>4</v>
       </c>
       <c r="G5" s="7" t="s">
@@ -2147,23 +2154,23 @@
       </c>
       <c r="H5" s="7"/>
       <c r="I5" s="9" t="s">
-        <v>119</v>
+        <v>100</v>
       </c>
       <c r="J5" s="4" t="s">
         <v>39</v>
       </c>
       <c r="K5" s="1"/>
-      <c r="L5" s="2">
+      <c r="L5" s="4">
         <v>4</v>
       </c>
-      <c r="M5" s="37" t="s">
-        <v>79</v>
-      </c>
-      <c r="N5" s="17"/>
-      <c r="O5" s="47" t="s">
-        <v>108</v>
-      </c>
-      <c r="P5" s="1"/>
+      <c r="M5" s="31" t="s">
+        <v>75</v>
+      </c>
+      <c r="O5" t="str">
+        <f>"- &lt;expr_id&gt;"</f>
+        <v>- &lt;expr_id&gt;</v>
+      </c>
+      <c r="P5" s="33"/>
       <c r="Q5" s="1"/>
       <c r="R5" s="1"/>
       <c r="S5" s="1"/>
@@ -2178,20 +2185,20 @@
       <c r="AB5" s="1"/>
     </row>
     <row r="6" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A6" s="20" t="s">
-        <v>65</v>
-      </c>
-      <c r="B6" s="16" t="s">
+      <c r="A6" s="19" t="s">
+        <v>106</v>
+      </c>
+      <c r="B6" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="C6" s="12" t="s">
-        <v>42</v>
+      <c r="C6" s="11" t="s">
+        <v>112</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>47</v>
+        <v>107</v>
       </c>
       <c r="E6" s="1"/>
-      <c r="F6" s="30">
+      <c r="F6" s="18">
         <v>5</v>
       </c>
       <c r="G6" s="7" t="s">
@@ -2199,17 +2206,23 @@
       </c>
       <c r="H6" s="7"/>
       <c r="I6" s="9" t="s">
-        <v>120</v>
+        <v>101</v>
       </c>
       <c r="J6" s="4" t="s">
-        <v>92</v>
-      </c>
-      <c r="K6" s="1"/>
-      <c r="L6" s="5"/>
-      <c r="M6" s="7"/>
+        <v>117</v>
+      </c>
+      <c r="K6" s="4"/>
+      <c r="L6" s="4">
+        <v>5</v>
+      </c>
+      <c r="M6" s="31" t="s">
+        <v>75</v>
+      </c>
       <c r="N6" s="5"/>
-      <c r="O6" s="10"/>
-      <c r="P6" s="1"/>
+      <c r="O6" s="9" t="s">
+        <v>79</v>
+      </c>
+      <c r="P6" s="33"/>
       <c r="Q6" s="1"/>
       <c r="R6" s="1"/>
       <c r="S6" s="1"/>
@@ -2225,36 +2238,42 @@
     </row>
     <row r="7" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A7" s="19" t="s">
-        <v>2</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>77</v>
+        <v>64</v>
+      </c>
+      <c r="B7" s="15" t="s">
+        <v>36</v>
+      </c>
+      <c r="C7" s="11" t="s">
+        <v>42</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>87</v>
+        <v>47</v>
       </c>
       <c r="E7" s="1"/>
-      <c r="F7" s="30">
+      <c r="F7" s="28">
         <v>6</v>
       </c>
       <c r="G7" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="I7" s="13" t="s">
+      <c r="I7" s="12" t="s">
         <v>51</v>
       </c>
-      <c r="J7" s="24" t="s">
-        <v>86</v>
-      </c>
-      <c r="K7" s="1"/>
-      <c r="L7" s="5"/>
-      <c r="M7" s="7"/>
+      <c r="J7" s="23" t="s">
+        <v>81</v>
+      </c>
+      <c r="K7" s="4"/>
+      <c r="L7" s="4">
+        <v>6</v>
+      </c>
+      <c r="M7" s="31" t="s">
+        <v>75</v>
+      </c>
       <c r="N7" s="5"/>
-      <c r="O7" s="10"/>
-      <c r="P7" s="1"/>
+      <c r="O7" s="9" t="s">
+        <v>90</v>
+      </c>
+      <c r="P7" s="33"/>
       <c r="Q7" s="1"/>
       <c r="R7" s="1"/>
       <c r="S7" s="1"/>
@@ -2269,37 +2288,43 @@
       <c r="AB7" s="1"/>
     </row>
     <row r="8" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A8" s="19" t="s">
-        <v>3</v>
+      <c r="A8" s="18" t="s">
+        <v>2</v>
       </c>
       <c r="B8" s="4" t="s">
         <v>38</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>76</v>
+        <v>113</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="E8" s="1"/>
-      <c r="F8" s="30">
+      <c r="F8" s="18">
         <v>7</v>
       </c>
       <c r="G8" s="7" t="s">
         <v>49</v>
       </c>
       <c r="I8" t="s">
-        <v>117</v>
+        <v>98</v>
       </c>
       <c r="J8" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="K8" s="1"/>
-      <c r="L8" s="5"/>
-      <c r="M8" s="7"/>
-      <c r="N8" s="5"/>
-      <c r="O8" s="10"/>
-      <c r="P8" s="1"/>
+      <c r="K8" s="4"/>
+      <c r="L8" s="4">
+        <v>7</v>
+      </c>
+      <c r="M8" s="31" t="s">
+        <v>77</v>
+      </c>
+      <c r="O8" s="9" t="str">
+        <f xml:space="preserve"> "+ &lt;expr_id&gt;"</f>
+        <v>+ &lt;expr_id&gt;</v>
+      </c>
+      <c r="P8" s="33"/>
       <c r="Q8" s="1"/>
       <c r="R8" s="1"/>
       <c r="S8" s="1"/>
@@ -2314,37 +2339,43 @@
       <c r="AB8" s="1"/>
     </row>
     <row r="9" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A9" s="19" t="s">
-        <v>4</v>
+      <c r="A9" s="18" t="s">
+        <v>3</v>
       </c>
       <c r="B9" s="4" t="s">
         <v>38</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>43</v>
+        <v>112</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="E9" s="1"/>
-      <c r="F9" s="30">
+      <c r="F9" s="28">
         <v>8</v>
       </c>
       <c r="G9" s="7" t="s">
         <v>49</v>
       </c>
       <c r="I9" t="s">
-        <v>118</v>
-      </c>
-      <c r="J9" s="15" t="s">
+        <v>99</v>
+      </c>
+      <c r="J9" s="14" t="s">
         <v>45</v>
       </c>
-      <c r="K9" s="1"/>
-      <c r="L9" s="5"/>
-      <c r="M9" s="7"/>
-      <c r="N9" s="5"/>
-      <c r="O9" s="10"/>
-      <c r="P9" s="1"/>
+      <c r="K9" s="4"/>
+      <c r="L9" s="4">
+        <v>8</v>
+      </c>
+      <c r="M9" s="31" t="s">
+        <v>77</v>
+      </c>
+      <c r="O9" s="9" t="str">
+        <f xml:space="preserve"> "- &lt;expr_id&gt;"</f>
+        <v>- &lt;expr_id&gt;</v>
+      </c>
+      <c r="P9" s="33"/>
       <c r="Q9" s="1"/>
       <c r="R9" s="1"/>
       <c r="S9" s="1"/>
@@ -2359,37 +2390,43 @@
       <c r="AB9" s="1"/>
     </row>
     <row r="10" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A10" s="19" t="s">
-        <v>5</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>36</v>
+      <c r="A10" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>38</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>47</v>
+        <v>83</v>
       </c>
       <c r="E10" s="1"/>
-      <c r="F10" s="30">
+      <c r="F10" s="18">
         <v>9</v>
       </c>
       <c r="G10" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="I10" s="13" t="s">
-        <v>121</v>
+      <c r="I10" s="12" t="s">
+        <v>102</v>
       </c>
       <c r="J10" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="K10" s="1"/>
-      <c r="L10" s="5"/>
-      <c r="M10" s="7"/>
-      <c r="N10" s="5"/>
-      <c r="O10" s="10"/>
-      <c r="P10" s="1"/>
+      <c r="K10" s="4"/>
+      <c r="L10" s="4">
+        <v>9</v>
+      </c>
+      <c r="M10" s="31" t="s">
+        <v>77</v>
+      </c>
+      <c r="O10" s="9" t="str">
+        <f xml:space="preserve"> "/ &lt;expr_id&gt;"</f>
+        <v>/ &lt;expr_id&gt;</v>
+      </c>
+      <c r="P10" s="33"/>
       <c r="Q10" s="1"/>
       <c r="R10" s="1"/>
       <c r="S10" s="1"/>
@@ -2404,37 +2441,43 @@
       <c r="AB10" s="1"/>
     </row>
     <row r="11" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A11" s="19" t="s">
-        <v>6</v>
+      <c r="A11" s="18" t="s">
+        <v>5</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>36</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="D11" s="24" t="s">
+        <v>44</v>
+      </c>
+      <c r="D11" s="4" t="s">
         <v>47</v>
       </c>
       <c r="E11" s="5"/>
-      <c r="F11" s="30">
+      <c r="F11" s="28">
         <v>10</v>
       </c>
       <c r="G11" s="7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="I11" s="9" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="J11" s="4" t="s">
-        <v>93</v>
-      </c>
-      <c r="K11" s="1"/>
-      <c r="L11" s="5"/>
-      <c r="M11" s="7"/>
-      <c r="N11" s="5"/>
-      <c r="O11" s="10"/>
-      <c r="P11" s="5"/>
+        <v>87</v>
+      </c>
+      <c r="K11" s="4"/>
+      <c r="L11" s="4">
+        <v>10</v>
+      </c>
+      <c r="M11" s="31" t="s">
+        <v>77</v>
+      </c>
+      <c r="O11" s="9" t="str">
+        <f xml:space="preserve"> "* &lt;expr_id&gt;"</f>
+        <v>* &lt;expr_id&gt;</v>
+      </c>
+      <c r="P11" s="33"/>
       <c r="Q11" s="5"/>
       <c r="R11" s="5"/>
       <c r="S11" s="5"/>
@@ -2449,38 +2492,45 @@
       <c r="AB11" s="5"/>
     </row>
     <row r="12" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A12" s="20" t="s">
-        <v>96</v>
+      <c r="A12" s="18" t="s">
+        <v>6</v>
       </c>
       <c r="B12" s="3" t="s">
         <v>36</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>97</v>
-      </c>
-      <c r="D12" s="4" t="s">
-        <v>87</v>
+        <v>45</v>
+      </c>
+      <c r="D12" s="23" t="s">
+        <v>47</v>
       </c>
       <c r="E12" s="5"/>
-      <c r="F12" s="30">
+      <c r="F12" s="18">
         <v>11</v>
       </c>
       <c r="G12" s="7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="H12" s="7"/>
-      <c r="I12" s="11" t="str">
+      <c r="I12" s="10" t="str">
         <f>"= &lt;defvar&gt;"</f>
         <v>= &lt;defvar&gt;</v>
       </c>
       <c r="J12" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="L12" s="5"/>
-      <c r="M12" s="7"/>
-      <c r="N12" s="5"/>
-      <c r="O12" s="10"/>
-      <c r="P12" s="1"/>
+        <v>88</v>
+      </c>
+      <c r="K12" s="28"/>
+      <c r="L12" s="4">
+        <v>11</v>
+      </c>
+      <c r="M12" s="31" t="s">
+        <v>77</v>
+      </c>
+      <c r="O12" s="9" t="str">
+        <f xml:space="preserve"> "== &lt;expr_id&gt;"</f>
+        <v>== &lt;expr_id&gt;</v>
+      </c>
+      <c r="P12" s="33"/>
       <c r="Q12" s="1"/>
       <c r="R12" s="1"/>
       <c r="S12" s="1"/>
@@ -2495,37 +2545,44 @@
       <c r="AB12" s="1"/>
     </row>
     <row r="13" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A13" s="20" t="s">
-        <v>69</v>
+      <c r="A13" s="18" t="s">
+        <v>92</v>
       </c>
       <c r="B13" s="3" t="s">
         <v>36</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>93</v>
+        <v>121</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="E13" s="1"/>
-      <c r="F13" s="30">
+      <c r="F13" s="28">
         <v>12</v>
       </c>
       <c r="G13" s="7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="H13" s="7"/>
       <c r="I13" s="9" t="s">
         <v>2</v>
       </c>
       <c r="J13" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="K13" s="28"/>
+      <c r="L13" s="4">
+        <v>12</v>
+      </c>
+      <c r="M13" s="31" t="s">
         <v>77</v>
       </c>
-      <c r="L13" s="5"/>
-      <c r="M13" s="7"/>
-      <c r="N13" s="5"/>
-      <c r="O13" s="10"/>
-      <c r="P13" s="1"/>
+      <c r="O13" s="9" t="str">
+        <f xml:space="preserve"> "!= &lt;expr_id&gt;"</f>
+        <v>!= &lt;expr_id&gt;</v>
+      </c>
+      <c r="P13" s="33"/>
       <c r="Q13" s="1"/>
       <c r="R13" s="1"/>
       <c r="S13" s="1"/>
@@ -2540,38 +2597,45 @@
       <c r="AB13" s="1"/>
     </row>
     <row r="14" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A14" s="19" t="s">
-        <v>110</v>
-      </c>
-      <c r="B14" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="C14" s="4" t="s">
-        <v>97</v>
-      </c>
-      <c r="D14" s="4" t="s">
-        <v>87</v>
+      <c r="A14" s="20" t="s">
+        <v>96</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>82</v>
       </c>
       <c r="E14" s="1"/>
-      <c r="F14" s="30">
+      <c r="F14" s="18">
         <v>13</v>
       </c>
       <c r="G14" s="7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="H14" s="7"/>
-      <c r="I14" s="13" t="s">
+      <c r="I14" s="12" t="s">
         <v>51</v>
       </c>
       <c r="J14" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="K14" s="5"/>
-      <c r="L14" s="5"/>
-      <c r="M14" s="7"/>
-      <c r="N14" s="5"/>
-      <c r="O14" s="10"/>
-      <c r="P14" s="1"/>
+      <c r="K14" s="4"/>
+      <c r="L14" s="4">
+        <v>13</v>
+      </c>
+      <c r="M14" s="31" t="s">
+        <v>77</v>
+      </c>
+      <c r="N14" s="8"/>
+      <c r="O14" s="9" t="str">
+        <f xml:space="preserve"> "&lt; &lt;expr_id&gt;"</f>
+        <v>&lt; &lt;expr_id&gt;</v>
+      </c>
+      <c r="P14" s="33"/>
       <c r="Q14" s="1"/>
       <c r="R14" s="1"/>
       <c r="S14" s="1"/>
@@ -2586,38 +2650,43 @@
       <c r="AB14" s="1"/>
     </row>
     <row r="15" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A15" s="21" t="s">
-        <v>114</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>87</v>
-      </c>
+      <c r="A15" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="D15" s="4"/>
       <c r="E15" s="1"/>
-      <c r="F15" s="30">
+      <c r="F15" s="28">
         <v>14</v>
       </c>
       <c r="G15" s="7" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="H15" s="6"/>
-      <c r="I15" s="11" t="s">
+      <c r="I15" s="10" t="s">
         <v>8</v>
       </c>
       <c r="J15" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="K15" s="1"/>
-      <c r="L15" s="5"/>
-      <c r="M15" s="7"/>
-      <c r="N15" s="5"/>
-      <c r="O15" s="10"/>
-      <c r="P15" s="1"/>
+      <c r="K15" s="4"/>
+      <c r="L15" s="4">
+        <v>14</v>
+      </c>
+      <c r="M15" s="31" t="s">
+        <v>77</v>
+      </c>
+      <c r="N15" s="8"/>
+      <c r="O15" s="9" t="str">
+        <f xml:space="preserve"> "&gt; &lt;expr_id&gt;"</f>
+        <v>&gt; &lt;expr_id&gt;</v>
+      </c>
+      <c r="P15" s="33"/>
       <c r="Q15" s="1"/>
       <c r="R15" s="1"/>
       <c r="S15" s="1"/>
@@ -2632,36 +2701,43 @@
       <c r="AB15" s="1"/>
     </row>
     <row r="16" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A16" s="19" t="s">
-        <v>7</v>
+      <c r="A16" s="18" t="s">
+        <v>8</v>
       </c>
       <c r="B16" s="4" t="s">
         <v>36</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D16" s="4"/>
       <c r="E16" s="1"/>
-      <c r="F16" s="30">
+      <c r="F16" s="18">
         <v>15</v>
       </c>
       <c r="G16" s="7" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="H16" s="6"/>
-      <c r="I16" s="13" t="s">
+      <c r="I16" s="12" t="s">
         <v>9</v>
       </c>
       <c r="J16" s="4" t="s">
-        <v>89</v>
-      </c>
-      <c r="K16" s="1"/>
-      <c r="L16" s="5"/>
-      <c r="M16" s="7"/>
-      <c r="N16" s="5"/>
-      <c r="O16" s="10"/>
-      <c r="P16" s="1"/>
+        <v>84</v>
+      </c>
+      <c r="K16" s="4"/>
+      <c r="L16" s="4">
+        <v>15</v>
+      </c>
+      <c r="M16" s="31" t="s">
+        <v>77</v>
+      </c>
+      <c r="N16" s="8"/>
+      <c r="O16" s="9" t="str">
+        <f xml:space="preserve"> "&lt;= &lt;expr_id&gt;"</f>
+        <v>&lt;= &lt;expr_id&gt;</v>
+      </c>
+      <c r="P16" s="33"/>
       <c r="Q16" s="1"/>
       <c r="R16" s="1"/>
       <c r="S16" s="1"/>
@@ -2676,36 +2752,44 @@
       <c r="AB16" s="1"/>
     </row>
     <row r="17" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A17" s="19" t="s">
-        <v>8</v>
+      <c r="A17" s="18" t="s">
+        <v>9</v>
       </c>
       <c r="B17" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="C17" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="D17" s="4"/>
+      <c r="C17" s="4" t="str">
+        <f t="shared" ref="C17:C45" si="0">"{"&amp;A17&amp;"}"</f>
+        <v>{integer}</v>
+      </c>
+      <c r="D17" s="11"/>
       <c r="E17" s="1"/>
-      <c r="F17" s="30">
+      <c r="F17" s="28">
         <v>16</v>
       </c>
       <c r="G17" s="7" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="H17" s="6"/>
-      <c r="I17" s="11" t="s">
+      <c r="I17" s="10" t="s">
         <v>11</v>
       </c>
       <c r="J17" s="4" t="s">
-        <v>90</v>
-      </c>
-      <c r="K17" s="1"/>
-      <c r="L17" s="5"/>
-      <c r="M17" s="7"/>
-      <c r="N17" s="5"/>
-      <c r="O17" s="10"/>
-      <c r="P17" s="1"/>
+        <v>85</v>
+      </c>
+      <c r="K17" s="4"/>
+      <c r="L17" s="4">
+        <v>16</v>
+      </c>
+      <c r="M17" s="31" t="s">
+        <v>77</v>
+      </c>
+      <c r="N17" s="8"/>
+      <c r="O17" s="9" t="str">
+        <f xml:space="preserve"> "&gt;= &lt;expr_id&gt;"</f>
+        <v>&gt;= &lt;expr_id&gt;</v>
+      </c>
+      <c r="P17" s="5"/>
       <c r="Q17" s="1"/>
       <c r="R17" s="1"/>
       <c r="S17" s="1"/>
@@ -2720,36 +2804,42 @@
       <c r="AB17" s="1"/>
     </row>
     <row r="18" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A18" s="19" t="s">
-        <v>9</v>
+      <c r="A18" s="18" t="s">
+        <v>11</v>
       </c>
       <c r="B18" s="4" t="s">
         <v>36</v>
       </c>
       <c r="C18" s="4" t="str">
-        <f>"{"&amp;A18&amp;"}"</f>
-        <v>{integer}</v>
-      </c>
-      <c r="D18" s="12"/>
+        <f t="shared" si="0"/>
+        <v>{float}</v>
+      </c>
+      <c r="D18" s="4"/>
       <c r="E18" s="1"/>
-      <c r="F18" s="30">
+      <c r="F18" s="18">
         <v>17</v>
       </c>
       <c r="G18" s="7" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="H18" s="6"/>
       <c r="I18" s="9" t="s">
         <v>10</v>
       </c>
       <c r="J18" s="4" t="s">
-        <v>91</v>
-      </c>
-      <c r="K18" s="1"/>
-      <c r="L18" s="5"/>
-      <c r="M18" s="7"/>
-      <c r="N18" s="5"/>
-      <c r="O18" s="6"/>
+        <v>86</v>
+      </c>
+      <c r="K18" s="4"/>
+      <c r="L18" s="4">
+        <v>17</v>
+      </c>
+      <c r="M18" s="31" t="s">
+        <v>77</v>
+      </c>
+      <c r="N18" s="6"/>
+      <c r="O18" s="12" t="s">
+        <v>51</v>
+      </c>
       <c r="P18" s="1"/>
       <c r="Q18" s="1"/>
       <c r="R18" s="1"/>
@@ -2765,37 +2855,41 @@
       <c r="AB18" s="1"/>
     </row>
     <row r="19" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A19" s="19" t="s">
+      <c r="A19" s="18" t="s">
         <v>10</v>
       </c>
       <c r="B19" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="C19" s="4" t="str">
-        <f t="shared" ref="C19:C44" si="0">"{"&amp;A19&amp;"}"</f>
+      <c r="C19" s="23" t="str">
+        <f t="shared" si="0"/>
         <v>{string}</v>
       </c>
       <c r="D19" s="4"/>
       <c r="E19" s="1"/>
-      <c r="F19" s="30">
+      <c r="F19" s="28">
         <v>18</v>
       </c>
-      <c r="G19" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="H19" s="7"/>
-      <c r="I19" s="9" t="s">
-        <v>72</v>
-      </c>
-      <c r="J19" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="K19" s="36"/>
-      <c r="L19" s="5"/>
-      <c r="M19" s="7"/>
-      <c r="N19" s="5"/>
-      <c r="O19" s="5"/>
-      <c r="P19" s="1"/>
+      <c r="G19" s="39" t="s">
+        <v>70</v>
+      </c>
+      <c r="I19" s="10" t="s">
+        <v>108</v>
+      </c>
+      <c r="J19" s="11" t="s">
+        <v>115</v>
+      </c>
+      <c r="K19" s="33"/>
+      <c r="L19" s="4">
+        <v>18</v>
+      </c>
+      <c r="M19" s="31" t="s">
+        <v>76</v>
+      </c>
+      <c r="O19" s="9" t="s">
+        <v>80</v>
+      </c>
+      <c r="P19" s="5"/>
       <c r="Q19" s="1"/>
       <c r="R19" s="1"/>
       <c r="S19" s="1"/>
@@ -2811,35 +2905,40 @@
     </row>
     <row r="20" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A20" s="19" t="s">
-        <v>11</v>
+        <v>108</v>
       </c>
       <c r="B20" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="C20" s="4" t="str">
+      <c r="C20" s="23" t="str">
         <f t="shared" si="0"/>
-        <v>{float}</v>
-      </c>
-      <c r="D20" s="4"/>
+        <v>{true}</v>
+      </c>
+      <c r="D20" s="28"/>
       <c r="E20" s="1"/>
-      <c r="F20" s="30">
+      <c r="F20" s="18">
         <v>19</v>
       </c>
-      <c r="G20" s="7" t="s">
-        <v>52</v>
-      </c>
-      <c r="H20" s="7"/>
-      <c r="I20" s="9" t="s">
-        <v>64</v>
-      </c>
-      <c r="J20" s="4" t="s">
+      <c r="G20" s="39" t="s">
+        <v>70</v>
+      </c>
+      <c r="I20" s="10" t="s">
+        <v>109</v>
+      </c>
+      <c r="J20" s="11" t="s">
+        <v>116</v>
+      </c>
+      <c r="K20" s="33"/>
+      <c r="L20" s="2">
+        <v>19</v>
+      </c>
+      <c r="M20" s="34" t="s">
+        <v>76</v>
+      </c>
+      <c r="N20" s="32"/>
+      <c r="O20" s="40" t="s">
         <v>67</v>
       </c>
-      <c r="K20" s="36"/>
-      <c r="L20" s="5"/>
-      <c r="M20" s="7"/>
-      <c r="N20" s="5"/>
-      <c r="O20" s="5"/>
       <c r="P20" s="1"/>
       <c r="Q20" s="1"/>
       <c r="R20" s="1"/>
@@ -2856,31 +2955,30 @@
     </row>
     <row r="21" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A21" s="19" t="s">
-        <v>14</v>
+        <v>109</v>
       </c>
       <c r="B21" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="C21" s="4" t="str">
+      <c r="C21" s="23" t="str">
         <f t="shared" si="0"/>
-        <v>{not}</v>
-      </c>
-      <c r="D21" s="4"/>
+        <v>{false}</v>
+      </c>
+      <c r="D21" s="28"/>
       <c r="E21" s="1"/>
-      <c r="F21" s="30">
+      <c r="F21" s="28">
         <v>20</v>
       </c>
-      <c r="G21" s="7" t="s">
-        <v>52</v>
-      </c>
-      <c r="H21" s="7"/>
-      <c r="I21" s="9" t="s">
-        <v>3</v>
+      <c r="G21" s="39" t="s">
+        <v>104</v>
+      </c>
+      <c r="I21" s="10" t="s">
+        <v>74</v>
       </c>
       <c r="J21" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="K21" s="36"/>
+        <v>111</v>
+      </c>
+      <c r="K21" s="33"/>
       <c r="L21" s="5"/>
       <c r="M21" s="7"/>
       <c r="N21" s="5"/>
@@ -2900,32 +2998,31 @@
       <c r="AB21" s="1"/>
     </row>
     <row r="22" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A22" s="19" t="s">
-        <v>13</v>
+      <c r="A22" s="18" t="s">
+        <v>14</v>
       </c>
       <c r="B22" s="4" t="s">
         <v>36</v>
       </c>
       <c r="C22" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>{EOF}</v>
-      </c>
-      <c r="D22" s="4"/>
+        <v>{not}</v>
+      </c>
+      <c r="D22" s="23"/>
       <c r="E22" s="1"/>
-      <c r="F22" s="30">
+      <c r="F22" s="18">
         <v>21</v>
       </c>
-      <c r="G22" s="7" t="s">
-        <v>53</v>
-      </c>
-      <c r="H22" s="7"/>
-      <c r="I22" s="9" t="s">
-        <v>51</v>
-      </c>
-      <c r="J22" s="4" t="s">
-        <v>88</v>
-      </c>
-      <c r="K22" s="36"/>
+      <c r="G22" s="39" t="s">
+        <v>104</v>
+      </c>
+      <c r="I22" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="J22" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="K22" s="33"/>
       <c r="L22" s="5"/>
       <c r="M22" s="7"/>
       <c r="N22" s="5"/>
@@ -2945,32 +3042,32 @@
       <c r="AB22" s="1"/>
     </row>
     <row r="23" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A23" s="19" t="s">
-        <v>12</v>
+      <c r="A23" s="18" t="s">
+        <v>13</v>
       </c>
       <c r="B23" s="4" t="s">
         <v>36</v>
       </c>
       <c r="C23" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>{EOL}</v>
+        <v>{EOF}</v>
       </c>
       <c r="D23" s="4"/>
       <c r="E23" s="1"/>
-      <c r="F23" s="30">
+      <c r="F23" s="28">
         <v>22</v>
       </c>
       <c r="G23" s="7" t="s">
-        <v>53</v>
+        <v>62</v>
       </c>
       <c r="H23" s="7"/>
       <c r="I23" s="9" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="J23" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="K23" s="36"/>
+        <v>42</v>
+      </c>
+      <c r="K23" s="33"/>
       <c r="L23" s="5"/>
       <c r="M23" s="7"/>
       <c r="N23" s="5"/>
@@ -2990,32 +3087,32 @@
       <c r="AB23" s="1"/>
     </row>
     <row r="24" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A24" s="19" t="s">
-        <v>15</v>
+      <c r="A24" s="18" t="s">
+        <v>12</v>
       </c>
       <c r="B24" s="4" t="s">
         <v>36</v>
       </c>
       <c r="C24" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>{+}</v>
+        <v>{EOL}</v>
       </c>
       <c r="D24" s="4"/>
       <c r="E24" s="1"/>
-      <c r="F24" s="30">
+      <c r="F24" s="18">
         <v>23</v>
       </c>
       <c r="G24" s="7" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="H24" s="7"/>
       <c r="I24" s="9" t="s">
-        <v>57</v>
+        <v>63</v>
       </c>
       <c r="J24" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="K24" s="36"/>
+        <v>66</v>
+      </c>
+      <c r="K24" s="33"/>
       <c r="L24" s="5"/>
       <c r="M24" s="7"/>
       <c r="N24" s="5"/>
@@ -3035,32 +3132,32 @@
       <c r="AB24" s="1"/>
     </row>
     <row r="25" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A25" s="19" t="s">
-        <v>16</v>
+      <c r="A25" s="18" t="s">
+        <v>15</v>
       </c>
       <c r="B25" s="4" t="s">
         <v>36</v>
       </c>
       <c r="C25" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>{-}</v>
+        <v>{+}</v>
       </c>
       <c r="D25" s="4"/>
       <c r="E25" s="1"/>
-      <c r="F25" s="30">
+      <c r="F25" s="28">
         <v>24</v>
       </c>
       <c r="G25" s="7" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="H25" s="7"/>
       <c r="I25" s="9" t="s">
-        <v>51</v>
+        <v>3</v>
       </c>
       <c r="J25" s="4" t="s">
-        <v>88</v>
-      </c>
-      <c r="K25" s="36"/>
+        <v>112</v>
+      </c>
+      <c r="K25" s="33"/>
       <c r="L25" s="5"/>
       <c r="M25" s="7"/>
       <c r="N25" s="5"/>
@@ -3080,32 +3177,32 @@
       <c r="AB25" s="1"/>
     </row>
     <row r="26" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A26" s="19" t="s">
-        <v>17</v>
+      <c r="A26" s="18" t="s">
+        <v>16</v>
       </c>
       <c r="B26" s="4" t="s">
         <v>36</v>
       </c>
       <c r="C26" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>{*}</v>
+        <v>{-}</v>
       </c>
       <c r="D26" s="4"/>
       <c r="E26" s="1"/>
-      <c r="F26" s="30">
+      <c r="F26" s="18">
         <v>25</v>
       </c>
       <c r="G26" s="7" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="H26" s="7"/>
       <c r="I26" s="9" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
       <c r="J26" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="K26" s="36"/>
+        <v>83</v>
+      </c>
+      <c r="K26" s="33"/>
       <c r="L26" s="5"/>
       <c r="M26" s="7"/>
       <c r="N26" s="5"/>
@@ -3125,32 +3222,32 @@
       <c r="AB26" s="1"/>
     </row>
     <row r="27" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A27" s="19" t="s">
-        <v>18</v>
+      <c r="A27" s="18" t="s">
+        <v>17</v>
       </c>
       <c r="B27" s="4" t="s">
         <v>36</v>
       </c>
       <c r="C27" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>{/}</v>
+        <v>{*}</v>
       </c>
       <c r="D27" s="4"/>
       <c r="E27" s="1"/>
-      <c r="F27" s="30">
+      <c r="F27" s="28">
         <v>26</v>
       </c>
-      <c r="G27" s="34" t="s">
-        <v>55</v>
+      <c r="G27" s="7" t="s">
+        <v>53</v>
       </c>
       <c r="H27" s="7"/>
       <c r="I27" s="9" t="s">
-        <v>59</v>
+        <v>72</v>
       </c>
       <c r="J27" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="K27" s="36"/>
+        <v>111</v>
+      </c>
+      <c r="K27" s="33"/>
       <c r="L27" s="5"/>
       <c r="M27" s="7"/>
       <c r="N27" s="5"/>
@@ -3170,32 +3267,32 @@
       <c r="AB27" s="1"/>
     </row>
     <row r="28" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A28" s="26" t="s">
-        <v>19</v>
+      <c r="A28" s="18" t="s">
+        <v>18</v>
       </c>
       <c r="B28" s="4" t="s">
         <v>36</v>
       </c>
       <c r="C28" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>{==}</v>
+        <v>{/}</v>
       </c>
       <c r="D28" s="4"/>
       <c r="E28" s="1"/>
-      <c r="F28" s="30">
+      <c r="F28" s="18">
         <v>27</v>
       </c>
-      <c r="G28" s="46" t="s">
-        <v>56</v>
-      </c>
-      <c r="H28" s="6"/>
-      <c r="I28" s="11" t="s">
-        <v>60</v>
+      <c r="G28" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="H28" s="7"/>
+      <c r="I28" s="9" t="s">
+        <v>57</v>
       </c>
       <c r="J28" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="K28" s="36"/>
+        <v>39</v>
+      </c>
+      <c r="K28" s="33"/>
       <c r="L28" s="5"/>
       <c r="M28" s="7"/>
       <c r="N28" s="5"/>
@@ -3215,31 +3312,32 @@
       <c r="AB28" s="1"/>
     </row>
     <row r="29" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A29" s="19" t="s">
-        <v>20</v>
+      <c r="A29" s="25" t="s">
+        <v>19</v>
       </c>
       <c r="B29" s="4" t="s">
         <v>36</v>
       </c>
       <c r="C29" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>{!=}</v>
+        <v>{==}</v>
       </c>
       <c r="D29" s="4"/>
       <c r="E29" s="1"/>
-      <c r="F29" s="30">
+      <c r="F29" s="28">
         <v>28</v>
       </c>
-      <c r="G29" s="34" t="s">
-        <v>80</v>
-      </c>
+      <c r="G29" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="H29" s="7"/>
       <c r="I29" s="9" t="s">
-        <v>84</v>
+        <v>51</v>
       </c>
       <c r="J29" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="K29" s="36"/>
+        <v>83</v>
+      </c>
+      <c r="K29" s="33"/>
       <c r="L29" s="5"/>
       <c r="M29" s="7"/>
       <c r="N29" s="5"/>
@@ -3259,31 +3357,32 @@
       <c r="AB29" s="1"/>
     </row>
     <row r="30" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A30" s="19" t="s">
-        <v>21</v>
+      <c r="A30" s="18" t="s">
+        <v>20</v>
       </c>
       <c r="B30" s="4" t="s">
         <v>36</v>
       </c>
       <c r="C30" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>{&lt;}</v>
+        <v>{!=}</v>
       </c>
       <c r="D30" s="4"/>
       <c r="E30" s="1"/>
-      <c r="F30" s="30">
+      <c r="F30" s="18">
         <v>29</v>
       </c>
-      <c r="G30" s="34" t="s">
-        <v>80</v>
-      </c>
+      <c r="G30" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="H30" s="7"/>
       <c r="I30" s="9" t="s">
-        <v>68</v>
+        <v>105</v>
       </c>
       <c r="J30" s="4" t="s">
-        <v>92</v>
-      </c>
-      <c r="K30" s="36"/>
+        <v>43</v>
+      </c>
+      <c r="K30" s="33"/>
       <c r="L30" s="5"/>
       <c r="M30" s="7"/>
       <c r="N30" s="5"/>
@@ -3303,30 +3402,30 @@
       <c r="AB30" s="1"/>
     </row>
     <row r="31" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A31" s="19" t="s">
-        <v>22</v>
+      <c r="A31" s="18" t="s">
+        <v>21</v>
       </c>
       <c r="B31" s="4" t="s">
         <v>36</v>
       </c>
       <c r="C31" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>{&gt;}</v>
+        <v>{&lt;}</v>
       </c>
       <c r="D31" s="4"/>
       <c r="E31" s="1"/>
-      <c r="F31" s="30">
+      <c r="F31" s="28">
         <v>30</v>
       </c>
-      <c r="G31" s="34" t="s">
-        <v>81</v>
-      </c>
-      <c r="I31" s="9" t="str">
-        <f xml:space="preserve"> "+ &lt;expr_id&gt;"</f>
-        <v>+ &lt;expr_id&gt;</v>
+      <c r="G31" s="31" t="s">
+        <v>55</v>
+      </c>
+      <c r="H31" s="7"/>
+      <c r="I31" s="9" t="s">
+        <v>58</v>
       </c>
       <c r="J31" s="4" t="s">
-        <v>98</v>
+        <v>44</v>
       </c>
       <c r="K31" s="1"/>
       <c r="L31" s="1"/>
@@ -3348,30 +3447,30 @@
       <c r="AB31" s="1"/>
     </row>
     <row r="32" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A32" s="19" t="s">
-        <v>23</v>
+      <c r="A32" s="18" t="s">
+        <v>22</v>
       </c>
       <c r="B32" s="4" t="s">
         <v>36</v>
       </c>
       <c r="C32" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>{&lt;=}</v>
+        <v>{&gt;}</v>
       </c>
       <c r="D32" s="4"/>
       <c r="E32" s="1"/>
-      <c r="F32" s="30">
+      <c r="F32" s="18">
         <v>31</v>
       </c>
-      <c r="G32" s="34" t="s">
-        <v>81</v>
-      </c>
-      <c r="I32" s="9" t="str">
-        <f xml:space="preserve"> "- &lt;expr_id&gt;"</f>
-        <v>- &lt;expr_id&gt;</v>
+      <c r="G32" s="39" t="s">
+        <v>56</v>
+      </c>
+      <c r="H32" s="6"/>
+      <c r="I32" s="10" t="s">
+        <v>59</v>
       </c>
       <c r="J32" s="4" t="s">
-        <v>99</v>
+        <v>45</v>
       </c>
       <c r="K32" s="1"/>
       <c r="L32" s="1"/>
@@ -3393,30 +3492,30 @@
       <c r="AB32" s="1"/>
     </row>
     <row r="33" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A33" s="19" t="s">
-        <v>24</v>
+      <c r="A33" s="18" t="s">
+        <v>23</v>
       </c>
       <c r="B33" s="4" t="s">
         <v>36</v>
       </c>
       <c r="C33" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>{&gt;=}</v>
+        <v>{&lt;=}</v>
       </c>
       <c r="D33" s="4"/>
       <c r="E33" s="1"/>
-      <c r="F33" s="30">
+      <c r="F33" s="28">
         <v>32</v>
       </c>
-      <c r="G33" s="34" t="s">
-        <v>81</v>
-      </c>
-      <c r="I33" s="9" t="str">
-        <f xml:space="preserve"> "/ &lt;expr_id&gt;"</f>
-        <v>/ &lt;expr_id&gt;</v>
+      <c r="G33" s="24" t="s">
+        <v>93</v>
+      </c>
+      <c r="H33" s="6"/>
+      <c r="I33" s="12" t="s">
+        <v>67</v>
       </c>
       <c r="J33" s="4" t="s">
-        <v>100</v>
+        <v>118</v>
       </c>
       <c r="K33" s="1"/>
       <c r="L33" s="1"/>
@@ -3438,30 +3537,30 @@
       <c r="AB33" s="1"/>
     </row>
     <row r="34" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A34" s="19" t="s">
-        <v>25</v>
+      <c r="A34" s="18" t="s">
+        <v>24</v>
       </c>
       <c r="B34" s="4" t="s">
         <v>36</v>
       </c>
       <c r="C34" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>{(}</v>
+        <v>{&gt;=}</v>
       </c>
       <c r="D34" s="4"/>
       <c r="E34" s="1"/>
-      <c r="F34" s="30">
+      <c r="F34" s="18">
         <v>33</v>
       </c>
-      <c r="G34" s="34" t="s">
-        <v>81</v>
-      </c>
-      <c r="I34" s="9" t="str">
-        <f xml:space="preserve"> "* &lt;expr_id&gt;"</f>
-        <v>* &lt;expr_id&gt;</v>
-      </c>
-      <c r="J34" s="4" t="s">
-        <v>101</v>
+      <c r="G34" s="24" t="s">
+        <v>93</v>
+      </c>
+      <c r="H34" s="6"/>
+      <c r="I34" s="12" t="s">
+        <v>95</v>
+      </c>
+      <c r="J34" s="23" t="s">
+        <v>39</v>
       </c>
       <c r="K34" s="1"/>
       <c r="L34" s="1"/>
@@ -3483,30 +3582,29 @@
       <c r="AB34" s="1"/>
     </row>
     <row r="35" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A35" s="19" t="s">
-        <v>26</v>
+      <c r="A35" s="18" t="s">
+        <v>25</v>
       </c>
       <c r="B35" s="4" t="s">
         <v>36</v>
       </c>
       <c r="C35" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>{)}</v>
+        <v>{(}</v>
       </c>
       <c r="D35" s="4"/>
       <c r="E35" s="1"/>
-      <c r="F35" s="30">
+      <c r="F35" s="28">
         <v>34</v>
       </c>
-      <c r="G35" s="34" t="s">
-        <v>81</v>
-      </c>
-      <c r="I35" s="9" t="str">
-        <f xml:space="preserve"> "== &lt;expr_id&gt;"</f>
-        <v>== &lt;expr_id&gt;</v>
+      <c r="G35" s="24" t="s">
+        <v>94</v>
+      </c>
+      <c r="I35" s="12" t="s">
+        <v>68</v>
       </c>
       <c r="J35" s="4" t="s">
-        <v>102</v>
+        <v>87</v>
       </c>
       <c r="K35" s="1"/>
       <c r="L35" s="1"/>
@@ -3528,30 +3626,30 @@
       <c r="AB35" s="1"/>
     </row>
     <row r="36" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A36" s="19" t="s">
-        <v>29</v>
+      <c r="A36" s="18" t="s">
+        <v>26</v>
       </c>
       <c r="B36" s="4" t="s">
         <v>36</v>
       </c>
       <c r="C36" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>{=}</v>
+        <v>{)}</v>
       </c>
       <c r="D36" s="4"/>
       <c r="E36" s="1"/>
-      <c r="F36" s="30">
+      <c r="F36" s="20">
         <v>35</v>
       </c>
-      <c r="G36" s="34" t="s">
-        <v>81</v>
-      </c>
-      <c r="I36" s="9" t="str">
-        <f xml:space="preserve"> "!= &lt;expr_id&gt;"</f>
-        <v>!= &lt;expr_id&gt;</v>
-      </c>
-      <c r="J36" s="4" t="s">
-        <v>103</v>
+      <c r="G36" s="43" t="s">
+        <v>94</v>
+      </c>
+      <c r="H36" s="32"/>
+      <c r="I36" s="35" t="s">
+        <v>2</v>
+      </c>
+      <c r="J36" s="2" t="s">
+        <v>113</v>
       </c>
       <c r="K36" s="1"/>
       <c r="L36" s="1"/>
@@ -3573,32 +3671,20 @@
       <c r="AB36" s="1"/>
     </row>
     <row r="37" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A37" s="19" t="s">
-        <v>30</v>
+      <c r="A37" s="18" t="s">
+        <v>29</v>
       </c>
       <c r="B37" s="4" t="s">
         <v>36</v>
       </c>
       <c r="C37" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>{,}</v>
+        <v>{=}</v>
       </c>
       <c r="D37" s="4"/>
       <c r="E37" s="1"/>
-      <c r="F37" s="30">
-        <v>36</v>
-      </c>
-      <c r="G37" s="34" t="s">
-        <v>81</v>
-      </c>
-      <c r="H37" s="8"/>
-      <c r="I37" s="9" t="str">
-        <f xml:space="preserve"> "&lt; &lt;expr_id&gt;"</f>
-        <v>&lt; &lt;expr_id&gt;</v>
-      </c>
-      <c r="J37" s="4" t="s">
-        <v>104</v>
-      </c>
+      <c r="F37" s="6"/>
+      <c r="G37" s="6"/>
       <c r="K37" s="1"/>
       <c r="L37" s="1"/>
       <c r="M37" s="1"/>
@@ -3619,32 +3705,20 @@
       <c r="AB37" s="1"/>
     </row>
     <row r="38" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A38" s="19" t="s">
-        <v>27</v>
+      <c r="A38" s="18" t="s">
+        <v>30</v>
       </c>
       <c r="B38" s="4" t="s">
         <v>36</v>
       </c>
       <c r="C38" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>{def}</v>
+        <v>{,}</v>
       </c>
       <c r="D38" s="4"/>
       <c r="E38" s="1"/>
-      <c r="F38" s="30">
-        <v>37</v>
-      </c>
-      <c r="G38" s="34" t="s">
-        <v>81</v>
-      </c>
-      <c r="H38" s="8"/>
-      <c r="I38" s="9" t="str">
-        <f xml:space="preserve"> "&gt; &lt;expr_id&gt;"</f>
-        <v>&gt; &lt;expr_id&gt;</v>
-      </c>
-      <c r="J38" s="4" t="s">
-        <v>105</v>
-      </c>
+      <c r="F38" s="6"/>
+      <c r="G38" s="6"/>
       <c r="K38" s="1"/>
       <c r="L38" s="1"/>
       <c r="M38" s="1"/>
@@ -3665,32 +3739,20 @@
       <c r="AB38" s="1"/>
     </row>
     <row r="39" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A39" s="19" t="s">
-        <v>28</v>
+      <c r="A39" s="18" t="s">
+        <v>27</v>
       </c>
       <c r="B39" s="4" t="s">
         <v>36</v>
       </c>
       <c r="C39" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>{end}</v>
+        <v>{def}</v>
       </c>
       <c r="D39" s="4"/>
       <c r="E39" s="1"/>
-      <c r="F39" s="30">
-        <v>38</v>
-      </c>
-      <c r="G39" s="34" t="s">
-        <v>81</v>
-      </c>
-      <c r="H39" s="8"/>
-      <c r="I39" s="9" t="str">
-        <f xml:space="preserve"> "&lt;= &lt;expr_id&gt;"</f>
-        <v>&lt;= &lt;expr_id&gt;</v>
-      </c>
-      <c r="J39" s="4" t="s">
-        <v>106</v>
-      </c>
+      <c r="F39" s="6"/>
+      <c r="G39" s="6"/>
       <c r="K39" s="1"/>
       <c r="L39" s="1"/>
       <c r="M39" s="1"/>
@@ -3711,32 +3773,20 @@
       <c r="AB39" s="1"/>
     </row>
     <row r="40" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A40" s="19" t="s">
-        <v>32</v>
+      <c r="A40" s="18" t="s">
+        <v>28</v>
       </c>
       <c r="B40" s="4" t="s">
         <v>36</v>
       </c>
       <c r="C40" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>{if}</v>
+        <v>{end}</v>
       </c>
       <c r="D40" s="4"/>
       <c r="E40" s="1"/>
-      <c r="F40" s="30">
-        <v>39</v>
-      </c>
-      <c r="G40" s="34" t="s">
-        <v>81</v>
-      </c>
-      <c r="H40" s="8"/>
-      <c r="I40" s="9" t="str">
-        <f xml:space="preserve"> "&gt;= &lt;expr_id&gt;"</f>
-        <v>&gt;= &lt;expr_id&gt;</v>
-      </c>
-      <c r="J40" s="4" t="s">
-        <v>107</v>
-      </c>
+      <c r="F40" s="6"/>
+      <c r="G40" s="6"/>
       <c r="K40" s="1"/>
       <c r="L40" s="1"/>
       <c r="M40" s="1"/>
@@ -3757,31 +3807,20 @@
       <c r="AB40" s="1"/>
     </row>
     <row r="41" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A41" s="20" t="s">
-        <v>31</v>
+      <c r="A41" s="18" t="s">
+        <v>32</v>
       </c>
       <c r="B41" s="4" t="s">
         <v>36</v>
       </c>
       <c r="C41" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>{then}</v>
+        <v>{if}</v>
       </c>
       <c r="D41" s="4"/>
       <c r="E41" s="1"/>
-      <c r="F41" s="30">
-        <v>40</v>
-      </c>
-      <c r="G41" s="34" t="s">
-        <v>81</v>
-      </c>
-      <c r="H41" s="6"/>
-      <c r="I41" s="13" t="s">
-        <v>51</v>
-      </c>
-      <c r="J41" s="4" t="s">
-        <v>87</v>
-      </c>
+      <c r="F41" s="6"/>
+      <c r="G41" s="6"/>
       <c r="K41" s="1"/>
       <c r="L41" s="1"/>
       <c r="M41" s="1"/>
@@ -3802,31 +3841,20 @@
       <c r="AB41" s="1"/>
     </row>
     <row r="42" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A42" s="20" t="s">
-        <v>33</v>
+      <c r="A42" s="19" t="s">
+        <v>31</v>
       </c>
       <c r="B42" s="4" t="s">
         <v>36</v>
       </c>
       <c r="C42" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>{else}</v>
+        <v>{then}</v>
       </c>
       <c r="D42" s="4"/>
       <c r="E42" s="5"/>
-      <c r="F42" s="30">
-        <v>41</v>
-      </c>
-      <c r="G42" s="25" t="s">
-        <v>111</v>
-      </c>
-      <c r="H42" s="6"/>
-      <c r="I42" s="13" t="s">
-        <v>68</v>
-      </c>
-      <c r="J42" s="4" t="s">
-        <v>92</v>
-      </c>
+      <c r="F42" s="6"/>
+      <c r="G42" s="6"/>
       <c r="K42" s="1"/>
       <c r="L42" s="1"/>
       <c r="M42" s="1"/>
@@ -3847,78 +3875,61 @@
       <c r="AB42" s="1"/>
     </row>
     <row r="43" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A43" s="20" t="s">
-        <v>34</v>
+      <c r="A43" s="19" t="s">
+        <v>33</v>
       </c>
       <c r="B43" s="4" t="s">
         <v>36</v>
       </c>
       <c r="C43" s="4" t="str">
         <f t="shared" si="0"/>
+        <v>{else}</v>
+      </c>
+      <c r="D43" s="4"/>
+      <c r="F43" s="6"/>
+      <c r="G43" s="6"/>
+    </row>
+    <row r="44" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A44" s="19" t="s">
+        <v>34</v>
+      </c>
+      <c r="B44" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C44" s="4" t="str">
+        <f t="shared" si="0"/>
         <v>{while}</v>
       </c>
-      <c r="D43" s="4"/>
-      <c r="F43" s="30">
-        <v>42</v>
-      </c>
-      <c r="G43" s="25" t="s">
-        <v>111</v>
-      </c>
-      <c r="H43" s="6"/>
-      <c r="I43" s="13" t="s">
-        <v>113</v>
-      </c>
-      <c r="J43" s="24" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="44" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A44" s="27" t="s">
+      <c r="D44" s="4"/>
+      <c r="E44" s="6"/>
+      <c r="F44" s="6"/>
+      <c r="G44" s="6"/>
+    </row>
+    <row r="45" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A45" s="26" t="s">
         <v>35</v>
       </c>
-      <c r="B44" s="2" t="s">
+      <c r="B45" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="C44" s="2" t="str">
+      <c r="C45" s="2" t="str">
         <f t="shared" si="0"/>
         <v>{do}</v>
       </c>
-      <c r="D44" s="2"/>
-      <c r="E44" s="13"/>
-      <c r="F44" s="30">
-        <v>43</v>
-      </c>
-      <c r="G44" s="25" t="s">
-        <v>112</v>
-      </c>
-      <c r="I44" s="13" t="s">
-        <v>69</v>
-      </c>
-      <c r="J44" s="4" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="45" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="E45" s="13"/>
-      <c r="F45" s="32">
-        <v>44</v>
-      </c>
-      <c r="G45" s="51" t="s">
-        <v>112</v>
-      </c>
-      <c r="H45" s="35"/>
-      <c r="I45" s="38" t="s">
-        <v>2</v>
-      </c>
-      <c r="J45" s="2" t="s">
-        <v>77</v>
-      </c>
+      <c r="D45" s="2"/>
+      <c r="E45" s="6"/>
+      <c r="F45" s="6"/>
+      <c r="G45" s="6"/>
     </row>
     <row r="46" spans="1:28" x14ac:dyDescent="0.25">
       <c r="E46" s="6"/>
+      <c r="F46" s="6"/>
+      <c r="G46" s="6"/>
     </row>
     <row r="47" spans="1:28" x14ac:dyDescent="0.25">
       <c r="E47" s="6"/>
+      <c r="F47" s="6"/>
+      <c r="G47" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>